<commit_message>
Added parts to schematic
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nipun/Documents/Arduino/LEMSv2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nipun/Documents/Arduino/LEMSv2/Hardware Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Shield Parts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t>Number</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Transistor for soil sensors</t>
+  </si>
+  <si>
+    <t>Headers for all sensors</t>
   </si>
 </sst>
 </file>
@@ -1158,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2249,10 +2252,10 @@
     <hyperlink ref="N9" r:id="rId1"/>
     <hyperlink ref="N10" r:id="rId2"/>
     <hyperlink ref="N11" r:id="rId3"/>
-    <hyperlink ref="N12" r:id="rId4"/>
-    <hyperlink ref="N15" r:id="rId5"/>
-    <hyperlink ref="N16" r:id="rId6"/>
-    <hyperlink ref="N18" r:id="rId7"/>
+    <hyperlink ref="N15" r:id="rId4"/>
+    <hyperlink ref="N16" r:id="rId5"/>
+    <hyperlink ref="N18" r:id="rId6"/>
+    <hyperlink ref="N12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2261,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2344,6 +2347,11 @@
         <v>82</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added library, more parts to schematic
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Shield Parts" sheetId="1" r:id="rId1"/>
-    <sheet name="To Add" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
+    <sheet name="To Add, Notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>Schematic Name</t>
-  </si>
-  <si>
     <t>Part Name</t>
   </si>
   <si>
@@ -87,18 +85,9 @@
     <t>Rough List</t>
   </si>
   <si>
-    <t>Charging IC</t>
-  </si>
-  <si>
     <t>Li200 Circuit</t>
   </si>
   <si>
-    <t>Barrel jack connector</t>
-  </si>
-  <si>
-    <t>Wifi Stuff?</t>
-  </si>
-  <si>
     <t>DS3231 Real Time Clock</t>
   </si>
   <si>
@@ -135,18 +124,9 @@
     <t>http://www.mouser.com/Search/ProductDetail.aspx?qs=sGAEpiMZZMtz8P%2feuiupSd2F%2fX%2ffEmeEyLDGD5JMOeY%3d</t>
   </si>
   <si>
-    <t>Spring Terminals</t>
-  </si>
-  <si>
     <t>Sparkfun</t>
   </si>
   <si>
-    <t>PRT-08077</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8077</t>
-  </si>
-  <si>
     <t>Green LED</t>
   </si>
   <si>
@@ -192,48 +172,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>2x18 Stackable Header</t>
-  </si>
-  <si>
-    <t>872-920-0103-01</t>
-  </si>
-  <si>
-    <t>2x18 0.1"</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/SchmartBoard/920-0103-01/?qs=sGAEpiMZZMvnsdhmqAkjhlsi9t0kUWFn</t>
-  </si>
-  <si>
-    <t>1x10 Stackable Header</t>
-  </si>
-  <si>
-    <t>872-920-0087-01</t>
-  </si>
-  <si>
-    <t>1x10 0.1"</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/SchmartBoard/920-0087-01/?qs=sGAEpiMZZMuw1rG4%252bG7fpuZB8%2fkk2RRRAxWI686DfXw%3d</t>
-  </si>
-  <si>
-    <t>Made by SchmartBoard. Comes in packages of 6 for $5.00</t>
-  </si>
-  <si>
-    <t>1x8 Stackable Header</t>
-  </si>
-  <si>
-    <t>872-920-0086-01</t>
-  </si>
-  <si>
-    <t>1x8 0.1"</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/SchmartBoard/920-0086-01/?qs=sGAEpiMZZMuw1rG4%252bG7fpiO%2f7Q9Nlygcqr%2fDExGrMMY%3d</t>
-  </si>
-  <si>
-    <t>Made by SchmartBoard. Comes in packages of 3 for $5.00. Better price at 4uconnector?</t>
-  </si>
-  <si>
     <t>I2C Level Shifting</t>
   </si>
   <si>
@@ -282,7 +220,67 @@
     <t>Transistor for soil sensors</t>
   </si>
   <si>
-    <t>Headers for all sensors</t>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Shipping costs not included!</t>
+  </si>
+  <si>
+    <t>2-Pin 3.5mm Screw Terminal</t>
+  </si>
+  <si>
+    <t>3-Pin 3.5mm Screw Terminal</t>
+  </si>
+  <si>
+    <t>PRT-08084</t>
+  </si>
+  <si>
+    <t>3.5mm Spacing</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8084</t>
+  </si>
+  <si>
+    <t>Possible different source? Check footprint carefully if so</t>
+  </si>
+  <si>
+    <t>PRT-08235</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8235</t>
+  </si>
+  <si>
+    <t>ADS10105</t>
+  </si>
+  <si>
+    <t>12-Pin Female Header</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>S7045-ND</t>
+  </si>
+  <si>
+    <t>0.1" Spacing</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC121LFBN-RC/S7045-ND/810184</t>
+  </si>
+  <si>
+    <t>Used gold instead of tin. May change to surface mount in future</t>
+  </si>
+  <si>
+    <t>16-Pin Female Header</t>
+  </si>
+  <si>
+    <t>S7049-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC161LFBN-RC/S7049-ND/810188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Headers: http://www.digikey.com/product-search/en/connectors-interconnects/rectangular-connectors-headers-receptacles-female-sockets/1442548?k=&amp;pkeyword=&amp;pv88=4&amp;pv88=32&amp;pv89=1&amp;pv90=1&amp;FV=fff40016%2Cfff802f4%2Cfffc0023&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25 </t>
   </si>
 </sst>
 </file>
@@ -335,7 +333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -696,6 +694,21 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -724,7 +737,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -777,6 +790,10 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,6 +821,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1159,10 +1179,874 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="129.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="53"/>
+      <c r="F2" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="53"/>
+      <c r="H2" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="53"/>
+      <c r="J2" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="51"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="49"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="46">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
+        <v>0.82</v>
+      </c>
+      <c r="E4" s="38">
+        <f t="shared" ref="E4:E30" si="0">C4*D4</f>
+        <v>0.82</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0.78</v>
+      </c>
+      <c r="G4" s="43">
+        <f t="shared" ref="G4:G30" si="1">C4*F4*10</f>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0.75</v>
+      </c>
+      <c r="I4" s="43">
+        <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
+        <v>18.75</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="44"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="44"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="44"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="44"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="44"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="44"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="44"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="44"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="44"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="44"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="44"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="44"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="44"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="44"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="44"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="44"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="44"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="44"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="44"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="21"/>
+      <c r="I26" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="44"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="44"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="44"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="44"/>
+    </row>
+    <row r="30" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="45"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D31" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="24">
+        <f>SUM(E4:E30)</f>
+        <v>0.82</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="24">
+        <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="24">
+        <f t="shared" si="3"/>
+        <v>18.75</v>
+      </c>
+      <c r="L31" s="30"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="24">
+        <f>E31</f>
+        <v>0.82</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="35">
+        <f>G31/10</f>
+        <v>0.78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="35">
+        <f>I31/25</f>
+        <v>0.75</v>
+      </c>
+      <c r="L32" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,48 +2063,50 @@
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="72.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="53"/>
+      <c r="A1" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="55"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="54" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="48" t="s">
+      <c r="J2" s="53"/>
+      <c r="K2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="46" t="s">
-        <v>53</v>
+      <c r="L2" s="51"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="48" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1231,178 +2117,276 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="F3" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="47"/>
+      <c r="O3" s="49"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="46">
+        <v>8</v>
+      </c>
+      <c r="E4" s="37">
+        <v>0.95</v>
+      </c>
       <c r="F4" s="38">
-        <f t="shared" ref="F4:F8" si="0">D4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="42"/>
+        <f t="shared" ref="F4:F30" si="0">D4*E4</f>
+        <v>7.6</v>
+      </c>
+      <c r="G4" s="42">
+        <v>0.95</v>
+      </c>
       <c r="H4" s="43">
-        <f t="shared" ref="H4:H8" si="1">D4*G4*10</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="42"/>
+        <f t="shared" ref="H4:H30" si="1">D4*G4*10</f>
+        <v>76</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0.9</v>
+      </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J8" si="2">D4*I4*25</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="44"/>
+        <f t="shared" ref="J4:J30" si="2">D4*I4*25</f>
+        <v>180</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="39"/>
+      <c r="C5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+      <c r="E5" s="39">
+        <v>0.95</v>
+      </c>
       <c r="F5" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="21"/>
+        <v>3.8</v>
+      </c>
+      <c r="G5" s="21">
+        <v>0.95</v>
+      </c>
       <c r="H5" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="21"/>
+        <v>38</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.9</v>
+      </c>
       <c r="J5" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="44"/>
+        <v>90</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="39"/>
+      <c r="C6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="39">
+        <v>1.01</v>
+      </c>
       <c r="F6" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="21"/>
+        <v>1.01</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0.84</v>
+      </c>
       <c r="H6" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="21"/>
+        <v>8.4</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0.77759999999999996</v>
+      </c>
       <c r="J6" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="44"/>
+        <v>19.439999999999998</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="39"/>
+      <c r="C7" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="39">
+        <v>1.27</v>
+      </c>
       <c r="F7" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="21"/>
+        <v>1.27</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1.056</v>
+      </c>
       <c r="H7" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="21"/>
+        <v>10.56</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0.97760000000000002</v>
+      </c>
       <c r="J7" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="44"/>
+        <v>24.44</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="39"/>
+      <c r="C8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="39">
+        <v>1.74</v>
+      </c>
       <c r="F8" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="21"/>
+        <f>D8*E8</f>
+        <v>1.74</v>
+      </c>
+      <c r="G8" s="21">
+        <v>1.74</v>
+      </c>
       <c r="H8" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="21"/>
+        <f>D8*G8*10</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I8" s="21">
+        <v>1.49</v>
+      </c>
       <c r="J8" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="44"/>
+        <f>D8*I8*25</f>
+        <v>37.25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1411,42 +2395,42 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F9" s="26">
-        <f t="shared" ref="F9:F30" si="3">D9*E9</f>
+        <f t="shared" si="0"/>
         <v>8.1199999999999992</v>
       </c>
       <c r="G9" s="21">
         <v>8.1199999999999992</v>
       </c>
       <c r="H9" s="20">
-        <f t="shared" ref="H9:H30" si="4">D9*G9*10</f>
+        <f t="shared" si="1"/>
         <v>81.199999999999989</v>
       </c>
       <c r="I9" s="21">
         <v>7.38</v>
       </c>
       <c r="J9" s="20">
-        <f t="shared" ref="J9:J30" si="5">D9*I9*25</f>
+        <f t="shared" si="2"/>
         <v>184.5</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="44"/>
+        <v>23</v>
+      </c>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1455,130 +2439,94 @@
         <v>0.64</v>
       </c>
       <c r="F10" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
       <c r="G10" s="21">
         <v>0.64</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="I10" s="21">
         <v>0.64</v>
       </c>
       <c r="J10" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="44"/>
+        <v>27</v>
+      </c>
+      <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="39">
-        <v>0.82</v>
-      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="26">
-        <f t="shared" si="3"/>
-        <v>0.82</v>
-      </c>
-      <c r="G11" s="21">
-        <v>0.78</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="21"/>
       <c r="H11" s="20">
-        <f t="shared" si="4"/>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="I11" s="21">
-        <v>0.75</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="21"/>
       <c r="J11" s="20">
-        <f t="shared" si="5"/>
-        <v>18.75</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="44"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="39">
-        <v>1.5</v>
-      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="21">
-        <v>1.43</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="21"/>
       <c r="H12" s="20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="21">
-        <v>1.35</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="21"/>
       <c r="J12" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" s="44"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -1587,42 +2535,42 @@
         <v>0.3</v>
       </c>
       <c r="F13" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="G13" s="21">
         <v>0.23799999999999999</v>
       </c>
       <c r="H13" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2.38</v>
       </c>
       <c r="I13" s="21">
         <v>0.23799999999999999</v>
       </c>
       <c r="J13" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>5.9499999999999993</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="O13" s="44"/>
+        <v>45</v>
+      </c>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -1631,42 +2579,42 @@
         <v>0.39</v>
       </c>
       <c r="F14" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="G14" s="21">
         <v>0.28799999999999998</v>
       </c>
       <c r="H14" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2.88</v>
       </c>
       <c r="I14" s="21">
         <v>0.28799999999999998</v>
       </c>
       <c r="J14" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7.1999999999999993</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="M14" s="29" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="O14" s="44"/>
+        <v>43</v>
+      </c>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -1675,80 +2623,52 @@
         <v>1.5</v>
       </c>
       <c r="F15" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="G15" s="21">
         <v>1.5</v>
       </c>
       <c r="H15" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I15" s="21">
         <v>1.43</v>
       </c>
       <c r="J15" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>35.75</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="M15" s="29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" s="44"/>
+        <v>37</v>
+      </c>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="39">
-        <v>1.74</v>
-      </c>
-      <c r="F16" s="26">
-        <f t="shared" si="3"/>
-        <v>1.74</v>
-      </c>
-      <c r="G16" s="21">
-        <v>1.74</v>
-      </c>
-      <c r="H16" s="20">
-        <f t="shared" si="4"/>
-        <v>17.399999999999999</v>
-      </c>
-      <c r="I16" s="21">
-        <v>1.49</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" si="5"/>
-        <v>37.25</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="O16" s="44"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -1757,168 +2677,108 @@
       <c r="D17" s="4"/>
       <c r="E17" s="39"/>
       <c r="F17" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I17" s="21"/>
       <c r="J17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="3"/>
       <c r="M17" s="29"/>
       <c r="N17" s="19"/>
-      <c r="O17" s="44"/>
+      <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
-      <c r="C18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="39">
-        <v>1.67</v>
-      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="26">
-        <f t="shared" si="3"/>
-        <v>1.67</v>
-      </c>
-      <c r="G18" s="21">
-        <v>1.58</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="21"/>
       <c r="H18" s="20">
-        <f t="shared" si="4"/>
-        <v>15.8</v>
-      </c>
-      <c r="I18" s="21">
-        <v>1.58</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="21"/>
       <c r="J18" s="20">
-        <f t="shared" si="5"/>
-        <v>39.5</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="O18" s="44" t="s">
-        <v>67</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="4"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="39">
-        <v>0.83</v>
-      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="26">
-        <f t="shared" si="3"/>
-        <v>0.83</v>
-      </c>
-      <c r="G19" s="21">
-        <v>0.79</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="21"/>
       <c r="H19" s="20">
-        <f t="shared" si="4"/>
-        <v>7.9</v>
-      </c>
-      <c r="I19" s="21">
-        <v>0.79</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="21"/>
       <c r="J19" s="20">
-        <f t="shared" si="5"/>
-        <v>19.75</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="N19" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="O19" s="44" t="s">
-        <v>62</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
-      <c r="C20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5</v>
-      </c>
-      <c r="E20" s="39">
-        <v>0.83</v>
-      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="26">
-        <f t="shared" si="3"/>
-        <v>4.1499999999999995</v>
-      </c>
-      <c r="G20" s="21">
-        <v>0.79</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="21"/>
       <c r="H20" s="20">
-        <f t="shared" si="4"/>
-        <v>39.5</v>
-      </c>
-      <c r="I20" s="21">
-        <v>0.79</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="21"/>
       <c r="J20" s="20">
-        <f t="shared" si="5"/>
-        <v>98.75</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="O20" s="44" t="s">
-        <v>62</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="4"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -1927,36 +2787,36 @@
         <v>2.74</v>
       </c>
       <c r="F21" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>2.74</v>
       </c>
       <c r="G21" s="21">
         <v>2.46</v>
       </c>
       <c r="H21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>24.6</v>
       </c>
       <c r="I21" s="21">
         <v>2.29</v>
       </c>
       <c r="J21" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>57.25</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="O21" s="44"/>
+        <v>58</v>
+      </c>
+      <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
@@ -1965,24 +2825,24 @@
       <c r="D22" s="4"/>
       <c r="E22" s="39"/>
       <c r="F22" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="3"/>
       <c r="M22" s="29"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="44"/>
+      <c r="O22" s="4"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
@@ -1991,24 +2851,24 @@
       <c r="D23" s="4"/>
       <c r="E23" s="39"/>
       <c r="F23" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="21"/>
       <c r="H23" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
       <c r="M23" s="29"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="44"/>
+      <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
@@ -2017,24 +2877,24 @@
       <c r="D24" s="4"/>
       <c r="E24" s="39"/>
       <c r="F24" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="21"/>
       <c r="H24" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="3"/>
       <c r="M24" s="29"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="44"/>
+      <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
@@ -2043,24 +2903,24 @@
       <c r="D25" s="4"/>
       <c r="E25" s="39"/>
       <c r="F25" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" s="21"/>
       <c r="H25" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
       <c r="M25" s="29"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="44"/>
+      <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
@@ -2069,24 +2929,24 @@
       <c r="D26" s="4"/>
       <c r="E26" s="39"/>
       <c r="F26" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" s="21"/>
       <c r="H26" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
       <c r="M26" s="29"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="44"/>
+      <c r="O26" s="4"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
@@ -2095,24 +2955,24 @@
       <c r="D27" s="4"/>
       <c r="E27" s="39"/>
       <c r="F27" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" s="21"/>
       <c r="H27" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="3"/>
       <c r="M27" s="29"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="44"/>
+      <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
@@ -2121,24 +2981,24 @@
       <c r="D28" s="4"/>
       <c r="E28" s="39"/>
       <c r="F28" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="3"/>
       <c r="M28" s="29"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="44"/>
+      <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -2147,24 +3007,24 @@
       <c r="D29" s="4"/>
       <c r="E29" s="39"/>
       <c r="F29" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="3"/>
       <c r="M29" s="29"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="44"/>
+      <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
@@ -2173,69 +3033,69 @@
       <c r="D30" s="7"/>
       <c r="E30" s="40"/>
       <c r="F30" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G30" s="23"/>
       <c r="H30" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I30" s="23"/>
       <c r="J30" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="6"/>
       <c r="M30" s="33"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="45"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>22.9</v>
+        <v>29.11</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31" s="24">
-        <f t="shared" ref="H31:J31" si="6">SUM(H4:H30)</f>
-        <v>220.85999999999999</v>
+        <f t="shared" ref="H31:J31" si="3">SUM(H4:H30)</f>
+        <v>282.82000000000005</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J31" s="24">
-        <f t="shared" si="6"/>
-        <v>520.65</v>
+        <f t="shared" si="3"/>
+        <v>657.78000000000009</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>22.9</v>
+        <v>29.11</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>22.085999999999999</v>
+        <v>28.282000000000004</v>
       </c>
       <c r="I32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>20.826000000000001</v>
+        <v>26.311200000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2251,105 +3111,94 @@
   <hyperlinks>
     <hyperlink ref="N9" r:id="rId1"/>
     <hyperlink ref="N10" r:id="rId2"/>
-    <hyperlink ref="N11" r:id="rId3"/>
-    <hyperlink ref="N15" r:id="rId4"/>
-    <hyperlink ref="N16" r:id="rId5"/>
-    <hyperlink ref="N18" r:id="rId6"/>
-    <hyperlink ref="N12" r:id="rId7"/>
+    <hyperlink ref="N15" r:id="rId3"/>
+    <hyperlink ref="N8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>84</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working test of LEMSv2, soil test
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>Number</t>
   </si>
@@ -217,9 +217,6 @@
     <t>http://www.linear.com/product/LT3652</t>
   </si>
   <si>
-    <t>Transistor for soil sensors</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -281,6 +278,33 @@
   </si>
   <si>
     <t xml:space="preserve">Good Headers: http://www.digikey.com/product-search/en/connectors-interconnects/rectangular-connectors-headers-receptacles-female-sockets/1442548?k=&amp;pkeyword=&amp;pv88=4&amp;pv88=32&amp;pv89=1&amp;pv90=1&amp;FV=fff40016%2Cfff802f4%2Cfffc0023&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25 </t>
+  </si>
+  <si>
+    <t>Transistor for soil sensors: MMBT3904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosfet for soil sensors?: </t>
+  </si>
+  <si>
+    <t>Possible Solar Panels:</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/search/results?term=solar+panel</t>
+  </si>
+  <si>
+    <t>http://www.voltaicsystems.com/2-watt-panel</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/200</t>
+  </si>
+  <si>
+    <t>Possible Mosfet:</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/2N7000_D26Z/?qs=VVLQfEDCVmOWAB6wZI7AfEGD75mPjRtd8jvfmfXcTKg%3d</t>
+  </si>
+  <si>
+    <t>See for MOSFET that's ESD protected: http://electronics.stackexchange.com/questions/9915/are-discrete-mosfets-esd-sensitive</t>
   </si>
 </sst>
 </file>
@@ -794,6 +818,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,13 +830,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -818,12 +848,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1181,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
@@ -1211,35 +1235,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="52"/>
+      <c r="B2" s="54"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="50" t="s">
+      <c r="G2" s="55"/>
+      <c r="H2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="50" t="s">
+      <c r="I2" s="55"/>
+      <c r="J2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="48" t="s">
+      <c r="K2" s="57"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="51" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1247,8 +1271,8 @@
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>63</v>
+      <c r="B3" s="48" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>12</v>
@@ -1283,7 +1307,7 @@
       <c r="M3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="49"/>
+      <c r="N3" s="52"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -1327,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -2045,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -2069,43 +2093,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="54"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="53"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="50" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="50" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="48" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="51" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2117,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
@@ -2152,13 +2176,13 @@
       <c r="N3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="49"/>
+      <c r="O3" s="52"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="46">
         <v>8</v>
@@ -2188,23 +2212,23 @@
         <v>31</v>
       </c>
       <c r="L4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="58" t="s">
+      <c r="N4" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="59" t="s">
+      <c r="O4" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4">
         <v>4</v>
@@ -2234,23 +2258,23 @@
         <v>31</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="M5" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>72</v>
-      </c>
       <c r="O5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -2277,26 +2301,26 @@
         <v>19.439999999999998</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="N6" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="O6" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -2323,19 +2347,19 @@
         <v>24.44</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="M7" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="O7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -3121,10 +3145,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3173,7 +3197,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3188,7 +3212,12 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -3198,7 +3227,42 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished routing sensor stick
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="94">
   <si>
     <t>Number</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>See for MOSFET that's ESD protected: http://electronics.stackexchange.com/questions/9915/are-discrete-mosfets-esd-sensitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiation Shield: </t>
+  </si>
+  <si>
+    <t>http://www.ambientweather.com/amwesrpatean.html#caption</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
@@ -3145,10 +3151,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3265,6 +3271,16 @@
         <v>91</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit before converting 5TM to library
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="110">
   <si>
     <t>Number</t>
   </si>
@@ -277,9 +277,6 @@
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC161LFBN-RC/S7049-ND/810188</t>
   </si>
   <si>
-    <t xml:space="preserve">Good Headers: http://www.digikey.com/product-search/en/connectors-interconnects/rectangular-connectors-headers-receptacles-female-sockets/1442548?k=&amp;pkeyword=&amp;pv88=4&amp;pv88=32&amp;pv89=1&amp;pv90=1&amp;FV=fff40016%2Cfff802f4%2Cfffc0023&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25 </t>
-  </si>
-  <si>
     <t>Transistor for soil sensors: MMBT3904</t>
   </si>
   <si>
@@ -311,6 +308,57 @@
   </si>
   <si>
     <t>http://www.ambientweather.com/amwesrpatean.html#caption</t>
+  </si>
+  <si>
+    <t>Battery Charger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Headers: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.digikey.com/product-search/en/connectors-interconnects/rectangular-connectors-headers-receptacles-female-sockets/1442548?k=&amp;pkeyword=&amp;pv88=4&amp;pv88=32&amp;pv89=1&amp;pv90=1&amp;FV=fff40016%2Cfff802f4%2Cfffc0023&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25 </t>
+  </si>
+  <si>
+    <t>Solar Panel/Battery Combo:</t>
+  </si>
+  <si>
+    <t>http://www.voltaicsystems.com/3-5-watt-kit</t>
+  </si>
+  <si>
+    <t>http://www.voltaicsystems.com/files/V15-products-one-page.pdf</t>
+  </si>
+  <si>
+    <t>Possible SLA Battery Charger ICs</t>
+  </si>
+  <si>
+    <t>http://www.linear.com/product/LTC4079</t>
+  </si>
+  <si>
+    <t>http://www.linear.com/product/LTC4121</t>
+  </si>
+  <si>
+    <t>http://www.linear.com/product/LTM8062</t>
+  </si>
+  <si>
+    <t>http://www.robotshop.com/en/arduino-mega-stackable-header-kit.html</t>
+  </si>
+  <si>
+    <t>Arduino Mega Headers:</t>
+  </si>
+  <si>
+    <t>https://www.itead.cc/arduino-mega-stackable-header-kit.html</t>
+  </si>
+  <si>
+    <t>http://www.nkcelectronics.com/header-pack-for-megashield-for-arduino-mega-stackable.html</t>
+  </si>
+  <si>
+    <t>5V Voltage Regulators:</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/product/TPS63061</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/product/tps62163</t>
   </si>
 </sst>
 </file>
@@ -767,7 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -827,6 +875,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,30 +1295,30 @@
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="54"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="53" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="53" t="s">
+      <c r="I2" s="56"/>
+      <c r="J2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="51" t="s">
+      <c r="K2" s="58"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="52" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1313,7 +1362,7 @@
       <c r="M3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="52"/>
+      <c r="N3" s="53"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2099,10 +2148,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="60"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -2111,31 +2160,31 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56" t="s">
+      <c r="F2" s="56"/>
+      <c r="G2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="53" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53" t="s">
+      <c r="J2" s="56"/>
+      <c r="K2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="51" t="s">
+      <c r="L2" s="58"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="52" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2182,7 +2231,7 @@
       <c r="N3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="52"/>
+      <c r="O3" s="53"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -3151,13 +3200,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
@@ -3218,67 +3270,147 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>61</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>85</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>89</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed how parts were added to BOM
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="19200" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
-    <sheet name="To Add, Notes" sheetId="2" r:id="rId3"/>
+    <sheet name="To Add" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Number</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Prototype Cost/Unit:</t>
   </si>
   <si>
-    <t>Rough List</t>
-  </si>
-  <si>
     <t>Li200 Circuit</t>
   </si>
   <si>
@@ -178,45 +175,6 @@
     <t>I2C Pullups</t>
   </si>
   <si>
-    <t>Voltage Regulator 5V</t>
-  </si>
-  <si>
-    <t>https://www.maximintegrated.com/en/products/power/switching-regulators/MAX17501.html</t>
-  </si>
-  <si>
-    <t>Voltage Regulator 3.3V</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/RT9193-33GB/1028-1014-1-ND/2470073</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/ADP2302ARDZ-5.0-R7/ADP2302ARDZ-5.0-R7CT-ND/2615949</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/MAX5035BASA%2B/MAX5035BASA%2B-ND/1513599</t>
-  </si>
-  <si>
-    <t>ADS1015 12-Bit ADC</t>
-  </si>
-  <si>
-    <t>595-ADS1015IDGSR</t>
-  </si>
-  <si>
-    <t>SSOP-10</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/ADS1015IDGSR/?qs=sGAEpiMZZMvTvDTV69d2QhvgeGfSYHYrpBxDfXo71%2fQ%3d</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/product/tps5403</t>
-  </si>
-  <si>
-    <t>https://www.maximintegrated.com/en/products/power/switching-regulators/MAX16920.htm</t>
-  </si>
-  <si>
-    <t>http://www.linear.com/product/LT3652</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -247,124 +205,40 @@
     <t>https://www.sparkfun.com/products/8235</t>
   </si>
   <si>
-    <t>ADS10105</t>
-  </si>
-  <si>
-    <t>12-Pin Female Header</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>S7045-ND</t>
-  </si>
-  <si>
-    <t>0.1" Spacing</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC121LFBN-RC/S7045-ND/810184</t>
-  </si>
-  <si>
-    <t>Used gold instead of tin. May change to surface mount in future</t>
-  </si>
-  <si>
-    <t>16-Pin Female Header</t>
-  </si>
-  <si>
-    <t>S7049-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC161LFBN-RC/S7049-ND/810188</t>
-  </si>
-  <si>
-    <t>Transistor for soil sensors: MMBT3904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mosfet for soil sensors?: </t>
-  </si>
-  <si>
-    <t>Possible Solar Panels:</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/search/results?term=solar+panel</t>
-  </si>
-  <si>
-    <t>http://www.voltaicsystems.com/2-watt-panel</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/products/200</t>
-  </si>
-  <si>
-    <t>Possible Mosfet:</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/2N7000_D26Z/?qs=VVLQfEDCVmOWAB6wZI7AfEGD75mPjRtd8jvfmfXcTKg%3d</t>
-  </si>
-  <si>
-    <t>See for MOSFET that's ESD protected: http://electronics.stackexchange.com/questions/9915/are-discrete-mosfets-esd-sensitive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radiation Shield: </t>
-  </si>
-  <si>
-    <t>http://www.ambientweather.com/amwesrpatean.html#caption</t>
-  </si>
-  <si>
-    <t>Battery Charger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good Headers: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.digikey.com/product-search/en/connectors-interconnects/rectangular-connectors-headers-receptacles-female-sockets/1442548?k=&amp;pkeyword=&amp;pv88=4&amp;pv88=32&amp;pv89=1&amp;pv90=1&amp;FV=fff40016%2Cfff802f4%2Cfffc0023&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25 </t>
-  </si>
-  <si>
-    <t>Solar Panel/Battery Combo:</t>
-  </si>
-  <si>
-    <t>http://www.voltaicsystems.com/3-5-watt-kit</t>
-  </si>
-  <si>
-    <t>http://www.voltaicsystems.com/files/V15-products-one-page.pdf</t>
-  </si>
-  <si>
-    <t>Possible SLA Battery Charger ICs</t>
-  </si>
-  <si>
-    <t>http://www.linear.com/product/LTC4079</t>
-  </si>
-  <si>
-    <t>http://www.linear.com/product/LTC4121</t>
-  </si>
-  <si>
-    <t>http://www.linear.com/product/LTM8062</t>
-  </si>
-  <si>
-    <t>http://www.robotshop.com/en/arduino-mega-stackable-header-kit.html</t>
-  </si>
-  <si>
-    <t>Arduino Mega Headers:</t>
-  </si>
-  <si>
-    <t>https://www.itead.cc/arduino-mega-stackable-header-kit.html</t>
-  </si>
-  <si>
-    <t>http://www.nkcelectronics.com/header-pack-for-megashield-for-arduino-mega-stackable.html</t>
-  </si>
-  <si>
-    <t>5V Voltage Regulators:</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/product/TPS63061</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/product/tps62163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://no.co/products/solar </t>
-  </si>
-  <si>
-    <t>Commercial Solar Charger</t>
+    <t>To Add Rough List</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/NOCO-Battery-BLSOLAR2-Charger-Maintainer/dp/B00B7GC50Y/ref=sr_1_1?ie=UTF8&amp;qid=1469347489&amp;sr=8-1&amp;keywords=noco+solar+panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-12069-1 </t>
+  </si>
+  <si>
+    <t>Noco 2.5 Watt Solar Panel</t>
+  </si>
+  <si>
+    <t>Noco 12V 2A Regulator</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/NOCO-GC027-12V-Flex-Regulator/dp/B00H36Y65O/ref=sr_1_fkmr1_1?ie=UTF8&amp;qid=1469347729&amp;sr=8-1-fkmr1&amp;keywords=X-Connect+12+Volt+2+Amp+Regulator</t>
+  </si>
+  <si>
+    <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-13106-2</t>
+  </si>
+  <si>
+    <t>Traco DC/DC Converter</t>
+  </si>
+  <si>
+    <t>495-TSR-1-2450</t>
+  </si>
+  <si>
+    <t>SIP-3</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TRACO-Power/TSR-1-2450/?qs=ckJk83FOD0XFKqda0Mzkgw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1141,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1284,8 +1158,8 @@
     <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="129.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="53" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="156.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="72.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1296,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="L1" s="30"/>
     </row>
@@ -1325,7 +1199,7 @@
       <c r="L2" s="55"/>
       <c r="M2" s="56"/>
       <c r="N2" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1333,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>12</v>
@@ -1373,7 +1247,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1400,70 +1274,110 @@
         <v>18.75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>30</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="39"/>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="39">
+        <v>24.95</v>
+      </c>
       <c r="E5" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="21"/>
+        <v>24.95</v>
+      </c>
+      <c r="F5" s="21">
+        <f>D5</f>
+        <v>24.95</v>
+      </c>
       <c r="G5" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="21"/>
+        <v>249.5</v>
+      </c>
+      <c r="H5" s="21">
+        <f>D5</f>
+        <v>24.95</v>
+      </c>
       <c r="I5" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="2"/>
+        <v>623.75</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="K5" s="3"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="44"/>
+      <c r="L5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="44" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="39"/>
+      <c r="B6" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="39">
+        <v>12.95</v>
+      </c>
       <c r="E6" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="21"/>
+        <v>12.95</v>
+      </c>
+      <c r="F6" s="21">
+        <f>D6</f>
+        <v>12.95</v>
+      </c>
       <c r="G6" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="21"/>
+        <v>129.5</v>
+      </c>
+      <c r="H6" s="21">
+        <f>D6</f>
+        <v>12.95</v>
+      </c>
       <c r="I6" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="2"/>
+        <v>323.75</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="K6" s="3"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="44"/>
+      <c r="L6" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="44" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -2071,21 +1985,21 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>0.82</v>
+        <v>38.72</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
-        <v>7.8000000000000007</v>
+        <v>386.8</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="3"/>
-        <v>18.75</v>
+        <v>966.25</v>
       </c>
       <c r="L31" s="30"/>
     </row>
@@ -2095,21 +2009,21 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>0.82</v>
+        <v>38.72</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>0.78</v>
+        <v>38.68</v>
       </c>
       <c r="H32" t="s">
         <v>16</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>0.75</v>
+        <v>38.65</v>
       </c>
       <c r="L32" s="30"/>
     </row>
@@ -2130,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2162,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2191,7 +2105,7 @@
       <c r="M2" s="55"/>
       <c r="N2" s="56"/>
       <c r="O2" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2202,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>12</v>
@@ -2243,191 +2157,165 @@
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="46">
-        <v>8</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D4" s="46"/>
       <c r="E4" s="37">
         <v>0.95</v>
       </c>
       <c r="F4" s="38">
         <f t="shared" ref="F4:F30" si="0">D4*E4</f>
-        <v>7.6</v>
+        <v>0</v>
       </c>
       <c r="G4" s="42">
         <v>0.95</v>
       </c>
       <c r="H4" s="43">
         <f t="shared" ref="H4:H30" si="1">D4*G4*10</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="I4" s="42">
         <v>0.9</v>
       </c>
       <c r="J4" s="43">
         <f t="shared" ref="J4:J30" si="2">D4*I4*25</f>
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="M4" s="49" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="N4" s="50" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="4">
-        <v>4</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="39">
         <v>0.95</v>
       </c>
       <c r="F5" s="26">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="G5" s="21">
         <v>0.95</v>
       </c>
       <c r="H5" s="20">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="I5" s="21">
         <v>0.9</v>
       </c>
       <c r="J5" s="20">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="N5" s="19" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="39">
-        <v>1.01</v>
+        <v>6.2</v>
       </c>
       <c r="F6" s="26">
         <f t="shared" si="0"/>
-        <v>1.01</v>
+        <v>6.2</v>
       </c>
       <c r="G6" s="21">
-        <v>0.84</v>
+        <v>5.7</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>57</v>
       </c>
       <c r="I6" s="21">
-        <v>0.77759999999999996</v>
+        <v>5.43</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="2"/>
-        <v>19.439999999999998</v>
+        <v>135.75</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M6" s="32" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>78</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="39">
-        <v>1.27</v>
-      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="26">
         <f t="shared" si="0"/>
-        <v>1.27</v>
-      </c>
-      <c r="G7" s="21">
-        <v>1.056</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G7" s="21"/>
       <c r="H7" s="20">
         <f t="shared" si="1"/>
-        <v>10.56</v>
-      </c>
-      <c r="I7" s="21">
-        <v>0.97760000000000002</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I7" s="21"/>
       <c r="J7" s="20">
         <f t="shared" si="2"/>
-        <v>24.44</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>78</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -2454,16 +2342,16 @@
         <v>37.25</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>41</v>
       </c>
       <c r="O8" s="4"/>
     </row>
@@ -2471,7 +2359,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -2498,16 +2386,16 @@
         <v>184.5</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>23</v>
       </c>
       <c r="O9" s="4"/>
     </row>
@@ -2515,7 +2403,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -2542,16 +2430,16 @@
         <v>16</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="N10" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>27</v>
       </c>
       <c r="O10" s="4"/>
     </row>
@@ -2611,7 +2499,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
@@ -2638,16 +2526,16 @@
         <v>5.9499999999999993</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="O13" s="4"/>
     </row>
@@ -2655,7 +2543,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
@@ -2682,16 +2570,16 @@
         <v>7.1999999999999993</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="M14" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>43</v>
       </c>
       <c r="O14" s="4"/>
     </row>
@@ -2699,7 +2587,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -2726,16 +2614,16 @@
         <v>35.75</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="M15" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="O15" s="4"/>
     </row>
@@ -2754,6 +2642,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="29"/>
       <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -2862,45 +2751,27 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
-      <c r="C21" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="39">
-        <v>2.74</v>
-      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="26">
         <f t="shared" si="0"/>
-        <v>2.74</v>
-      </c>
-      <c r="G21" s="21">
-        <v>2.46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G21" s="21"/>
       <c r="H21" s="20">
         <f t="shared" si="1"/>
-        <v>24.6</v>
-      </c>
-      <c r="I21" s="21">
-        <v>2.29</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I21" s="21"/>
       <c r="J21" s="20">
         <f t="shared" si="2"/>
-        <v>57.25</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M21" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="19"/>
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -3143,21 +3014,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>29.11</v>
+        <v>18.89</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="24">
         <f t="shared" ref="H31:J31" si="3">SUM(H4:H30)</f>
-        <v>282.82000000000005</v>
+        <v>182.26</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="24">
         <f t="shared" si="3"/>
-        <v>657.78000000000009</v>
+        <v>422.4</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -3166,21 +3037,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>29.11</v>
+        <v>18.89</v>
       </c>
       <c r="G32" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>28.282000000000004</v>
+        <v>18.225999999999999</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>26.311200000000003</v>
+        <v>16.896000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3206,10 +3077,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3217,217 +3088,28 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>108</v>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>106</v>
-      </c>
+      <c r="A34" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Determined more parts, added to lib/schematic
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="19200" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>Part Name</t>
-  </si>
-  <si>
     <t>Cost/Unit</t>
   </si>
   <si>
@@ -121,27 +118,15 @@
     <t>http://www.mouser.com/Search/ProductDetail.aspx?qs=sGAEpiMZZMtz8P%2feuiupSd2F%2fX%2ffEmeEyLDGD5JMOeY%3d</t>
   </si>
   <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
     <t>Green LED</t>
   </si>
   <si>
-    <t>0805</t>
-  </si>
-  <si>
     <t>Red LED</t>
   </si>
   <si>
     <t>SPDT Switch</t>
   </si>
   <si>
-    <t>COM-00102</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/102</t>
-  </si>
-  <si>
     <t>SD Card Holder</t>
   </si>
   <si>
@@ -154,18 +139,6 @@
     <t>http://www.newark.com/te-connectivity/2041021-3/memory-card-connector-sd-9-position/dp/35R2925?CMP=AFC-QO1721829242?gross_price=</t>
   </si>
   <si>
-    <t>859-LTST-C170CKT</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Lite-On/LTST-C170CKT/?qs=%2fha2pyFadugHsX7bdQzWjBExQ7XjT4CUBfeBcW9RpZq6WjKm4USc7Q%3d%3d</t>
-  </si>
-  <si>
-    <t>859-LTST-S220GKT</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Lite-On/LTST-S220GKT/?qs=%2fha2pyFadug1AbwKhoPm9iYDEuf3iJG%252b7xZNjBWhq%252bziCtB93UlDkw%3d%3d</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -187,24 +160,9 @@
     <t>3-Pin 3.5mm Screw Terminal</t>
   </si>
   <si>
-    <t>PRT-08084</t>
-  </si>
-  <si>
-    <t>3.5mm Spacing</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8084</t>
-  </si>
-  <si>
     <t>Possible different source? Check footprint carefully if so</t>
   </si>
   <si>
-    <t>PRT-08235</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8235</t>
-  </si>
-  <si>
     <t>To Add Rough List</t>
   </si>
   <si>
@@ -239,6 +197,78 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/TRACO-Power/TSR-1-2450/?qs=ckJk83FOD0XFKqda0Mzkgw%3D%3D</t>
+  </si>
+  <si>
+    <t>2x3 Female Header</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>S5712-ND</t>
+  </si>
+  <si>
+    <t>Distributor Part Number</t>
+  </si>
+  <si>
+    <t>Schematic Name</t>
+  </si>
+  <si>
+    <t>0.1"</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC032KFMS-RC/S5712-ND/776171</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>1x5 Female Header</t>
+  </si>
+  <si>
+    <t>1x6 Female Header</t>
+  </si>
+  <si>
+    <t>1x8 Female Header</t>
+  </si>
+  <si>
+    <t>1x10 Female Header</t>
+  </si>
+  <si>
+    <t>S5636-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC051KFXC-RC/S5636-ND/776095</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC061KFXC-RC/S5637-ND/776096</t>
+  </si>
+  <si>
+    <t>S5637-ND</t>
+  </si>
+  <si>
+    <t>S5639-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC081KFXC-RC/S5639-ND/776098 </t>
+  </si>
+  <si>
+    <t>S5641-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC101KFXC-RC/S5641-ND/776100</t>
   </si>
 </sst>
 </file>
@@ -1164,42 +1194,42 @@
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="17"/>
       <c r="D2" s="54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="56"/>
       <c r="F2" s="57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="56"/>
       <c r="H2" s="54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="56"/>
       <c r="J2" s="54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="58"/>
       <c r="L2" s="55"/>
       <c r="M2" s="56"/>
       <c r="N2" s="52" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1207,47 +1237,47 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="N3" s="53"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1274,25 +1304,25 @@
         <v>18.75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1321,23 +1351,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="N5" s="44" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1366,17 +1396,17 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="N6" s="44" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1981,21 +2011,21 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
         <v>38.72</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
         <v>386.8</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="3"/>
@@ -2005,21 +2035,21 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="24">
         <f>E31</f>
         <v>38.72</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
         <v>38.68</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
@@ -2044,14 +2074,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -2061,7 +2091,7 @@
     <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.5" style="30" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="72.33203125" bestFit="1" customWidth="1"/>
@@ -2069,43 +2099,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="58"/>
       <c r="C2" s="55"/>
       <c r="D2" s="17"/>
       <c r="E2" s="54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="56"/>
       <c r="G2" s="57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="56"/>
       <c r="I2" s="54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="56"/>
       <c r="K2" s="54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="58"/>
       <c r="M2" s="55"/>
       <c r="N2" s="56"/>
       <c r="O2" s="52" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2113,43 +2143,43 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="F3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>5</v>
       </c>
       <c r="O3" s="53"/>
     </row>
@@ -2157,95 +2187,69 @@
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D4" s="46"/>
-      <c r="E4" s="37">
-        <v>0.95</v>
-      </c>
+      <c r="E4" s="37"/>
       <c r="F4" s="38">
         <f t="shared" ref="F4:F30" si="0">D4*E4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="42">
-        <v>0.95</v>
-      </c>
+      <c r="G4" s="42"/>
       <c r="H4" s="43">
         <f t="shared" ref="H4:H30" si="1">D4*G4*10</f>
         <v>0</v>
       </c>
-      <c r="I4" s="42">
-        <v>0.9</v>
-      </c>
+      <c r="I4" s="42"/>
       <c r="J4" s="43">
         <f t="shared" ref="J4:J30" si="2">D4*I4*25</f>
         <v>0</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="50" t="s">
-        <v>54</v>
-      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="50"/>
       <c r="O4" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="39">
-        <v>0.95</v>
-      </c>
+      <c r="E5" s="39"/>
       <c r="F5" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="21">
-        <v>0.95</v>
-      </c>
+      <c r="G5" s="21"/>
       <c r="H5" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="21">
-        <v>0.9</v>
-      </c>
+      <c r="I5" s="21"/>
       <c r="J5" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>57</v>
-      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="19"/>
       <c r="O5" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C6" s="25" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -2272,130 +2276,154 @@
         <v>135.75</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="M6" s="32" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="39">
+        <v>1.74</v>
+      </c>
       <c r="F7" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="21"/>
+        <f>D7*E7</f>
+        <v>1.74</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1.74</v>
+      </c>
       <c r="H7" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="21"/>
+        <f>D7*G7*10</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I7" s="21">
+        <v>1.49</v>
+      </c>
       <c r="J7" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="19"/>
+        <f>D7*I7*25</f>
+        <v>37.25</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="27" t="s">
+        <v>35</v>
+      </c>
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="25"/>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="C8" s="25" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="39">
-        <v>1.74</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="F8" s="26">
         <f>D8*E8</f>
-        <v>1.74</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="G8" s="21">
-        <v>1.74</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="H8" s="20">
         <f>D8*G8*10</f>
-        <v>17.399999999999999</v>
+        <v>81.199999999999989</v>
       </c>
       <c r="I8" s="21">
-        <v>1.49</v>
+        <v>7.38</v>
       </c>
       <c r="J8" s="20">
         <f>D8*I8*25</f>
-        <v>37.25</v>
+        <v>184.5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="C9" s="25" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="39">
-        <v>8.1199999999999992</v>
+        <v>0.64</v>
       </c>
       <c r="F9" s="26">
-        <f t="shared" si="0"/>
-        <v>8.1199999999999992</v>
+        <f>D9*E9</f>
+        <v>0.64</v>
       </c>
       <c r="G9" s="21">
-        <v>8.1199999999999992</v>
+        <v>0.64</v>
       </c>
       <c r="H9" s="20">
-        <f t="shared" si="1"/>
-        <v>81.199999999999989</v>
+        <f>D9*G9*10</f>
+        <v>6.4</v>
       </c>
       <c r="I9" s="21">
-        <v>7.38</v>
+        <v>0.64</v>
       </c>
       <c r="J9" s="20">
-        <f t="shared" si="2"/>
-        <v>184.5</v>
+        <f>D9*I9*25</f>
+        <v>16</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="O9" s="4"/>
     </row>
@@ -2403,51 +2431,41 @@
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="39">
-        <v>0.64</v>
-      </c>
+      <c r="E10" s="39"/>
       <c r="F10" s="26">
-        <f t="shared" si="0"/>
-        <v>0.64</v>
-      </c>
-      <c r="G10" s="21">
-        <v>0.64</v>
-      </c>
+        <f>D10*E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="21"/>
       <c r="H10" s="20">
-        <f t="shared" si="1"/>
-        <v>6.4</v>
-      </c>
-      <c r="I10" s="21">
-        <v>0.64</v>
-      </c>
+        <f>D10*G10*10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="21"/>
       <c r="J10" s="20">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>26</v>
-      </c>
+        <f>D10*I10*25</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="19"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
       <c r="E11" s="39"/>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
@@ -2472,8 +2490,12 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
       <c r="E12" s="39"/>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
@@ -2497,45 +2519,47 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="C13" s="25" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13" s="39">
-        <v>0.3</v>
+        <v>1.28</v>
       </c>
       <c r="F13" s="26">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>1.28</v>
       </c>
       <c r="G13" s="21">
-        <v>0.23799999999999999</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="H13" s="20">
         <f t="shared" si="1"/>
-        <v>2.38</v>
+        <v>10.67</v>
       </c>
       <c r="I13" s="21">
-        <v>0.23799999999999999</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="J13" s="20">
         <f t="shared" si="2"/>
-        <v>5.9499999999999993</v>
+        <v>24.675000000000001</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="O13" s="4"/>
     </row>
@@ -2543,43 +2567,43 @@
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="39">
-        <v>0.39</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F14" s="26">
         <f t="shared" si="0"/>
-        <v>0.39</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="G14" s="21">
-        <v>0.28799999999999998</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="H14" s="20">
         <f t="shared" si="1"/>
-        <v>2.88</v>
+        <v>9.2900000000000009</v>
       </c>
       <c r="I14" s="21">
-        <v>0.28799999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="J14" s="20">
         <f t="shared" si="2"/>
-        <v>7.1999999999999993</v>
+        <v>21.5</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="M14" s="29" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="O14" s="4"/>
     </row>
@@ -2587,87 +2611,132 @@
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
       </c>
       <c r="E15" s="39">
-        <v>1.5</v>
+        <v>1.17</v>
       </c>
       <c r="F15" s="26">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.17</v>
       </c>
       <c r="G15" s="21">
-        <v>1.5</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H15" s="20">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>9.75</v>
       </c>
       <c r="I15" s="21">
-        <v>1.43</v>
+        <v>0.90239999999999998</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="2"/>
-        <v>35.75</v>
+        <v>22.56</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="F16" s="26">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="1"/>
+        <v>25.7</v>
+      </c>
+      <c r="I16" s="21">
+        <v>1.19</v>
+      </c>
+      <c r="J16" s="20">
+        <f t="shared" si="2"/>
+        <v>59.5</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="39"/>
+      <c r="C17" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="39">
+        <v>1.57</v>
+      </c>
       <c r="F17" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="21"/>
+        <v>1.57</v>
+      </c>
+      <c r="G17" s="21">
+        <v>1.3009999999999999</v>
+      </c>
       <c r="H17" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="21"/>
+        <v>13.01</v>
+      </c>
+      <c r="I17" s="21">
+        <v>1.2196</v>
+      </c>
       <c r="J17" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="19"/>
+        <v>30.490000000000002</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>79</v>
+      </c>
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -3010,48 +3079,48 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>18.89</v>
+        <v>24.940000000000005</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="24">
         <f t="shared" ref="H31:J31" si="3">SUM(H4:H30)</f>
-        <v>182.26</v>
+        <v>230.41999999999996</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" s="24">
         <f t="shared" si="3"/>
-        <v>422.4</v>
+        <v>532.22500000000002</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>18.89</v>
+        <v>24.940000000000005</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>18.225999999999999</v>
+        <v>23.041999999999994</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>16.896000000000001</v>
+        <v>21.289000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3066,9 +3135,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N9" r:id="rId1"/>
-    <hyperlink ref="N10" r:id="rId2"/>
-    <hyperlink ref="N15" r:id="rId3"/>
-    <hyperlink ref="N8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3090,22 +3156,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Improved BOM and added parts
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
   <si>
     <t>Number</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-13106-2</t>
   </si>
   <si>
-    <t>Traco DC/DC Converter</t>
-  </si>
-  <si>
     <t>495-TSR-1-2450</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>http://www.mouser.com/ProductDetail/TRACO-Power/TSR-1-2450/?qs=ckJk83FOD0XFKqda0Mzkgw%3D%3D</t>
   </si>
   <si>
-    <t>2x3 Female Header</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
@@ -211,12 +205,6 @@
     <t>Distributor Part Number</t>
   </si>
   <si>
-    <t>Schematic Name</t>
-  </si>
-  <si>
-    <t>0.1"</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC032KFMS-RC/S5712-ND/776171</t>
   </si>
   <si>
@@ -235,18 +223,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>1x5 Female Header</t>
-  </si>
-  <si>
-    <t>1x6 Female Header</t>
-  </si>
-  <si>
-    <t>1x8 Female Header</t>
-  </si>
-  <si>
-    <t>1x10 Female Header</t>
-  </si>
-  <si>
     <t>S5636-ND</t>
   </si>
   <si>
@@ -262,13 +238,163 @@
     <t>S5639-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC081KFXC-RC/S5639-ND/776098 </t>
-  </si>
-  <si>
     <t>S5641-ND</t>
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC101KFXC-RC/S5641-ND/776100</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/NPPC081KFXC-RC/S5639-ND/776098</t>
+  </si>
+  <si>
+    <t>2x3 SMT Female Header</t>
+  </si>
+  <si>
+    <t>1x6 SMT Female Header</t>
+  </si>
+  <si>
+    <t>1x5 SMT Female Header</t>
+  </si>
+  <si>
+    <t>1x8 SMT Female Header</t>
+  </si>
+  <si>
+    <t>1x10 SMT Female Header</t>
+  </si>
+  <si>
+    <t>Reference Designator</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>0.1" SMT</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Part Description</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Wurth Electronics</t>
+  </si>
+  <si>
+    <t>691103110002</t>
+  </si>
+  <si>
+    <t>691103110003</t>
+  </si>
+  <si>
+    <t>710-691103110002</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Wurth-Electronics/691103110002/?qs=%2fha2pyFadujUbUS%252bt6nLituZRCwZEM9J%252bNVrPRp0gdDl8b75rjMxqA%3d%3d</t>
+  </si>
+  <si>
+    <t>3.5mm Spacing TH</t>
+  </si>
+  <si>
+    <t>TH = Through Hole</t>
+  </si>
+  <si>
+    <t>SMT = Surface Mount</t>
+  </si>
+  <si>
+    <t>710-691103110003</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Wurth-Electronics/691103110003/?qs=%2fha2pyFadujUbUS%252bt6nLipVHXF0Oc0gS7k5BkdvmKReUZjE00BGlMQ%3d%3d</t>
+  </si>
+  <si>
+    <t>Traco</t>
+  </si>
+  <si>
+    <t>TSR 1-2450</t>
+  </si>
+  <si>
+    <t>DC/DC 5V Regulator</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>2041021-3</t>
+  </si>
+  <si>
+    <t>DS3231SN#T&amp;R</t>
+  </si>
+  <si>
+    <t>Maxim Integrated</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>Sullins Connector</t>
+  </si>
+  <si>
+    <t>NPPC032KFMS-RC</t>
+  </si>
+  <si>
+    <t>NPPC051KFXC-RC</t>
+  </si>
+  <si>
+    <t>NPPC061KFXC-RC</t>
+  </si>
+  <si>
+    <t>NPPC081KFXC-RC</t>
+  </si>
+  <si>
+    <t>NPPC101KFXC-RC</t>
+  </si>
+  <si>
+    <t>No-DNP</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ECA-1HM220</t>
+  </si>
+  <si>
+    <t>22uF 50V Capacitor</t>
+  </si>
+  <si>
+    <t>P5179-ND</t>
+  </si>
+  <si>
+    <t>5mm Diam. Radial TH</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ECA-1HM220/P5179-ND/245038?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
 </sst>
 </file>
@@ -313,12 +439,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="32">
@@ -725,7 +857,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -786,6 +918,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,12 +942,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1205,30 +1354,30 @@
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="E2" s="57"/>
+      <c r="F2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="54" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="56"/>
-      <c r="J2" s="54" t="s">
+      <c r="I2" s="57"/>
+      <c r="J2" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="52" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="53" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1272,7 +1421,7 @@
       <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="53"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2072,1069 +2221,1298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="130.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="138.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="72.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
-        <v>10</v>
+    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>95</v>
       </c>
       <c r="B1" s="60"/>
-      <c r="C1" s="1">
+      <c r="C1" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="61"/>
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="57"/>
+      <c r="M2" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="59"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="58"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="28" t="s">
+      <c r="H3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="31" t="s">
+      <c r="N3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="53"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="Q3" s="54"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38">
-        <f t="shared" ref="F4:F30" si="0">D4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43">
-        <f t="shared" ref="H4:H30" si="1">D4*G4*10</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="42"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="37">
+        <v>0.83</v>
+      </c>
+      <c r="H4" s="38">
+        <f t="shared" ref="H4:H31" si="0">F4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0.73899999999999999</v>
+      </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J30" si="2">D4*I4*25</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="4" t="s">
+        <f t="shared" ref="J4:J31" si="1">F4*I4*10</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="42">
+        <f>I4</f>
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="L4" s="43">
+        <f t="shared" ref="L4:L31" si="2">F4*K4*25</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="21"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.98599999999999999</v>
+      </c>
       <c r="J5" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="4" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <f>I5</f>
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="L5" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C6" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="39">
+        <v>6.2</v>
+      </c>
+      <c r="H6" s="26">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+      <c r="I6" s="21">
+        <v>5.7</v>
+      </c>
+      <c r="J6" s="20">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="K6" s="21">
+        <v>5.43</v>
+      </c>
+      <c r="L6" s="20">
+        <f t="shared" si="2"/>
+        <v>135.75</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="4">
+      <c r="O6" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="68">
         <v>1</v>
       </c>
-      <c r="E6" s="39">
-        <v>6.2</v>
-      </c>
-      <c r="F6" s="26">
-        <f t="shared" si="0"/>
-        <v>6.2</v>
-      </c>
-      <c r="G6" s="21">
-        <v>5.7</v>
-      </c>
-      <c r="H6" s="20">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="I6" s="21">
-        <v>5.43</v>
-      </c>
-      <c r="J6" s="20">
-        <f t="shared" si="2"/>
-        <v>135.75</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="G7" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="H7" s="70">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="I7" s="71">
+        <v>0.153</v>
+      </c>
+      <c r="J7" s="72">
+        <f t="shared" si="1"/>
+        <v>1.53</v>
+      </c>
+      <c r="K7" s="71">
+        <v>0.1124</v>
+      </c>
+      <c r="L7" s="72">
+        <f t="shared" si="2"/>
+        <v>2.81</v>
+      </c>
+      <c r="M7" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="P7" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q7" s="68"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="39">
+        <v>1.74</v>
+      </c>
+      <c r="H8" s="26">
+        <f>F8*G8</f>
+        <v>1.74</v>
+      </c>
+      <c r="I8" s="21">
+        <v>1.74</v>
+      </c>
+      <c r="J8" s="20">
+        <f>F8*I8*10</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="K8" s="21">
+        <v>1.49</v>
+      </c>
+      <c r="L8" s="20">
+        <f>F8*K8*25</f>
+        <v>37.25</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="39">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="H9" s="26">
+        <f>F9*G9</f>
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="I9" s="21">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J9" s="20">
+        <f>F9*I9*10</f>
+        <v>81.199999999999989</v>
+      </c>
+      <c r="K9" s="21">
+        <v>7.38</v>
+      </c>
+      <c r="L9" s="20">
+        <f>F9*K9*25</f>
+        <v>184.5</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="N9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="39">
-        <v>1.74</v>
-      </c>
-      <c r="F7" s="26">
-        <f>D7*E7</f>
-        <v>1.74</v>
-      </c>
-      <c r="G7" s="21">
-        <v>1.74</v>
-      </c>
-      <c r="H7" s="20">
-        <f>D7*G7*10</f>
-        <v>17.399999999999999</v>
-      </c>
-      <c r="I7" s="21">
-        <v>1.49</v>
-      </c>
-      <c r="J7" s="20">
-        <f>D7*I7*25</f>
-        <v>37.25</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="G10" s="39">
+        <v>0.64</v>
+      </c>
+      <c r="H10" s="26">
+        <f>F10*G10</f>
+        <v>0.64</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.64</v>
+      </c>
+      <c r="J10" s="20">
+        <f>F10*I10*10</f>
+        <v>6.4</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0.64</v>
+      </c>
+      <c r="L10" s="20">
+        <f>F10*K10*25</f>
+        <v>16</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="39">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="F8" s="26">
-        <f>D8*E8</f>
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="G8" s="21">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="H8" s="20">
-        <f>D8*G8*10</f>
-        <v>81.199999999999989</v>
-      </c>
-      <c r="I8" s="21">
-        <v>7.38</v>
-      </c>
-      <c r="J8" s="20">
-        <f>D8*I8*25</f>
-        <v>184.5</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="39">
-        <v>0.64</v>
-      </c>
-      <c r="F9" s="26">
-        <f>D9*E9</f>
-        <v>0.64</v>
-      </c>
-      <c r="G9" s="21">
-        <v>0.64</v>
-      </c>
-      <c r="H9" s="20">
-        <f>D9*G9*10</f>
-        <v>6.4</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0.64</v>
-      </c>
-      <c r="J9" s="20">
-        <f>D9*I9*25</f>
-        <v>16</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="26">
-        <f>D10*E10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="20">
-        <f>D10*G10*10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="20">
-        <f>D10*I10*25</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="20">
-        <f t="shared" si="1"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="26">
+        <f>F11*G11</f>
         <v>0</v>
       </c>
       <c r="I11" s="21"/>
       <c r="J11" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="4">
+        <f>F11*I11*10</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="20">
+        <f>F11*K11*25</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="20">
-        <f t="shared" si="1"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="25" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="21"/>
+      <c r="L13" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="39">
+        <v>1.28</v>
+      </c>
+      <c r="H14" s="26">
+        <f t="shared" si="0"/>
+        <v>1.28</v>
+      </c>
+      <c r="I14" s="21">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="J14" s="20">
+        <f t="shared" si="1"/>
+        <v>10.67</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="2"/>
+        <v>24.675000000000001</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="39">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H15" s="26">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I15" s="21">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J15" s="20">
+        <f t="shared" si="1"/>
+        <v>9.2900000000000009</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0.86</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="39">
+        <v>1.17</v>
+      </c>
+      <c r="H16" s="26">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
+      <c r="I16" s="21">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J16" s="20">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="L16" s="20">
+        <f t="shared" si="2"/>
+        <v>22.56</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="O16" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" s="4"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="H17" s="26">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="I17" s="21">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="J17" s="20">
+        <f t="shared" si="1"/>
+        <v>25.7</v>
+      </c>
+      <c r="K17" s="21">
+        <v>1.19</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="2"/>
+        <v>59.5</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="39">
-        <v>1.28</v>
-      </c>
-      <c r="F13" s="26">
-        <f t="shared" si="0"/>
-        <v>1.28</v>
-      </c>
-      <c r="G13" s="21">
-        <v>1.0669999999999999</v>
-      </c>
-      <c r="H13" s="20">
-        <f t="shared" si="1"/>
-        <v>10.67</v>
-      </c>
-      <c r="I13" s="21">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="J13" s="20">
-        <f t="shared" si="2"/>
-        <v>24.675000000000001</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="39">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F14" s="26">
-        <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G14" s="21">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="H14" s="20">
-        <f t="shared" si="1"/>
-        <v>9.2900000000000009</v>
-      </c>
-      <c r="I14" s="21">
-        <v>0.86</v>
-      </c>
-      <c r="J14" s="20">
-        <f t="shared" si="2"/>
-        <v>21.5</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25" t="s">
+      <c r="G18" s="39">
+        <v>1.57</v>
+      </c>
+      <c r="H18" s="26">
+        <f t="shared" si="0"/>
+        <v>1.57</v>
+      </c>
+      <c r="I18" s="21">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="J18" s="20">
+        <f t="shared" si="1"/>
+        <v>13.01</v>
+      </c>
+      <c r="K18" s="21">
+        <v>1.2196</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="2"/>
+        <v>30.490000000000002</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="39">
-        <v>1.17</v>
-      </c>
-      <c r="F15" s="26">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
-      <c r="G15" s="21">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H15" s="20">
-        <f t="shared" si="1"/>
-        <v>9.75</v>
-      </c>
-      <c r="I15" s="21">
-        <v>0.90239999999999998</v>
-      </c>
-      <c r="J15" s="20">
-        <f t="shared" si="2"/>
-        <v>22.56</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="M15" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="25" t="s">
+      <c r="O18" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="P18" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1.55</v>
-      </c>
-      <c r="F16" s="26">
-        <f t="shared" si="0"/>
-        <v>3.1</v>
-      </c>
-      <c r="G16" s="21">
-        <v>1.2849999999999999</v>
-      </c>
-      <c r="H16" s="20">
-        <f t="shared" si="1"/>
-        <v>25.7</v>
-      </c>
-      <c r="I16" s="21">
-        <v>1.19</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" si="2"/>
-        <v>59.5</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="39">
-        <v>1.57</v>
-      </c>
-      <c r="F17" s="26">
-        <f t="shared" si="0"/>
-        <v>1.57</v>
-      </c>
-      <c r="G17" s="21">
-        <v>1.3009999999999999</v>
-      </c>
-      <c r="H17" s="20">
-        <f t="shared" si="1"/>
-        <v>13.01</v>
-      </c>
-      <c r="I17" s="21">
-        <v>1.2196</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="2"/>
-        <v>30.490000000000002</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="M17" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="N17" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="34"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="25"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="20">
-        <f t="shared" si="1"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="21"/>
+      <c r="L19" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="20">
-        <f t="shared" si="1"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I20" s="21"/>
       <c r="J20" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="20">
-        <f t="shared" si="1"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I21" s="21"/>
       <c r="J21" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="21"/>
+      <c r="L21" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="20">
-        <f t="shared" si="1"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="21"/>
+      <c r="L22" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="20">
-        <f t="shared" si="1"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="21"/>
       <c r="J23" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="21"/>
+      <c r="L23" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="4"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="20">
-        <f t="shared" si="1"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="L24" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="20">
-        <f t="shared" si="1"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="21"/>
+      <c r="L25" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="4"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="20">
-        <f t="shared" si="1"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I26" s="21"/>
       <c r="J26" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="21"/>
+      <c r="L26" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="4"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="20">
-        <f t="shared" si="1"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="21"/>
+      <c r="L27" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="21"/>
-      <c r="H28" s="20">
-        <f t="shared" si="1"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="21"/>
+      <c r="L28" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="20">
-        <f t="shared" si="1"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E31" s="24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="21"/>
+      <c r="L29" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="21"/>
+      <c r="J30" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="21"/>
+      <c r="L30" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="23"/>
+      <c r="J31" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="23"/>
+      <c r="L31" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G32" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="24">
-        <f>SUM(F4:F30)</f>
-        <v>24.940000000000005</v>
-      </c>
-      <c r="G31" s="24" t="s">
+      <c r="H32" s="24">
+        <f>SUM(H4:H31)</f>
+        <v>25.160000000000004</v>
+      </c>
+      <c r="I32" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="24">
-        <f t="shared" ref="H31:J31" si="3">SUM(H4:H30)</f>
-        <v>230.41999999999996</v>
-      </c>
-      <c r="I31" s="24" t="s">
+      <c r="J32" s="24">
+        <f t="shared" ref="J32:L32" si="3">SUM(J4:J31)</f>
+        <v>231.94999999999996</v>
+      </c>
+      <c r="K32" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="24">
+      <c r="L32" s="24">
         <f t="shared" si="3"/>
-        <v>532.22500000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E32" t="s">
+        <v>535.03499999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="24">
-        <f>F31</f>
-        <v>24.940000000000005</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H33" s="24">
+        <f>H32</f>
+        <v>25.160000000000004</v>
+      </c>
+      <c r="I33" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="35">
-        <f>H31/10</f>
-        <v>23.041999999999994</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="J33" s="35">
+        <f>J32/10</f>
+        <v>23.194999999999997</v>
+      </c>
+      <c r="K33" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="35">
-        <f>J31/25</f>
-        <v>21.289000000000001</v>
+      <c r="L33" s="35">
+        <f>L32/25</f>
+        <v>21.401399999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A2:C2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N9" r:id="rId1"/>
+    <hyperlink ref="P10" r:id="rId1"/>
+    <hyperlink ref="P17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added more parts to schematic
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="169">
   <si>
     <t>Number</t>
   </si>
@@ -88,27 +88,15 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>700-DS3231SN#T&amp;R-</t>
-  </si>
-  <si>
     <t>SOIC-16</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Maxim-Integrated/DS3231SNTR/?qs=sGAEpiMZZMuuBt6TL7D%2f6PgM9QV8pLmA</t>
-  </si>
-  <si>
     <t>12mm Battery Holder</t>
   </si>
   <si>
-    <t>534-3000</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Keystone-Electronics/3000/?qs=sGAEpiMZZMtT9MhkajLHrnU1d13jcSgSROM9zhZkF8A%3d</t>
-  </si>
-  <si>
     <t>CR1220 Battery</t>
   </si>
   <si>
@@ -145,9 +133,6 @@
     <t>I2C Level Shifting</t>
   </si>
   <si>
-    <t>I2C Pullups</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -328,9 +313,6 @@
     <t>http://www.mouser.com/ProductDetail/Wurth-Electronics/691103110003/?qs=%2fha2pyFadujUbUS%252bt6nLipVHXF0Oc0gS7k5BkdvmKReUZjE00BGlMQ%3d%3d</t>
   </si>
   <si>
-    <t>Traco</t>
-  </si>
-  <si>
     <t>TSR 1-2450</t>
   </si>
   <si>
@@ -373,15 +355,9 @@
     <t>NPPC101KFXC-RC</t>
   </si>
   <si>
-    <t>No-DNP</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
     <t>ECA-1HM220</t>
   </si>
   <si>
@@ -395,6 +371,171 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/ECA-1HM220/P5179-ND/245038?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>Octopart has alt. distributors</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>Traco Power</t>
+  </si>
+  <si>
+    <t>Panasonic Electronics</t>
+  </si>
+  <si>
+    <t>GRM21BR71H105KA12L</t>
+  </si>
+  <si>
+    <t>1uF 50V Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>490-4736-1-ND</t>
+  </si>
+  <si>
+    <t>0805 (Imperial)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM21BR71H105KA12L/490-4736-1-ND/1244332?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0805FR-0710KL</t>
+  </si>
+  <si>
+    <t>10k 1% 1/8W Resistor</t>
+  </si>
+  <si>
+    <t>311-10.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0805FR-0710KL/311-10.0KCRCT-ND/730482?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>Distributor Link</t>
+  </si>
+  <si>
+    <t>36-3000-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/3000/36-3000-ND/227440?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>DS3231SN#T&amp;RCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/DS3231SN%2523T%26R/DS3231SN%2523T%26RCT-ND/3894827?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>BMP280</t>
+  </si>
+  <si>
+    <t>Screw Terminals</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9, J10</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>2x3 TH Female Header</t>
+  </si>
+  <si>
+    <t>1x5 TH Female Header</t>
+  </si>
+  <si>
+    <t>1x6 TH Female Header</t>
+  </si>
+  <si>
+    <t>1x8 Th Female Header</t>
+  </si>
+  <si>
+    <t>1x10 TH Female Header</t>
+  </si>
+  <si>
+    <t>0.1" TH</t>
+  </si>
+  <si>
+    <t>Future Expansion Connector</t>
+  </si>
+  <si>
+    <t>Sonic Anemometer 5V Hardware</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>LEDs with transistors</t>
+  </si>
+  <si>
+    <t>Reverse voltage protection</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>BSS138CT-ND</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/BSS138/BSS138CT-ND/244294?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>To Test</t>
+  </si>
+  <si>
+    <t>5TM Level shifting w/ 2 sensors</t>
+  </si>
+  <si>
+    <t>Solar panel Open Voltage - change reverse mosfet if necessary</t>
+  </si>
+  <si>
+    <t>Q1-Q7</t>
+  </si>
+  <si>
+    <t>R1-R13</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>EG1218</t>
+  </si>
+  <si>
+    <t>612-EG1218</t>
+  </si>
+  <si>
+    <t>2.5mm TH</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/E-Switch/EG1218/?qs=sGAEpiMZZMtHXLepoqNyVZDOWY7elTCOE4MJ3sXRkSs%3d</t>
   </si>
 </sst>
 </file>
@@ -857,7 +998,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -921,6 +1062,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -945,23 +1106,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1349,36 +1493,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58" t="s">
+      <c r="E2" s="71"/>
+      <c r="F2" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="55" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="55" t="s">
+      <c r="I2" s="71"/>
+      <c r="J2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="53" t="s">
-        <v>36</v>
+      <c r="K2" s="73"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="67" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1386,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>11</v>
@@ -1421,12 +1565,12 @@
       <c r="M3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="54"/>
+      <c r="N3" s="68"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1456,22 +1600,22 @@
         <v>18</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="L4" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1500,23 +1644,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N5" s="44" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1545,17 +1689,17 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N6" s="44" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2221,17 +2365,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -2248,64 +2393,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="60"/>
+      <c r="A1" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="74"/>
       <c r="C1" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>91</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58" t="s">
+      <c r="H2" s="71"/>
+      <c r="I2" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="55" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="55" t="s">
+      <c r="L2" s="71"/>
+      <c r="M2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="53" t="s">
-        <v>36</v>
+      <c r="N2" s="73"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="67" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>84</v>
+        <v>77</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>11</v>
@@ -2332,43 +2479,43 @@
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>12</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="54"/>
+        <v>129</v>
+      </c>
+      <c r="Q3" s="68"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="37">
         <v>0.83</v>
       </c>
       <c r="H4" s="38">
-        <f t="shared" ref="H4:H31" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H33" si="0">F4*G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="42">
         <v>0.73899999999999999</v>
       </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J31" si="1">F4*I4*10</f>
+        <f t="shared" ref="J4:J33" si="1">F4*I4*10</f>
         <v>0</v>
       </c>
       <c r="K4" s="42">
@@ -2376,38 +2523,38 @@
         <v>0.73899999999999999</v>
       </c>
       <c r="L4" s="43">
-        <f t="shared" ref="L4:L31" si="2">F4*K4*25</f>
+        <f t="shared" ref="L4:L33" si="2">F4*K4*25</f>
         <v>0</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O4" s="49" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="39">
@@ -2436,33 +2583,33 @@
         <v>18</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -2492,85 +2639,85 @@
         <v>18</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" s="66" t="s">
+      <c r="A7" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="68">
+      <c r="D7" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="59">
         <v>1</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="60">
         <v>0.22</v>
       </c>
-      <c r="H7" s="70">
+      <c r="H7" s="61">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="62">
         <v>0.153</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="63">
         <f t="shared" si="1"/>
         <v>1.53</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7" s="62">
         <v>0.1124</v>
       </c>
-      <c r="L7" s="72">
+      <c r="L7" s="63">
         <f t="shared" si="2"/>
         <v>2.81</v>
       </c>
-      <c r="M7" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="O7" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="P7" s="73" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q7" s="68"/>
+      <c r="M7" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q7" s="59"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2579,49 +2726,49 @@
         <v>1.74</v>
       </c>
       <c r="H8" s="26">
-        <f>F8*G8</f>
+        <f t="shared" ref="H8:H13" si="3">F8*G8</f>
         <v>1.74</v>
       </c>
       <c r="I8" s="21">
         <v>1.74</v>
       </c>
       <c r="J8" s="20">
-        <f>F8*I8*10</f>
+        <f t="shared" ref="J8:J13" si="4">F8*I8*10</f>
         <v>17.399999999999999</v>
       </c>
       <c r="K8" s="21">
         <v>1.49</v>
       </c>
       <c r="L8" s="20">
-        <f>F8*K8*25</f>
+        <f t="shared" ref="L8:L13" si="5">F8*K8*25</f>
         <v>37.25</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>17</v>
@@ -2630,696 +2777,857 @@
         <v>1</v>
       </c>
       <c r="G9" s="39">
-        <v>8.1199999999999992</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="H9" s="26">
-        <f>F9*G9</f>
-        <v>8.1199999999999992</v>
+        <f t="shared" si="3"/>
+        <v>9.9700000000000006</v>
       </c>
       <c r="I9" s="21">
-        <v>8.1199999999999992</v>
+        <v>9.41</v>
       </c>
       <c r="J9" s="20">
-        <f>F9*I9*10</f>
-        <v>81.199999999999989</v>
+        <f t="shared" si="4"/>
+        <v>94.1</v>
       </c>
       <c r="K9" s="21">
-        <v>7.38</v>
+        <v>7.5275999999999996</v>
       </c>
       <c r="L9" s="20">
-        <f>F9*K9*25</f>
-        <v>184.5</v>
+        <f t="shared" si="5"/>
+        <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="N9" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="O9" s="32" t="s">
-        <v>20</v>
-      </c>
       <c r="P9" s="19" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>162</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="F10" s="4">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G10" s="39">
-        <v>0.64</v>
+        <v>0.1</v>
       </c>
       <c r="H10" s="26">
-        <f>F10*G10</f>
-        <v>0.64</v>
+        <f t="shared" si="3"/>
+        <v>1.3</v>
       </c>
       <c r="I10" s="21">
-        <v>0.64</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
-        <f>F10*I10*10</f>
-        <v>6.4</v>
+        <f t="shared" si="4"/>
+        <v>2.7300000000000004</v>
       </c>
       <c r="K10" s="21">
-        <v>0.64</v>
+        <v>1.52E-2</v>
       </c>
       <c r="L10" s="20">
-        <f>F10*K10*25</f>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>4.9399999999999995</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="29"/>
+        <v>82</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>119</v>
+      </c>
       <c r="E11" s="25" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="39">
+        <v>0.25</v>
+      </c>
       <c r="H11" s="26">
-        <f>F11*G11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="21"/>
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.20799999999999999</v>
+      </c>
       <c r="J11" s="20">
-        <f>F11*I11*10</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="21"/>
+        <f t="shared" si="4"/>
+        <v>2.08</v>
+      </c>
+      <c r="K11" s="21">
+        <f>I11</f>
+        <v>0.20799999999999999</v>
+      </c>
       <c r="L11" s="20">
-        <f>F11*K11*25</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="19"/>
+        <f t="shared" si="5"/>
+        <v>5.2</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>123</v>
+      </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="32"/>
+        <v>82</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="E12" s="25" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="39">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="H12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="21"/>
+        <f t="shared" si="3"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I12" s="21">
+        <v>0.54500000000000004</v>
+      </c>
       <c r="J12" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="21"/>
+        <f t="shared" si="4"/>
+        <v>5.45</v>
+      </c>
+      <c r="K12" s="21">
+        <f>I12</f>
+        <v>0.54500000000000004</v>
+      </c>
       <c r="L12" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="19"/>
+        <f t="shared" si="5"/>
+        <v>13.625000000000002</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="64"/>
+        <v>82</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="25" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="G13" s="39"/>
       <c r="H13" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="29"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>109</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="25" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="39">
-        <v>1.28</v>
-      </c>
+      <c r="G14" s="39"/>
       <c r="H14" s="26">
         <f t="shared" si="0"/>
-        <v>1.28</v>
-      </c>
-      <c r="I14" s="21">
-        <v>1.0669999999999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I14" s="21"/>
       <c r="J14" s="20">
         <f t="shared" si="1"/>
-        <v>10.67</v>
-      </c>
-      <c r="K14" s="21">
-        <v>0.98699999999999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K14" s="21"/>
       <c r="L14" s="20">
         <f t="shared" si="2"/>
-        <v>24.675000000000001</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="19"/>
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>110</v>
+        <v>82</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>165</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
       <c r="G15" s="39">
-        <v>1.1200000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I15" s="21">
-        <v>0.92900000000000005</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>9.2900000000000009</v>
+        <v>5.42</v>
       </c>
       <c r="K15" s="21">
-        <v>0.86</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="L15" s="20">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>13.275</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
       </c>
       <c r="G16" s="39">
-        <v>1.17</v>
+        <v>1.28</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
-        <v>1.17</v>
+        <v>1.28</v>
       </c>
       <c r="I16" s="21">
-        <v>0.97499999999999998</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="J16" s="20">
         <f t="shared" si="1"/>
-        <v>9.75</v>
+        <v>10.67</v>
       </c>
       <c r="K16" s="21">
-        <v>0.90239999999999998</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="L16" s="20">
         <f t="shared" si="2"/>
-        <v>22.56</v>
+        <v>24.675000000000001</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B17" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="F17" s="4">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1.55</v>
+        <v>1</v>
+      </c>
+      <c r="G17" s="39">
+        <v>1.1200000000000001</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>3.1</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I17" s="21">
-        <v>1.2849999999999999</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
-        <v>25.7</v>
+        <v>9.2900000000000009</v>
       </c>
       <c r="K17" s="21">
-        <v>1.19</v>
+        <v>0.86</v>
       </c>
       <c r="L17" s="20">
         <f t="shared" si="2"/>
-        <v>59.5</v>
+        <v>21.5</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="O17" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
       <c r="G18" s="39">
+        <v>1.17</v>
+      </c>
+      <c r="H18" s="26">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J18" s="20">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="2"/>
+        <v>22.56</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.55</v>
+      </c>
+      <c r="H19" s="26">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="I19" s="21">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" si="1"/>
+        <v>25.7</v>
+      </c>
+      <c r="K19" s="21">
+        <v>1.19</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" si="2"/>
+        <v>59.5</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="39">
         <v>1.57</v>
       </c>
-      <c r="H18" s="26">
+      <c r="H20" s="26">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I20" s="21">
         <v>1.3009999999999999</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J20" s="20">
         <f t="shared" si="1"/>
         <v>13.01</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K20" s="21">
         <v>1.2196</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L20" s="20">
         <f t="shared" si="2"/>
         <v>30.490000000000002</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="O18" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="19"/>
+      <c r="M20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="21"/>
-      <c r="J21" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="4"/>
+      <c r="A21" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="59">
+        <v>1</v>
+      </c>
+      <c r="G21" s="60"/>
+      <c r="H21" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="62"/>
+      <c r="L21" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="56"/>
+      <c r="N21" s="57"/>
+      <c r="O21" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="59" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="21"/>
-      <c r="L22" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="4"/>
+      <c r="A22" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="59">
+        <v>1</v>
+      </c>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="62"/>
+      <c r="L22" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="56"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="59" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="21"/>
-      <c r="L23" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="4"/>
+      <c r="A23" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="59">
+        <v>1</v>
+      </c>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="62"/>
+      <c r="L23" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57"/>
+      <c r="O23" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="59" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="21"/>
-      <c r="L24" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="4"/>
+      <c r="A24" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="F24" s="59">
+        <v>2</v>
+      </c>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="62"/>
+      <c r="J24" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="62"/>
+      <c r="L24" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="56"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="59" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="21"/>
-      <c r="L25" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="4"/>
+      <c r="A25" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="59">
+        <v>1</v>
+      </c>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="62"/>
+      <c r="L25" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="56"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="59" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="39"/>
+      <c r="A26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" s="4">
+        <v>7</v>
+      </c>
+      <c r="G26" s="39">
+        <v>0.22</v>
+      </c>
       <c r="H26" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="21"/>
+        <v>1.54</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0.17799999999999999</v>
+      </c>
       <c r="J26" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="21"/>
+        <v>12.46</v>
+      </c>
+      <c r="K26" s="21">
+        <f>I26</f>
+        <v>0.17799999999999999</v>
+      </c>
       <c r="L26" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="19"/>
+        <v>31.15</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O26" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="P26" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="3"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="25"/>
       <c r="F27" s="4"/>
       <c r="G27" s="39"/>
       <c r="H27" s="26">
@@ -3339,15 +3647,15 @@
       <c r="M27" s="2"/>
       <c r="N27" s="3"/>
       <c r="O27" s="29"/>
-      <c r="P27" s="4"/>
+      <c r="P27" s="19"/>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="3"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="4"/>
       <c r="G28" s="39"/>
       <c r="H28" s="26">
@@ -3367,7 +3675,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="3"/>
       <c r="O28" s="29"/>
-      <c r="P28" s="4"/>
+      <c r="P28" s="19"/>
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -3426,78 +3734,134 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
     </row>
-    <row r="31" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="23"/>
-      <c r="L31" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G32" s="24" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="L32" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+    </row>
+    <row r="33" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="23"/>
+      <c r="J33" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="5"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G34" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="24">
-        <f>SUM(H4:H31)</f>
-        <v>25.160000000000004</v>
-      </c>
-      <c r="I32" s="24" t="s">
+      <c r="H34" s="24">
+        <f>SUM(H4:H33)</f>
+        <v>30.6</v>
+      </c>
+      <c r="I34" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="24">
-        <f t="shared" ref="J32:L32" si="3">SUM(J4:J31)</f>
-        <v>231.94999999999996</v>
-      </c>
-      <c r="K32" s="24" t="s">
+      <c r="J34" s="24">
+        <f t="shared" ref="J34:L34" si="6">SUM(J4:J33)</f>
+        <v>266.58999999999992</v>
+      </c>
+      <c r="K34" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L32" s="24">
-        <f t="shared" si="3"/>
-        <v>535.03499999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G33" t="s">
+      <c r="L34" s="24">
+        <f t="shared" si="6"/>
+        <v>590.91499999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="24">
-        <f>H32</f>
-        <v>25.160000000000004</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="H35" s="24">
+        <f>H34</f>
+        <v>30.6</v>
+      </c>
+      <c r="I35" t="s">
         <v>15</v>
       </c>
-      <c r="J33" s="35">
-        <f>J32/10</f>
-        <v>23.194999999999997</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="J35" s="35">
+        <f>J34/10</f>
+        <v>26.658999999999992</v>
+      </c>
+      <c r="K35" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="35">
-        <f>L32/25</f>
-        <v>21.401399999999999</v>
+      <c r="L35" s="35">
+        <f>L34/25</f>
+        <v>23.636599999999998</v>
       </c>
     </row>
   </sheetData>
@@ -3511,8 +3875,7 @@
     <mergeCell ref="K2:L2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P10" r:id="rId1"/>
-    <hyperlink ref="P17" r:id="rId2"/>
+    <hyperlink ref="P19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3521,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3532,24 +3895,60 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added circuits to schematic
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="194">
   <si>
     <t>Number</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Prototype Cost/Unit:</t>
   </si>
   <si>
-    <t>Li200 Circuit</t>
-  </si>
-  <si>
     <t>DS3231 Real Time Clock</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
     <t>Octopart has alt. distributors</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>Murata Electronics</t>
   </si>
   <si>
@@ -463,9 +457,6 @@
     <t>1x6 TH Female Header</t>
   </si>
   <si>
-    <t>1x8 Th Female Header</t>
-  </si>
-  <si>
     <t>1x10 TH Female Header</t>
   </si>
   <si>
@@ -536,6 +527,90 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/E-Switch/EG1218/?qs=sGAEpiMZZMtHXLepoqNyVZDOWY7elTCOE4MJ3sXRkSs%3d</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>0.1uF 50V Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>311-1140-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CC0805KRX7R9BB104/311-1140-1-ND/303050?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TLV2372IDR</t>
+  </si>
+  <si>
+    <t>2-Channel Rail-To-Rail Op-Amp</t>
+  </si>
+  <si>
+    <t>595-TLV2372IDR</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/TLV2372IDR/?qs=sGAEpiMZZMtCHixnSjNA6P3Ssczg4flJu9W%2ftdqxyhc%3d</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>1x3 TH Female Header</t>
+  </si>
+  <si>
+    <t>1x8 TH Female Header</t>
+  </si>
+  <si>
+    <t>C2, C4</t>
+  </si>
+  <si>
+    <t>Li200-ADC Connections</t>
+  </si>
+  <si>
+    <t>Li200 Resistor Values</t>
+  </si>
+  <si>
+    <t>ADS1115</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>Gain Resistor</t>
+  </si>
+  <si>
+    <t>Not added yet</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Bosch Sensortec</t>
+  </si>
+  <si>
+    <t>Digital Barometer</t>
+  </si>
+  <si>
+    <t>262-BMP280</t>
+  </si>
+  <si>
+    <t>LGA-8</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Bosch-Sensortec/BMP280/?qs=QhAb4EtQfbUP9Z%252bCHM3Wyg%3D%3D</t>
+  </si>
+  <si>
+    <t>C3, C5, C6</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1073,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1106,6 +1181,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1493,7 +1575,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="30"/>
     </row>
@@ -1522,7 +1604,7 @@
       <c r="L2" s="70"/>
       <c r="M2" s="71"/>
       <c r="N2" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1530,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>11</v>
@@ -1570,7 +1652,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1597,25 +1679,25 @@
         <v>18.75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>24</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1644,23 +1726,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="44" t="s">
         <v>41</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1689,17 +1771,17 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="44" t="s">
         <v>45</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2365,10 +2447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2394,17 +2476,17 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2435,24 +2517,24 @@
       <c r="O2" s="70"/>
       <c r="P2" s="71"/>
       <c r="Q2" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>77</v>
-      </c>
       <c r="D3" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>11</v>
@@ -2479,43 +2561,43 @@
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>12</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q3" s="68"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>84</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="37">
         <v>0.83</v>
       </c>
       <c r="H4" s="38">
-        <f t="shared" ref="H4:H33" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H34" si="0">F4*G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="42">
         <v>0.73899999999999999</v>
       </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J33" si="1">F4*I4*10</f>
+        <f t="shared" ref="J4:J34" si="1">F4*I4*10</f>
         <v>0</v>
       </c>
       <c r="K4" s="42">
@@ -2523,38 +2605,38 @@
         <v>0.73899999999999999</v>
       </c>
       <c r="L4" s="43">
-        <f t="shared" ref="L4:L33" si="2">F4*K4*25</f>
+        <f t="shared" ref="L4:L34" si="2">F4*K4*25</f>
         <v>0</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O4" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="39">
@@ -2580,36 +2662,36 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="P5" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="O5" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="Q5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>94</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>95</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -2636,34 +2718,34 @@
         <v>135.75</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="P6" s="19" t="s">
         <v>48</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>49</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B7" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="58" t="s">
+      <c r="E7" s="57" t="s">
         <v>109</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>110</v>
       </c>
       <c r="F7" s="59">
         <v>1</v>
@@ -2690,34 +2772,34 @@
         <v>2.81</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="O7" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="P7" s="64" t="s">
         <v>112</v>
-      </c>
-      <c r="P7" s="64" t="s">
-        <v>113</v>
       </c>
       <c r="Q7" s="59"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>97</v>
-      </c>
       <c r="E8" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2744,34 +2826,34 @@
         <v>37.25</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>31</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2798,34 +2880,34 @@
         <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="25" t="s">
         <v>124</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>126</v>
       </c>
       <c r="F10" s="4">
         <v>13</v>
@@ -2852,51 +2934,51 @@
         <v>4.9399999999999995</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="39">
         <v>0.25</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I11" s="21">
         <v>0.20799999999999999</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="4"/>
-        <v>2.08</v>
+        <v>4.16</v>
       </c>
       <c r="K11" s="21">
         <f>I11</f>
@@ -2904,37 +2986,37 @@
       </c>
       <c r="L11" s="20">
         <f t="shared" si="5"/>
-        <v>5.2</v>
+        <v>10.4</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="P11" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="O11" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>101</v>
-      </c>
       <c r="E12" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -2962,28 +3044,28 @@
         <v>13.625000000000002</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O12" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="29"/>
       <c r="E13" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -3011,13 +3093,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="32"/>
       <c r="E14" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -3045,19 +3127,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -3084,34 +3166,34 @@
         <v>13.275</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="32" t="s">
-        <v>103</v>
-      </c>
       <c r="E16" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -3138,34 +3220,34 @@
         <v>24.675000000000001</v>
       </c>
       <c r="M16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="O16" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -3192,34 +3274,34 @@
         <v>21.5</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P17" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="O17" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -3246,34 +3328,34 @@
         <v>22.56</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O18" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -3300,34 +3382,34 @@
         <v>59.5</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -3354,30 +3436,30 @@
         <v>30.490000000000002</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P20" s="19" t="s">
         <v>64</v>
-      </c>
-      <c r="O20" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>65</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C21" s="57"/>
       <c r="D21" s="58"/>
       <c r="E21" s="57" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F21" s="59">
         <v>1</v>
@@ -3400,24 +3482,24 @@
       <c r="M21" s="56"/>
       <c r="N21" s="57"/>
       <c r="O21" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P21" s="64"/>
       <c r="Q21" s="59" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="66"/>
       <c r="E22" s="57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F22" s="59">
         <v>1</v>
@@ -3440,24 +3522,24 @@
       <c r="M22" s="56"/>
       <c r="N22" s="57"/>
       <c r="O22" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P22" s="64"/>
       <c r="Q22" s="59" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="58"/>
       <c r="E23" s="57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F23" s="59">
         <v>1</v>
@@ -3480,24 +3562,24 @@
       <c r="M23" s="56"/>
       <c r="N23" s="57"/>
       <c r="O23" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P23" s="64"/>
       <c r="Q23" s="59" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" s="57"/>
       <c r="D24" s="58"/>
       <c r="E24" s="57" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="F24" s="59">
         <v>2</v>
@@ -3520,24 +3602,24 @@
       <c r="M24" s="56"/>
       <c r="N24" s="57"/>
       <c r="O24" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P24" s="64"/>
       <c r="Q24" s="59" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="C25" s="57"/>
       <c r="D25" s="58"/>
       <c r="E25" s="57" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="F25" s="59">
         <v>1</v>
@@ -3560,207 +3642,308 @@
       <c r="M25" s="56"/>
       <c r="N25" s="57"/>
       <c r="O25" s="58" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P25" s="64"/>
       <c r="Q25" s="59" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="25" t="s">
+      <c r="A26" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="59">
+        <v>1</v>
+      </c>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="62"/>
+      <c r="J26" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="62"/>
+      <c r="L26" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="56"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="64"/>
+      <c r="Q26" s="59" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7</v>
+      </c>
+      <c r="G27" s="39">
+        <v>0.22</v>
+      </c>
+      <c r="H27" s="26">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J27" s="20">
+        <f t="shared" si="1"/>
+        <v>12.46</v>
+      </c>
+      <c r="K27" s="21">
+        <f>I27</f>
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="L27" s="20">
+        <f t="shared" si="2"/>
+        <v>31.15</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="O27" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="P27" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="F26" s="4">
-        <v>7</v>
-      </c>
-      <c r="G26" s="39">
-        <v>0.22</v>
-      </c>
-      <c r="H26" s="26">
-        <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-      <c r="I26" s="21">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="J26" s="20">
-        <f t="shared" si="1"/>
-        <v>12.46</v>
-      </c>
-      <c r="K26" s="21">
-        <f>I26</f>
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="L26" s="20">
-        <f t="shared" si="2"/>
-        <v>31.15</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="O26" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="P26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q26" s="4"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="21"/>
-      <c r="L27" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="19"/>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="39"/>
+      <c r="A28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="39">
+        <v>0.1</v>
+      </c>
       <c r="H28" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="21"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I28" s="21">
+        <v>5.0999999999999997E-2</v>
+      </c>
       <c r="J28" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="21"/>
+        <v>1.53</v>
+      </c>
+      <c r="K28" s="21">
+        <v>3.56E-2</v>
+      </c>
       <c r="L28" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="19"/>
+        <v>2.67</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O28" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="P28" s="19" t="s">
+        <v>169</v>
+      </c>
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="39"/>
+      <c r="A29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="39">
+        <v>1.61</v>
+      </c>
       <c r="H29" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="21"/>
+        <v>1.61</v>
+      </c>
+      <c r="I29" s="21">
+        <v>1.37</v>
+      </c>
       <c r="J29" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="21"/>
+        <v>13.700000000000001</v>
+      </c>
+      <c r="K29" s="21">
+        <f>I29</f>
+        <v>1.37</v>
+      </c>
       <c r="L29" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="29"/>
-      <c r="P29" s="4"/>
+        <v>34.25</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O29" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="21"/>
-      <c r="J30" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="21"/>
-      <c r="L30" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+      <c r="A30" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="57" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="59">
+        <v>1</v>
+      </c>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="62"/>
+      <c r="J30" s="63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="62"/>
+      <c r="L30" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="56"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="F31" s="76">
+        <v>1</v>
+      </c>
+      <c r="G31" s="77">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H31" s="78">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I31" s="79">
+        <v>2.08</v>
+      </c>
+      <c r="J31" s="80">
+        <f t="shared" si="1"/>
+        <v>20.8</v>
+      </c>
+      <c r="K31" s="79">
+        <v>1.92</v>
+      </c>
+      <c r="L31" s="80">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="M31" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="O31" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="P31" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q31" s="76"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
@@ -3790,78 +3973,106 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
     </row>
-    <row r="33" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="23"/>
-      <c r="J33" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="23"/>
-      <c r="L33" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G34" s="24" t="s">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="21"/>
+      <c r="J33" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="21"/>
+      <c r="L33" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+    </row>
+    <row r="34" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="23"/>
+      <c r="J34" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="23"/>
+      <c r="L34" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="5"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G35" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="24">
-        <f>SUM(H4:H33)</f>
-        <v>30.6</v>
-      </c>
-      <c r="I34" s="24" t="s">
+      <c r="H35" s="24">
+        <f>SUM(H4:H34)</f>
+        <v>35.040000000000006</v>
+      </c>
+      <c r="I35" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="24">
-        <f t="shared" ref="J34:L34" si="6">SUM(J4:J33)</f>
-        <v>266.58999999999992</v>
-      </c>
-      <c r="K34" s="24" t="s">
+      <c r="J35" s="24">
+        <f t="shared" ref="J35:L35" si="6">SUM(J4:J34)</f>
+        <v>304.69999999999987</v>
+      </c>
+      <c r="K35" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L34" s="24">
+      <c r="L35" s="24">
         <f t="shared" si="6"/>
-        <v>590.91499999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G35" t="s">
+        <v>681.03499999999985</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="24">
-        <f>H34</f>
-        <v>30.6</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="H36" s="24">
+        <f>H35</f>
+        <v>35.040000000000006</v>
+      </c>
+      <c r="I36" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="35">
-        <f>J34/10</f>
-        <v>26.658999999999992</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="J36" s="35">
+        <f>J35/10</f>
+        <v>30.469999999999988</v>
+      </c>
+      <c r="K36" t="s">
         <v>15</v>
       </c>
-      <c r="L35" s="35">
-        <f>L34/25</f>
-        <v>23.636599999999998</v>
+      <c r="L36" s="35">
+        <f>L35/25</f>
+        <v>27.241399999999995</v>
       </c>
     </row>
   </sheetData>
@@ -3887,7 +4098,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3897,58 +4108,61 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>134</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added ADC and support parts
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="244">
   <si>
     <t>Number</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Ordering</t>
   </si>
   <si>
-    <t>Number of Prototypes:</t>
-  </si>
-  <si>
     <t>Quantity/Board</t>
   </si>
   <si>
@@ -505,9 +502,6 @@
     <t>Q1-Q7</t>
   </si>
   <si>
-    <t>R1-R13</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -568,18 +562,9 @@
     <t>1x8 TH Female Header</t>
   </si>
   <si>
-    <t>C2, C4</t>
-  </si>
-  <si>
-    <t>Li200-ADC Connections</t>
-  </si>
-  <si>
     <t>Li200 Resistor Values</t>
   </si>
   <si>
-    <t>ADS1115</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -701,6 +686,81 @@
   </si>
   <si>
     <t>Total Quantity Cost</t>
+  </si>
+  <si>
+    <t>TDK Corp.</t>
+  </si>
+  <si>
+    <t>MMZ2012Y152BT000</t>
+  </si>
+  <si>
+    <t>1.5kOhm Imp. 400 mOhm Ferrite Bead</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MMZ2012Y152BT000/445-1560-1-ND/571890?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>445-1560-1-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>ADS1115IDGSR</t>
+  </si>
+  <si>
+    <t>16-bit 4-Channel ADC</t>
+  </si>
+  <si>
+    <t>296-38849-1-ND</t>
+  </si>
+  <si>
+    <t>10-MSOP</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ADS1115IDGSR/296-38849-1-ND/5142969?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>C2, C4, C7</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>AVX Corp.</t>
+  </si>
+  <si>
+    <t>08055A102JAT2A</t>
+  </si>
+  <si>
+    <t>1000pF 50V Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>478-1328-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/08055A102JAT2A/478-1328-1-ND/564360?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>3.3V to ADS1115</t>
+  </si>
+  <si>
+    <t>Resistors on SD Card</t>
+  </si>
+  <si>
+    <t>R1-R13, R19</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>1x1 TH Female Header</t>
   </si>
 </sst>
 </file>
@@ -1165,7 +1225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1286,6 +1346,7 @@
     <xf numFmtId="169" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1644,7 +1705,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1666,14 +1727,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
+      <c r="A1" s="47"/>
+      <c r="B1" s="1"/>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="30"/>
     </row>
@@ -1702,7 +1759,7 @@
       <c r="L2" s="73"/>
       <c r="M2" s="74"/>
       <c r="N2" s="70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1710,28 +1767,28 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>2</v>
@@ -1740,7 +1797,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" s="13" t="s">
         <v>4</v>
@@ -1750,7 +1807,7 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1777,25 +1834,25 @@
         <v>18.75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>23</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1824,23 +1881,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="44" t="s">
         <v>40</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1869,17 +1926,17 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="44" t="s">
         <v>44</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2484,21 +2541,21 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D31" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
         <v>38.72</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
         <v>386.8</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="3"/>
@@ -2508,21 +2565,21 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="24">
         <f>E31</f>
         <v>38.72</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
         <v>38.68</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
@@ -2545,10 +2602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2557,7 +2614,7 @@
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -2574,17 +2631,17 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="77"/>
       <c r="C1" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2597,15 +2654,15 @@
       <c r="E2" s="73"/>
       <c r="F2" s="17"/>
       <c r="G2" s="72" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H2" s="74"/>
       <c r="I2" s="75" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J2" s="74"/>
       <c r="K2" s="72" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="L2" s="74"/>
       <c r="M2" s="72" t="s">
@@ -2615,87 +2672,87 @@
       <c r="O2" s="73"/>
       <c r="P2" s="74"/>
       <c r="Q2" s="70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>76</v>
-      </c>
       <c r="D3" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="F3" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="71"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>83</v>
-      </c>
       <c r="E4" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="78">
         <v>0.83</v>
       </c>
       <c r="H4" s="38">
-        <f t="shared" ref="H4:H37" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H41" si="0">F4*G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="83">
         <v>0.73899999999999999</v>
       </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J37" si="1">F4*I4*10</f>
+        <f t="shared" ref="J4:J41" si="1">F4*I4*10</f>
         <v>0</v>
       </c>
       <c r="K4" s="83">
@@ -2703,38 +2760,38 @@
         <v>0.73899999999999999</v>
       </c>
       <c r="L4" s="43">
-        <f t="shared" ref="L4:L37" si="2">F4*K4*25</f>
+        <f t="shared" ref="L4:L41" si="2">F4*K4*25</f>
         <v>0</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O4" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="79">
@@ -2760,36 +2817,36 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="P5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="O5" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>92</v>
-      </c>
       <c r="Q5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>93</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>94</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -2816,34 +2873,34 @@
         <v>135.75</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="P6" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="58" t="s">
+      <c r="E7" s="57" t="s">
         <v>108</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>109</v>
       </c>
       <c r="F7" s="59">
         <v>1</v>
@@ -2870,34 +2927,34 @@
         <v>2.81</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="O7" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="P7" s="62" t="s">
         <v>111</v>
-      </c>
-      <c r="P7" s="62" t="s">
-        <v>112</v>
       </c>
       <c r="Q7" s="59"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>96</v>
-      </c>
       <c r="E8" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2924,34 +2981,34 @@
         <v>37.25</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="27" t="s">
         <v>29</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>30</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2978,105 +3035,105 @@
         <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="O9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="O9" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="19" t="s">
-        <v>131</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>124</v>
-      </c>
       <c r="F10" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="79">
         <v>0.1</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="3"/>
-        <v>1.3</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="I10" s="84">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
         <f t="shared" si="4"/>
-        <v>2.7300000000000004</v>
+        <v>2.9400000000000004</v>
       </c>
       <c r="K10" s="84">
         <v>1.52E-2</v>
       </c>
       <c r="L10" s="20">
         <f t="shared" si="5"/>
-        <v>4.9399999999999995</v>
+        <v>5.3199999999999994</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="O10" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="P10" s="19" t="s">
-        <v>126</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>118</v>
-      </c>
       <c r="F11" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="79">
         <v>0.25</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I11" s="84">
         <v>0.20799999999999999</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="4"/>
-        <v>4.16</v>
+        <v>6.24</v>
       </c>
       <c r="K11" s="84">
         <f>I11</f>
@@ -3084,37 +3141,37 @@
       </c>
       <c r="L11" s="20">
         <f t="shared" si="5"/>
-        <v>10.4</v>
+        <v>15.6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O11" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="P11" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>100</v>
-      </c>
       <c r="E12" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -3142,34 +3199,34 @@
         <v>13.625000000000002</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="O12" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -3196,34 +3253,34 @@
         <v>3.62</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -3250,34 +3307,34 @@
         <v>3.62</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="O14" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="P14" s="19" t="s">
         <v>213</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -3304,34 +3361,34 @@
         <v>1.44</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -3358,34 +3415,34 @@
         <v>0.76</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -3413,477 +3470,521 @@
         <v>7.1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O17" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="55" t="s">
-        <v>161</v>
+        <v>80</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>220</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>26</v>
+        <v>221</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
       <c r="G18" s="79">
-        <v>0.56000000000000005</v>
+        <v>0.11</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.11</v>
       </c>
       <c r="I18" s="84">
-        <v>0.54200000000000004</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="J18" s="20">
         <f t="shared" si="1"/>
-        <v>5.42</v>
+        <v>0.87999999999999989</v>
       </c>
       <c r="K18" s="84">
-        <v>0.53100000000000003</v>
+        <f>I18</f>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="L18" s="20">
         <f t="shared" si="2"/>
-        <v>13.275</v>
+        <v>2.1999999999999997</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="O18" s="29" t="s">
-        <v>163</v>
+        <v>223</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>119</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>57</v>
+        <v>233</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>101</v>
+        <v>234</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>102</v>
+        <v>235</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>70</v>
+        <v>236</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
       <c r="G19" s="79">
-        <v>1.28</v>
+        <v>0.1</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" si="0"/>
-        <v>1.28</v>
+        <v>0.1</v>
       </c>
       <c r="I19" s="84">
-        <v>1.0669999999999999</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="J19" s="20">
         <f t="shared" si="1"/>
-        <v>10.67</v>
+        <v>0.73</v>
       </c>
       <c r="K19" s="84">
-        <v>0.98699999999999999</v>
+        <v>5.28E-2</v>
       </c>
       <c r="L19" s="20">
         <f t="shared" si="2"/>
-        <v>24.675000000000001</v>
+        <v>1.32</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="O19" s="29" t="s">
-        <v>77</v>
+        <v>237</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>119</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>52</v>
+        <v>238</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>65</v>
+        <v>224</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>103</v>
+        <v>225</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
       <c r="G20" s="79">
-        <v>1.1200000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="H20" s="26">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="I20" s="84">
-        <v>0.92900000000000005</v>
+        <v>5.0720000000000001</v>
       </c>
       <c r="J20" s="20">
         <f t="shared" si="1"/>
-        <v>9.2900000000000009</v>
+        <v>50.72</v>
       </c>
       <c r="K20" s="84">
-        <v>0.86</v>
+        <f>I20</f>
+        <v>5.0720000000000001</v>
       </c>
       <c r="L20" s="20">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>126.8</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O20" s="29" t="s">
-        <v>77</v>
+        <v>227</v>
+      </c>
+      <c r="O20" s="32" t="s">
+        <v>228</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>59</v>
+        <v>229</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>104</v>
+        <v>80</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>159</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
       <c r="G21" s="79">
-        <v>1.17</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="0"/>
-        <v>1.17</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I21" s="84">
-        <v>0.97499999999999998</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
-        <v>9.75</v>
+        <v>5.42</v>
       </c>
       <c r="K21" s="84">
-        <v>0.90239999999999998</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="L21" s="20">
         <f t="shared" si="2"/>
-        <v>22.56</v>
+        <v>13.275</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="O21" s="29" t="s">
-        <v>77</v>
+        <v>161</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C22" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="32" t="s">
-        <v>105</v>
-      </c>
       <c r="E22" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="79">
-        <v>1.55</v>
+        <v>1.28</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="0"/>
-        <v>3.1</v>
+        <v>1.28</v>
       </c>
       <c r="I22" s="84">
-        <v>1.2849999999999999</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="J22" s="20">
         <f t="shared" si="1"/>
-        <v>25.7</v>
+        <v>10.67</v>
       </c>
       <c r="K22" s="84">
-        <v>1.19</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="L22" s="20">
         <f t="shared" si="2"/>
-        <v>59.5</v>
+        <v>24.675000000000001</v>
       </c>
       <c r="M22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N22" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="O22" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
       <c r="G23" s="79">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H23" s="26">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I23" s="84">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J23" s="20">
+        <f t="shared" si="1"/>
+        <v>9.2900000000000009</v>
+      </c>
+      <c r="K23" s="84">
+        <v>0.86</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q23" s="4"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="79">
+        <v>1.17</v>
+      </c>
+      <c r="H24" s="26">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
+      <c r="I24" s="84">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J24" s="20">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="K24" s="84">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="L24" s="20">
+        <f t="shared" si="2"/>
+        <v>22.56</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P24" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="79">
+        <v>1.55</v>
+      </c>
+      <c r="H25" s="26">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="I25" s="84">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="J25" s="20">
+        <f t="shared" si="1"/>
+        <v>25.7</v>
+      </c>
+      <c r="K25" s="84">
+        <v>1.19</v>
+      </c>
+      <c r="L25" s="20">
+        <f t="shared" si="2"/>
+        <v>59.5</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O25" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q25" s="4"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="79">
         <v>1.57</v>
       </c>
-      <c r="H23" s="26">
+      <c r="H26" s="26">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="I23" s="84">
+      <c r="I26" s="84">
         <v>1.3009999999999999</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J26" s="20">
         <f t="shared" si="1"/>
         <v>13.01</v>
       </c>
-      <c r="K23" s="84">
+      <c r="K26" s="84">
         <v>1.2196</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L26" s="20">
         <f t="shared" si="2"/>
         <v>30.490000000000002</v>
       </c>
-      <c r="M23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N23" s="3" t="s">
+      <c r="M26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="P26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="P23" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="59">
-        <v>1</v>
-      </c>
-      <c r="G24" s="80"/>
-      <c r="H24" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="85"/>
-      <c r="J24" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="85"/>
-      <c r="L24" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="56"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="59" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B25" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="63"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="59">
-        <v>1</v>
-      </c>
-      <c r="G25" s="80"/>
-      <c r="H25" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="85"/>
-      <c r="J25" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="85"/>
-      <c r="L25" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="56"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="59" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="59">
-        <v>1</v>
-      </c>
-      <c r="G26" s="80"/>
-      <c r="H26" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="85"/>
-      <c r="J26" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="85"/>
-      <c r="L26" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="56"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="P26" s="62"/>
-      <c r="Q26" s="59" t="s">
-        <v>144</v>
-      </c>
+      <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="58"/>
       <c r="E27" s="57" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="F27" s="59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27" s="80"/>
       <c r="H27" s="60">
@@ -3903,24 +4004,24 @@
       <c r="M27" s="56"/>
       <c r="N27" s="57"/>
       <c r="O27" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P27" s="62"/>
       <c r="Q27" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>176</v>
-      </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
+        <v>145</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="63"/>
+      <c r="D28" s="64"/>
       <c r="E28" s="57" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="F28" s="59">
         <v>1</v>
@@ -3943,24 +4044,24 @@
       <c r="M28" s="56"/>
       <c r="N28" s="57"/>
       <c r="O28" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P28" s="62"/>
       <c r="Q28" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" s="57" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C29" s="57"/>
       <c r="D29" s="58"/>
       <c r="E29" s="57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F29" s="59">
         <v>1</v>
@@ -3983,188 +4084,144 @@
       <c r="M29" s="56"/>
       <c r="N29" s="57"/>
       <c r="O29" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P29" s="62"/>
       <c r="Q29" s="59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F30" s="4">
-        <v>7</v>
-      </c>
-      <c r="G30" s="79">
-        <v>0.22</v>
-      </c>
-      <c r="H30" s="26">
-        <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-      <c r="I30" s="84">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="J30" s="20">
-        <f t="shared" si="1"/>
-        <v>12.46</v>
-      </c>
-      <c r="K30" s="84">
-        <f>I30</f>
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="L30" s="20">
-        <f t="shared" si="2"/>
-        <v>31.15</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="O30" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="P30" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q30" s="4"/>
+      <c r="A30" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="59">
+        <v>2</v>
+      </c>
+      <c r="G30" s="80"/>
+      <c r="H30" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="85"/>
+      <c r="J30" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="85"/>
+      <c r="L30" s="61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="56"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="59" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F31" s="4">
-        <v>3</v>
-      </c>
-      <c r="G31" s="79">
-        <v>0.1</v>
-      </c>
-      <c r="H31" s="26">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="I31" s="84">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="J31" s="20">
-        <f t="shared" si="1"/>
-        <v>1.53</v>
-      </c>
-      <c r="K31" s="84">
-        <v>3.56E-2</v>
-      </c>
-      <c r="L31" s="20">
-        <f t="shared" si="2"/>
-        <v>2.67</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="O31" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="P31" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q31" s="4"/>
+      <c r="A31" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="F31" s="59">
+        <v>1</v>
+      </c>
+      <c r="G31" s="80"/>
+      <c r="H31" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="85"/>
+      <c r="J31" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="85"/>
+      <c r="L31" s="61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="56"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="59" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="A32" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="59">
         <v>1</v>
       </c>
-      <c r="G32" s="79">
-        <v>1.61</v>
-      </c>
-      <c r="H32" s="26">
-        <f t="shared" si="0"/>
-        <v>1.61</v>
-      </c>
-      <c r="I32" s="84">
-        <v>1.37</v>
-      </c>
-      <c r="J32" s="20">
-        <f t="shared" si="1"/>
-        <v>13.700000000000001</v>
-      </c>
-      <c r="K32" s="84">
-        <f>I32</f>
-        <v>1.37</v>
-      </c>
-      <c r="L32" s="20">
-        <f t="shared" si="2"/>
-        <v>34.25</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="O32" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="P32" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q32" s="4"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="85"/>
+      <c r="J32" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="85"/>
+      <c r="L32" s="61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="56"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="59" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="58"/>
       <c r="E33" s="57" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="F33" s="59">
         <v>1</v>
@@ -4186,194 +4243,398 @@
       </c>
       <c r="M33" s="56"/>
       <c r="N33" s="57"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="59"/>
+      <c r="O33" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="P33" s="62"/>
       <c r="Q33" s="59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F34" s="4">
+        <v>7</v>
+      </c>
+      <c r="G34" s="79">
+        <v>0.22</v>
+      </c>
+      <c r="H34" s="26">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="I34" s="84">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J34" s="20">
+        <f t="shared" si="1"/>
+        <v>12.46</v>
+      </c>
+      <c r="K34" s="84">
+        <f>I34</f>
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="L34" s="20">
+        <f t="shared" si="2"/>
+        <v>31.15</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O34" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="P34" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q34" s="4"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3</v>
+      </c>
+      <c r="G35" s="79">
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="26">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I35" s="84">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J35" s="20">
+        <f t="shared" si="1"/>
+        <v>1.53</v>
+      </c>
+      <c r="K35" s="84">
+        <v>3.56E-2</v>
+      </c>
+      <c r="L35" s="20">
+        <f t="shared" si="2"/>
+        <v>2.67</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="O35" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="P35" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="79">
+        <v>1.61</v>
+      </c>
+      <c r="H36" s="26">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+      <c r="I36" s="84">
+        <v>1.37</v>
+      </c>
+      <c r="J36" s="20">
+        <f t="shared" si="1"/>
+        <v>13.700000000000001</v>
+      </c>
+      <c r="K36" s="84">
+        <f>I36</f>
+        <v>1.37</v>
+      </c>
+      <c r="L36" s="20">
+        <f t="shared" si="2"/>
+        <v>34.25</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="O36" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="P36" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q36" s="4"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="59">
+        <v>1</v>
+      </c>
+      <c r="G37" s="80"/>
+      <c r="H37" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="85"/>
+      <c r="J37" s="61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="85"/>
+      <c r="L37" s="61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="56"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" s="66">
+        <v>1</v>
+      </c>
+      <c r="G38" s="81">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H38" s="67">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I38" s="86">
+        <v>2.08</v>
+      </c>
+      <c r="J38" s="68">
+        <f t="shared" si="1"/>
+        <v>20.8</v>
+      </c>
+      <c r="K38" s="86">
+        <v>1.92</v>
+      </c>
+      <c r="L38" s="68">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="M38" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="O38" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="65" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="25" t="s">
+      <c r="P38" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="66">
+      <c r="Q38" s="66"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="84"/>
+      <c r="J39" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="84"/>
+      <c r="L39" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="84"/>
+      <c r="J40" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="84"/>
+      <c r="L40" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+    </row>
+    <row r="41" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="82"/>
+      <c r="H41" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="87"/>
+      <c r="J41" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="87"/>
+      <c r="L41" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G42" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="H42" s="24">
+        <f>SUM(H4:H41)</f>
+        <v>42.51</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="J42" s="24">
+        <f t="shared" ref="J42:L42" si="6">SUM(J4:J41)</f>
+        <v>367.29999999999995</v>
+      </c>
+      <c r="K42" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="L42" s="24">
+        <f t="shared" si="6"/>
+        <v>833.4749999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
         <v>1</v>
       </c>
-      <c r="G34" s="81">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="H34" s="67">
-        <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="I34" s="86">
-        <v>2.08</v>
-      </c>
-      <c r="J34" s="68">
-        <f t="shared" si="1"/>
-        <v>20.8</v>
-      </c>
-      <c r="K34" s="86">
-        <v>1.92</v>
-      </c>
-      <c r="L34" s="68">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="M34" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="N34" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="O34" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="P34" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q34" s="66"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="84"/>
-      <c r="J35" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="84"/>
-      <c r="L35" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="84"/>
-      <c r="J36" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="84"/>
-      <c r="L36" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-    </row>
-    <row r="37" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="87"/>
-      <c r="J37" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K37" s="87"/>
-      <c r="L37" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="5"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G38" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="24">
-        <f>SUM(H4:H37)</f>
-        <v>36.299999999999997</v>
-      </c>
-      <c r="I38" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="24">
-        <f t="shared" ref="J38:L38" si="6">SUM(J4:J37)</f>
-        <v>312.67999999999989</v>
-      </c>
-      <c r="K38" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L38" s="24">
-        <f t="shared" si="6"/>
-        <v>697.57499999999993</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="24">
-        <f>H38</f>
-        <v>36.299999999999997</v>
-      </c>
-      <c r="I39" t="s">
-        <v>15</v>
-      </c>
-      <c r="J39" s="35">
-        <f>J38/10</f>
-        <v>31.26799999999999</v>
-      </c>
-      <c r="K39" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" s="35">
-        <f>L38/25</f>
-        <v>27.902999999999999</v>
+      <c r="H43" s="24">
+        <f>H42</f>
+        <v>42.51</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43" s="35">
+        <f>J42/10</f>
+        <v>36.729999999999997</v>
+      </c>
+      <c r="K43" t="s">
+        <v>1</v>
+      </c>
+      <c r="L43" s="35">
+        <f>L42/25</f>
+        <v>33.338999999999992</v>
       </c>
     </row>
   </sheetData>
@@ -4387,7 +4648,8 @@
     <mergeCell ref="K2:L2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P22" r:id="rId1"/>
+    <hyperlink ref="P25" r:id="rId1"/>
+    <hyperlink ref="P38" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4398,8 +4660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4409,53 +4671,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added final schematic parts
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="244">
   <si>
     <t>Number</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Part Number</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -274,24 +271,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Wurth Electronics</t>
-  </si>
-  <si>
-    <t>691103110002</t>
-  </si>
-  <si>
-    <t>691103110003</t>
-  </si>
-  <si>
-    <t>710-691103110002</t>
-  </si>
-  <si>
     <t>SMT</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Wurth-Electronics/691103110002/?qs=%2fha2pyFadujUbUS%252bt6nLituZRCwZEM9J%252bNVrPRp0gdDl8b75rjMxqA%3d%3d</t>
-  </si>
-  <si>
     <t>3.5mm Spacing TH</t>
   </si>
   <si>
@@ -301,12 +283,6 @@
     <t>SMT = Surface Mount</t>
   </si>
   <si>
-    <t>710-691103110003</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Wurth-Electronics/691103110003/?qs=%2fha2pyFadujUbUS%252bt6nLipVHXF0Oc0gS7k5BkdvmKReUZjE00BGlMQ%3d%3d</t>
-  </si>
-  <si>
     <t>TSR 1-2450</t>
   </si>
   <si>
@@ -430,33 +406,6 @@
     <t>Screw Terminals</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>J9, J10</t>
-  </si>
-  <si>
-    <t>J12</t>
-  </si>
-  <si>
-    <t>2x3 TH Female Header</t>
-  </si>
-  <si>
-    <t>1x5 TH Female Header</t>
-  </si>
-  <si>
-    <t>1x6 TH Female Header</t>
-  </si>
-  <si>
-    <t>1x10 TH Female Header</t>
-  </si>
-  <si>
     <t>0.1" TH</t>
   </si>
   <si>
@@ -499,9 +448,6 @@
     <t>Solar panel Open Voltage - change reverse mosfet if necessary</t>
   </si>
   <si>
-    <t>Q1-Q7</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -559,9 +505,6 @@
     <t>1x3 TH Female Header</t>
   </si>
   <si>
-    <t>1x8 TH Female Header</t>
-  </si>
-  <si>
     <t>Li200 Resistor Values</t>
   </si>
   <si>
@@ -748,19 +691,76 @@
     <t>http://www.digikey.com/product-detail/en/08055A102JAT2A/478-1328-1-ND/564360?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>3.3V to ADS1115</t>
-  </si>
-  <si>
     <t>Resistors on SD Card</t>
   </si>
   <si>
-    <t>R1-R13, R19</t>
-  </si>
-  <si>
     <t>J14</t>
   </si>
   <si>
     <t>1x1 TH Female Header</t>
+  </si>
+  <si>
+    <t>Solar Panel Battery voltage for resistor divider</t>
+  </si>
+  <si>
+    <t>On Shore Technology Inc.</t>
+  </si>
+  <si>
+    <t>OSTTE020104</t>
+  </si>
+  <si>
+    <t>ED2740-ND</t>
+  </si>
+  <si>
+    <t>OSTTE040104</t>
+  </si>
+  <si>
+    <t>ED2742-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/on-shore-technology-inc/OSTTE020104/ED2740-ND/2351816</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/on-shore-technology-inc/OSTTE040104/ED2742-ND/2351818</t>
+  </si>
+  <si>
+    <t>J15-J26</t>
+  </si>
+  <si>
+    <t>J27-J30</t>
+  </si>
+  <si>
+    <t>SAMD21 Dev Board</t>
+  </si>
+  <si>
+    <t>Quantity/Prototype</t>
+  </si>
+  <si>
+    <t>Sparkfun</t>
+  </si>
+  <si>
+    <t>DEV-13672</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/13672</t>
+  </si>
+  <si>
+    <t>Arduino Stacking Headers</t>
+  </si>
+  <si>
+    <t>1528-1074-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?mpart=85&amp;vendor=1528</t>
+  </si>
+  <si>
+    <t>Alt. Source: https://www.adafruit.com/product/85</t>
+  </si>
+  <si>
+    <t>Q1-Q7, Q10</t>
+  </si>
+  <si>
+    <t>R1-R13, R19-R21</t>
   </si>
 </sst>
 </file>
@@ -771,8 +771,8 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1225,7 +1225,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1301,17 +1301,22 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1336,17 +1341,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1704,15 +1698,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
@@ -1729,37 +1723,37 @@
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="82"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="83"/>
+      <c r="F2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="72" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75" t="s">
+      <c r="G2" s="83"/>
+      <c r="H2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="72" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="76"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="70" t="s">
-        <v>30</v>
+      <c r="K2" s="85"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="79" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1767,47 +1761,47 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>10</v>
+        <v>234</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="71"/>
+      <c r="N3" s="80"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="46">
         <v>1</v>
@@ -1834,25 +1828,25 @@
         <v>18.75</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>22</v>
-      </c>
       <c r="N4" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1881,23 +1875,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" s="44" t="s">
         <v>39</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1926,68 +1920,107 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="44" t="s">
         <v>43</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="39">
+        <v>24.95</v>
+      </c>
       <c r="E7" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="21"/>
+        <v>24.95</v>
+      </c>
+      <c r="F7" s="21">
+        <v>23.7</v>
+      </c>
       <c r="G7" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="21"/>
+        <v>237</v>
+      </c>
+      <c r="H7" s="21">
+        <v>22.46</v>
+      </c>
       <c r="I7" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="19"/>
+        <v>561.5</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>237</v>
+      </c>
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39">
+        <v>1.95</v>
+      </c>
       <c r="E8" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="21"/>
+        <v>1.95</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1.7549999999999999</v>
+      </c>
       <c r="G8" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="21"/>
+        <v>17.549999999999997</v>
+      </c>
+      <c r="H8" s="21">
+        <f>F8</f>
+        <v>1.7549999999999999</v>
+      </c>
       <c r="I8" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="44"/>
+        <v>43.875</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="N8" s="44" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
@@ -2541,49 +2574,49 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D31" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>38.72</v>
+        <v>65.62</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
-        <v>386.8</v>
+        <v>641.34999999999991</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="3"/>
-        <v>966.25</v>
+        <v>1571.625</v>
       </c>
       <c r="L31" s="30"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>38.72</v>
+        <v>65.62</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>38.68</v>
+        <v>64.134999999999991</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>38.65</v>
+        <v>62.865000000000002</v>
       </c>
       <c r="L32" s="30"/>
     </row>
@@ -2602,17 +2635,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
@@ -2630,242 +2663,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="77"/>
+      <c r="A1" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="86"/>
       <c r="C1" s="52" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
+      <c r="A2" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="72" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75" t="s">
-        <v>215</v>
-      </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="72" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="74"/>
-      <c r="M2" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="70" t="s">
-        <v>30</v>
+      <c r="G2" s="81" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="83"/>
+      <c r="I2" s="84" t="s">
+        <v>196</v>
+      </c>
+      <c r="J2" s="83"/>
+      <c r="K2" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="L2" s="83"/>
+      <c r="M2" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="85"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="79" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>75</v>
-      </c>
       <c r="D3" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="F3" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q3" s="71"/>
+        <v>118</v>
+      </c>
+      <c r="Q3" s="80"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>231</v>
+      </c>
       <c r="C4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="46">
+        <v>12</v>
+      </c>
+      <c r="G4" s="68">
+        <v>0.38</v>
+      </c>
+      <c r="H4" s="38">
+        <f t="shared" ref="H4:H36" si="0">F4*G4</f>
+        <v>4.5600000000000005</v>
+      </c>
+      <c r="I4" s="73">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="J4" s="43">
+        <f t="shared" ref="J4:J36" si="1">F4*I4*10</f>
+        <v>43.680000000000007</v>
+      </c>
+      <c r="K4" s="73">
+        <v>0.312</v>
+      </c>
+      <c r="L4" s="43">
+        <f t="shared" ref="L4:L36" si="2">F4*K4*25</f>
+        <v>93.6</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="O4" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="78">
-        <v>0.83</v>
-      </c>
-      <c r="H4" s="38">
-        <f t="shared" ref="H4:H41" si="0">F4*G4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="83">
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="J4" s="43">
-        <f t="shared" ref="J4:J41" si="1">F4*I4*10</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="83">
-        <f>I4</f>
-        <v>0.73899999999999999</v>
-      </c>
-      <c r="L4" s="43">
-        <f t="shared" ref="L4:L41" si="2">F4*K4*25</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" s="49" t="s">
-        <v>87</v>
-      </c>
       <c r="P4" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="C5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="69">
+        <v>0.67</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" si="0"/>
+        <v>2.68</v>
+      </c>
+      <c r="I5" s="74">
+        <v>0.624</v>
+      </c>
+      <c r="J5" s="20">
+        <f t="shared" si="1"/>
+        <v>24.96</v>
+      </c>
+      <c r="K5" s="74">
+        <v>0.56159999999999999</v>
+      </c>
+      <c r="L5" s="20">
+        <f t="shared" si="2"/>
+        <v>56.16</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="O5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="79">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H5" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="84">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="J5" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="84">
-        <f>I5</f>
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="L5" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>87</v>
-      </c>
       <c r="P5" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="79">
+      <c r="G6" s="69">
         <v>6.2</v>
       </c>
       <c r="H6" s="26">
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
-      <c r="I6" s="84">
+      <c r="I6" s="74">
         <v>5.7</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="74">
         <v>5.43</v>
       </c>
       <c r="L6" s="20">
@@ -2873,53 +2908,53 @@
         <v>135.75</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="P6" s="19" t="s">
         <v>46</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>47</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F7" s="59">
         <v>1</v>
       </c>
-      <c r="G7" s="80">
+      <c r="G7" s="70">
         <v>0.22</v>
       </c>
       <c r="H7" s="60">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="I7" s="85">
+      <c r="I7" s="75">
         <v>0.153</v>
       </c>
       <c r="J7" s="61">
         <f t="shared" si="1"/>
         <v>1.53</v>
       </c>
-      <c r="K7" s="85">
+      <c r="K7" s="75">
         <v>0.1124</v>
       </c>
       <c r="L7" s="61">
@@ -2927,53 +2962,53 @@
         <v>2.81</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N7" s="57" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="O7" s="58" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="P7" s="62" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="Q7" s="59"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="79">
+      <c r="G8" s="69">
         <v>1.74</v>
       </c>
       <c r="H8" s="26">
         <f t="shared" ref="H8:H13" si="3">F8*G8</f>
         <v>1.74</v>
       </c>
-      <c r="I8" s="84">
+      <c r="I8" s="74">
         <v>1.74</v>
       </c>
       <c r="J8" s="20">
         <f t="shared" ref="J8:J13" si="4">F8*I8*10</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="K8" s="84">
+      <c r="K8" s="74">
         <v>1.49</v>
       </c>
       <c r="L8" s="20">
@@ -2981,53 +3016,53 @@
         <v>37.25</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="27" t="s">
         <v>28</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="79">
+      <c r="G9" s="69">
         <v>9.9700000000000006</v>
       </c>
       <c r="H9" s="26">
         <f t="shared" si="3"/>
         <v>9.9700000000000006</v>
       </c>
-      <c r="I9" s="84">
+      <c r="I9" s="74">
         <v>9.41</v>
       </c>
       <c r="J9" s="20">
         <f t="shared" si="4"/>
         <v>94.1</v>
       </c>
-      <c r="K9" s="84">
+      <c r="K9" s="74">
         <v>7.5275999999999996</v>
       </c>
       <c r="L9" s="20">
@@ -3035,107 +3070,107 @@
         <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F10" s="4">
-        <v>14</v>
-      </c>
-      <c r="G10" s="79">
+        <v>16</v>
+      </c>
+      <c r="G10" s="69">
         <v>0.1</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="3"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="I10" s="84">
+        <v>1.6</v>
+      </c>
+      <c r="I10" s="74">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
         <f t="shared" si="4"/>
-        <v>2.9400000000000004</v>
-      </c>
-      <c r="K10" s="84">
+        <v>3.3600000000000003</v>
+      </c>
+      <c r="K10" s="74">
         <v>1.52E-2</v>
       </c>
       <c r="L10" s="20">
         <f t="shared" si="5"/>
-        <v>5.3199999999999994</v>
+        <v>6.08</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11" s="79">
+      <c r="G11" s="69">
         <v>0.25</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="I11" s="84">
+      <c r="I11" s="74">
         <v>0.20799999999999999</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="4"/>
         <v>6.24</v>
       </c>
-      <c r="K11" s="84">
+      <c r="K11" s="74">
         <f>I11</f>
         <v>0.20799999999999999</v>
       </c>
@@ -3144,53 +3179,53 @@
         <v>15.6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="79">
+      <c r="G12" s="69">
         <v>0.57999999999999996</v>
       </c>
       <c r="H12" s="26">
         <f t="shared" si="3"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="I12" s="84">
+      <c r="I12" s="74">
         <v>0.54500000000000004</v>
       </c>
       <c r="J12" s="20">
         <f t="shared" si="4"/>
         <v>5.45</v>
       </c>
-      <c r="K12" s="84">
+      <c r="K12" s="74">
         <f>I12</f>
         <v>0.54500000000000004</v>
       </c>
@@ -3199,53 +3234,53 @@
         <v>13.625000000000002</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="O12" s="32" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="79">
+      <c r="G13" s="69">
         <v>0.27</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" si="3"/>
         <v>0.27</v>
       </c>
-      <c r="I13" s="84">
+      <c r="I13" s="74">
         <v>0.19600000000000001</v>
       </c>
       <c r="J13" s="20">
         <f t="shared" si="4"/>
         <v>1.96</v>
       </c>
-      <c r="K13" s="84">
+      <c r="K13" s="74">
         <v>0.14480000000000001</v>
       </c>
       <c r="L13" s="20">
@@ -3253,53 +3288,53 @@
         <v>3.62</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="79">
+      <c r="G14" s="69">
         <v>0.27</v>
       </c>
       <c r="H14" s="26">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="I14" s="84">
+      <c r="I14" s="74">
         <v>0.19600000000000001</v>
       </c>
       <c r="J14" s="20">
         <f t="shared" si="1"/>
         <v>1.96</v>
       </c>
-      <c r="K14" s="84">
+      <c r="K14" s="74">
         <v>0.14480000000000001</v>
       </c>
       <c r="L14" s="20">
@@ -3307,53 +3342,53 @@
         <v>3.62</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
       </c>
-      <c r="G15" s="79">
+      <c r="G15" s="69">
         <v>0.1</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I15" s="84">
+      <c r="I15" s="74">
         <v>0.04</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="K15" s="84">
+      <c r="K15" s="74">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="L15" s="20">
@@ -3361,53 +3396,53 @@
         <v>1.44</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="79">
+      <c r="G16" s="69">
         <v>0.1</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I16" s="84">
+      <c r="I16" s="74">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J16" s="20">
         <f t="shared" si="1"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="K16" s="84">
+      <c r="K16" s="74">
         <v>1.52E-2</v>
       </c>
       <c r="L16" s="20">
@@ -3415,53 +3450,53 @@
         <v>0.76</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
       </c>
-      <c r="G17" s="79">
+      <c r="G17" s="69">
         <v>0.16</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="I17" s="84">
+      <c r="I17" s="74">
         <v>0.14199999999999999</v>
       </c>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
         <v>2.84</v>
       </c>
-      <c r="K17" s="84">
+      <c r="K17" s="74">
         <f>I17</f>
         <v>0.14199999999999999</v>
       </c>
@@ -3470,53 +3505,53 @@
         <v>7.1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="O17" s="32" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="79">
+      <c r="G18" s="69">
         <v>0.11</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="I18" s="84">
+      <c r="I18" s="74">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="J18" s="20">
         <f t="shared" si="1"/>
         <v>0.87999999999999989</v>
       </c>
-      <c r="K18" s="84">
+      <c r="K18" s="74">
         <f>I18</f>
         <v>8.7999999999999995E-2</v>
       </c>
@@ -3525,53 +3560,53 @@
         <v>2.1999999999999997</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="O18" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="G19" s="79">
+      <c r="G19" s="69">
         <v>0.1</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I19" s="84">
+      <c r="I19" s="74">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="J19" s="20">
         <f t="shared" si="1"/>
         <v>0.73</v>
       </c>
-      <c r="K19" s="84">
+      <c r="K19" s="74">
         <v>5.28E-2</v>
       </c>
       <c r="L19" s="20">
@@ -3579,53 +3614,53 @@
         <v>1.32</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="O19" s="32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="79">
+      <c r="G20" s="69">
         <v>5.65</v>
       </c>
       <c r="H20" s="26">
         <f t="shared" si="0"/>
         <v>5.65</v>
       </c>
-      <c r="I20" s="84">
+      <c r="I20" s="74">
         <v>5.0720000000000001</v>
       </c>
       <c r="J20" s="20">
         <f t="shared" si="1"/>
         <v>50.72</v>
       </c>
-      <c r="K20" s="84">
+      <c r="K20" s="74">
         <f>I20</f>
         <v>5.0720000000000001</v>
       </c>
@@ -3634,53 +3669,53 @@
         <v>126.8</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="79">
+      <c r="G21" s="69">
         <v>0.56000000000000005</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="I21" s="84">
+      <c r="I21" s="74">
         <v>0.54200000000000004</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
         <v>5.42</v>
       </c>
-      <c r="K21" s="84">
+      <c r="K21" s="74">
         <v>0.53100000000000003</v>
       </c>
       <c r="L21" s="20">
@@ -3688,53 +3723,53 @@
         <v>13.275</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="O21" s="29" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="79">
+      <c r="G22" s="69">
         <v>1.28</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-      <c r="I22" s="84">
+      <c r="I22" s="74">
         <v>1.0669999999999999</v>
       </c>
       <c r="J22" s="20">
         <f t="shared" si="1"/>
         <v>10.67</v>
       </c>
-      <c r="K22" s="84">
+      <c r="K22" s="74">
         <v>0.98699999999999999</v>
       </c>
       <c r="L22" s="20">
@@ -3742,53 +3777,53 @@
         <v>24.675000000000001</v>
       </c>
       <c r="M22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N22" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="O22" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="79">
+      <c r="G23" s="69">
         <v>1.1200000000000001</v>
       </c>
       <c r="H23" s="26">
         <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
-      <c r="I23" s="84">
+      <c r="I23" s="74">
         <v>0.92900000000000005</v>
       </c>
       <c r="J23" s="20">
         <f t="shared" si="1"/>
         <v>9.2900000000000009</v>
       </c>
-      <c r="K23" s="84">
+      <c r="K23" s="74">
         <v>0.86</v>
       </c>
       <c r="L23" s="20">
@@ -3796,53 +3831,53 @@
         <v>21.5</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O23" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="P23" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="O23" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="P23" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="79">
+      <c r="G24" s="69">
         <v>1.17</v>
       </c>
       <c r="H24" s="26">
         <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
-      <c r="I24" s="84">
+      <c r="I24" s="74">
         <v>0.97499999999999998</v>
       </c>
       <c r="J24" s="20">
         <f t="shared" si="1"/>
         <v>9.75</v>
       </c>
-      <c r="K24" s="84">
+      <c r="K24" s="74">
         <v>0.90239999999999998</v>
       </c>
       <c r="L24" s="20">
@@ -3850,53 +3885,53 @@
         <v>22.56</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="79">
+      <c r="G25" s="69">
         <v>1.55</v>
       </c>
       <c r="H25" s="26">
         <f t="shared" si="0"/>
         <v>3.1</v>
       </c>
-      <c r="I25" s="84">
+      <c r="I25" s="74">
         <v>1.2849999999999999</v>
       </c>
       <c r="J25" s="20">
         <f t="shared" si="1"/>
         <v>25.7</v>
       </c>
-      <c r="K25" s="84">
+      <c r="K25" s="74">
         <v>1.19</v>
       </c>
       <c r="L25" s="20">
@@ -3904,53 +3939,53 @@
         <v>59.5</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O25" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
       </c>
-      <c r="G26" s="79">
+      <c r="G26" s="69">
         <v>1.57</v>
       </c>
       <c r="H26" s="26">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="I26" s="84">
+      <c r="I26" s="74">
         <v>1.3009999999999999</v>
       </c>
       <c r="J26" s="20">
         <f t="shared" si="1"/>
         <v>13.01</v>
       </c>
-      <c r="K26" s="84">
+      <c r="K26" s="74">
         <v>1.2196</v>
       </c>
       <c r="L26" s="20">
@@ -3958,45 +3993,45 @@
         <v>30.490000000000002</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O26" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="P26" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="O26" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="P26" s="19" t="s">
-        <v>63</v>
       </c>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>133</v>
+        <v>221</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="58"/>
       <c r="E27" s="57" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="F27" s="59">
         <v>1</v>
       </c>
-      <c r="G27" s="80"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="60">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="85"/>
+      <c r="I27" s="75"/>
       <c r="J27" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K27" s="85"/>
+      <c r="K27" s="75"/>
       <c r="L27" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4004,39 +4039,39 @@
       <c r="M27" s="56"/>
       <c r="N27" s="57"/>
       <c r="O27" s="58" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="P27" s="62"/>
       <c r="Q27" s="59" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="63" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="64"/>
+        <v>128</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
       <c r="E28" s="57" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="F28" s="59">
         <v>1</v>
       </c>
-      <c r="G28" s="80"/>
+      <c r="G28" s="70"/>
       <c r="H28" s="60">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="85"/>
+      <c r="I28" s="75"/>
       <c r="J28" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="85"/>
+      <c r="K28" s="75"/>
       <c r="L28" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4044,597 +4079,397 @@
       <c r="M28" s="56"/>
       <c r="N28" s="57"/>
       <c r="O28" s="58" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="P28" s="62"/>
       <c r="Q28" s="59" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="4">
+        <v>8</v>
+      </c>
+      <c r="G29" s="69">
+        <v>0.22</v>
+      </c>
+      <c r="H29" s="26">
+        <f t="shared" si="0"/>
+        <v>1.76</v>
+      </c>
+      <c r="I29" s="74">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="J29" s="20">
+        <f t="shared" si="1"/>
+        <v>14.239999999999998</v>
+      </c>
+      <c r="K29" s="74">
+        <f>I29</f>
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="L29" s="20">
+        <f t="shared" si="2"/>
+        <v>35.6</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O29" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29" s="59">
+      <c r="E30" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3</v>
+      </c>
+      <c r="G30" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="H30" s="26">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I30" s="74">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J30" s="20">
+        <f t="shared" si="1"/>
+        <v>1.53</v>
+      </c>
+      <c r="K30" s="74">
+        <v>3.56E-2</v>
+      </c>
+      <c r="L30" s="20">
+        <f t="shared" si="2"/>
+        <v>2.67</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O30" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="P30" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="80"/>
-      <c r="H29" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="85"/>
-      <c r="J29" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="85"/>
-      <c r="L29" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="56"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="57" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="57" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="59">
-        <v>2</v>
-      </c>
-      <c r="G30" s="80"/>
-      <c r="H30" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="85"/>
-      <c r="J30" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="85"/>
-      <c r="L30" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="56"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B31" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="F31" s="59">
-        <v>1</v>
-      </c>
-      <c r="G31" s="80"/>
-      <c r="H31" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="85"/>
-      <c r="J31" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="85"/>
-      <c r="L31" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="56"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="59" t="s">
-        <v>143</v>
-      </c>
+      <c r="G31" s="69">
+        <v>1.61</v>
+      </c>
+      <c r="H31" s="26">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+      <c r="I31" s="74">
+        <v>1.37</v>
+      </c>
+      <c r="J31" s="20">
+        <f t="shared" si="1"/>
+        <v>13.700000000000001</v>
+      </c>
+      <c r="K31" s="74">
+        <f>I31</f>
+        <v>1.37</v>
+      </c>
+      <c r="L31" s="20">
+        <f t="shared" si="2"/>
+        <v>34.25</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="P31" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="56" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="58"/>
       <c r="E32" s="57" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="F32" s="59">
         <v>1</v>
       </c>
-      <c r="G32" s="80"/>
+      <c r="G32" s="70"/>
       <c r="H32" s="60">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="85"/>
+      <c r="I32" s="75"/>
       <c r="J32" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K32" s="85"/>
+      <c r="K32" s="75"/>
       <c r="L32" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M32" s="56"/>
       <c r="N32" s="57"/>
-      <c r="O32" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="P32" s="62"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="59"/>
       <c r="Q32" s="59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="59">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="64">
         <v>1</v>
       </c>
-      <c r="G33" s="80"/>
-      <c r="H33" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="85"/>
-      <c r="J33" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="85"/>
-      <c r="L33" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="56"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="59" t="s">
-        <v>143</v>
-      </c>
+      <c r="G33" s="71">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="H33" s="65">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I33" s="76">
+        <v>2.08</v>
+      </c>
+      <c r="J33" s="66">
+        <f t="shared" si="1"/>
+        <v>20.8</v>
+      </c>
+      <c r="K33" s="76">
+        <v>1.92</v>
+      </c>
+      <c r="L33" s="66">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="M33" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="O33" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="P33" s="78" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q33" s="64"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="F34" s="4">
-        <v>7</v>
-      </c>
-      <c r="G34" s="79">
-        <v>0.22</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="69"/>
       <c r="H34" s="26">
         <f t="shared" si="0"/>
-        <v>1.54</v>
-      </c>
-      <c r="I34" s="84">
-        <v>0.17799999999999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I34" s="74"/>
       <c r="J34" s="20">
         <f t="shared" si="1"/>
-        <v>12.46</v>
-      </c>
-      <c r="K34" s="84">
-        <f>I34</f>
-        <v>0.17799999999999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K34" s="74"/>
       <c r="L34" s="20">
         <f t="shared" si="2"/>
-        <v>31.15</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="O34" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="P34" s="19" t="s">
-        <v>152</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="F35" s="4">
-        <v>3</v>
-      </c>
-      <c r="G35" s="79">
-        <v>0.1</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="69"/>
       <c r="H35" s="26">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="I35" s="84">
-        <v>5.0999999999999997E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I35" s="74"/>
       <c r="J35" s="20">
         <f t="shared" si="1"/>
-        <v>1.53</v>
-      </c>
-      <c r="K35" s="84">
-        <v>3.56E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K35" s="74"/>
       <c r="L35" s="20">
         <f t="shared" si="2"/>
-        <v>2.67</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="O35" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="P35" s="19" t="s">
-        <v>166</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="4">
+    <row r="36" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="77"/>
+      <c r="J36" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="77"/>
+      <c r="L36" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="5"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G37" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="H37" s="24">
+        <f>SUM(H4:H36)</f>
+        <v>50.17</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="J37" s="24">
+        <f t="shared" ref="J37:L37" si="6">SUM(J4:J36)</f>
+        <v>438.1400000000001</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="L37" s="24">
+        <f t="shared" si="6"/>
+        <v>988.44500000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
         <v>1</v>
       </c>
-      <c r="G36" s="79">
-        <v>1.61</v>
-      </c>
-      <c r="H36" s="26">
-        <f t="shared" si="0"/>
-        <v>1.61</v>
-      </c>
-      <c r="I36" s="84">
-        <v>1.37</v>
-      </c>
-      <c r="J36" s="20">
-        <f t="shared" si="1"/>
-        <v>13.700000000000001</v>
-      </c>
-      <c r="K36" s="84">
-        <f>I36</f>
-        <v>1.37</v>
-      </c>
-      <c r="L36" s="20">
-        <f t="shared" si="2"/>
-        <v>34.25</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="O36" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="P36" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q36" s="4"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="57" t="s">
-        <v>178</v>
-      </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="57" t="s">
-        <v>179</v>
-      </c>
-      <c r="F37" s="59">
+      <c r="H38" s="24">
+        <f>H37</f>
+        <v>50.17</v>
+      </c>
+      <c r="I38" t="s">
         <v>1</v>
       </c>
-      <c r="G37" s="80"/>
-      <c r="H37" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="85"/>
-      <c r="J37" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K37" s="85"/>
-      <c r="L37" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="56"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="F38" s="66">
+      <c r="J38" s="35">
+        <f>J37/10</f>
+        <v>43.814000000000007</v>
+      </c>
+      <c r="K38" t="s">
         <v>1</v>
       </c>
-      <c r="G38" s="81">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="H38" s="67">
-        <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="I38" s="86">
-        <v>2.08</v>
-      </c>
-      <c r="J38" s="68">
-        <f t="shared" si="1"/>
-        <v>20.8</v>
-      </c>
-      <c r="K38" s="86">
-        <v>1.92</v>
-      </c>
-      <c r="L38" s="68">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="M38" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="O38" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="P38" s="88" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q38" s="66"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="84"/>
-      <c r="J39" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K39" s="84"/>
-      <c r="L39" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="29"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="84"/>
-      <c r="J40" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K40" s="84"/>
-      <c r="L40" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-    </row>
-    <row r="41" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="82"/>
-      <c r="H41" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="87"/>
-      <c r="J41" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K41" s="87"/>
-      <c r="L41" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="5"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G42" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="H42" s="24">
-        <f>SUM(H4:H41)</f>
-        <v>42.51</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="J42" s="24">
-        <f t="shared" ref="J42:L42" si="6">SUM(J4:J41)</f>
-        <v>367.29999999999995</v>
-      </c>
-      <c r="K42" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="L42" s="24">
-        <f t="shared" si="6"/>
-        <v>833.4749999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G43" t="s">
-        <v>1</v>
-      </c>
-      <c r="H43" s="24">
-        <f>H42</f>
-        <v>42.51</v>
-      </c>
-      <c r="I43" t="s">
-        <v>1</v>
-      </c>
-      <c r="J43" s="35">
-        <f>J42/10</f>
-        <v>36.729999999999997</v>
-      </c>
-      <c r="K43" t="s">
-        <v>1</v>
-      </c>
-      <c r="L43" s="35">
-        <f>L42/25</f>
-        <v>33.338999999999992</v>
+      <c r="L38" s="35">
+        <f>L37/25</f>
+        <v>39.537800000000004</v>
       </c>
     </row>
   </sheetData>
@@ -4649,7 +4484,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P25" r:id="rId1"/>
-    <hyperlink ref="P38" r:id="rId2"/>
+    <hyperlink ref="P33" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4661,7 +4496,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4671,53 +4506,51 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>239</v>
+      <c r="E2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>124</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
5TM library bug fix, board layout changes
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="245">
   <si>
     <t>Number</t>
   </si>
@@ -649,9 +649,6 @@
     <t>http://www.digikey.com/product-detail/en/on-shore-technology-inc/OSTTE040104/ED2742-ND/2351818</t>
   </si>
   <si>
-    <t>J15-J26</t>
-  </si>
-  <si>
     <t>J27-J30</t>
   </si>
   <si>
@@ -751,9 +748,6 @@
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC101LFBN-RC/S7043-ND/810182</t>
   </si>
   <si>
-    <t>Test Wind</t>
-  </si>
-  <si>
     <t>Fan screwterm and transistor, flyback diode</t>
   </si>
   <si>
@@ -761,6 +755,15 @@
   </si>
   <si>
     <t>LED2</t>
+  </si>
+  <si>
+    <t>Test fan with transistor</t>
+  </si>
+  <si>
+    <t>J7, J15-J26</t>
+  </si>
+  <si>
+    <t>Switch reverse mosfet with schottky</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1767,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
@@ -1936,7 +1939,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1963,23 +1966,23 @@
         <v>561.5</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2010,16 +2013,16 @@
         <v>47</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="N8" s="44" t="s">
         <v>215</v>
-      </c>
-      <c r="N8" s="44" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2637,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2764,7 +2767,7 @@
         <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>206</v>
+        <v>243</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>199</v>
@@ -2776,28 +2779,28 @@
         <v>33</v>
       </c>
       <c r="F4" s="46">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="68">
         <v>0.38</v>
       </c>
       <c r="H4" s="38">
         <f t="shared" ref="H4:H36" si="0">F4*G4</f>
-        <v>4.5600000000000005</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="I4" s="73">
         <v>0.36399999999999999</v>
       </c>
       <c r="J4" s="43">
         <f t="shared" ref="J4:J36" si="1">F4*I4*10</f>
-        <v>43.680000000000007</v>
+        <v>47.32</v>
       </c>
       <c r="K4" s="73">
         <v>0.312</v>
       </c>
       <c r="L4" s="43">
         <f t="shared" ref="L4:L36" si="2">F4*K4*25</f>
-        <v>93.6</v>
+        <v>101.4</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>47</v>
@@ -2818,7 +2821,7 @@
         <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>199</v>
@@ -3088,7 +3091,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>92</v>
@@ -3252,7 +3255,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>162</v>
@@ -3306,7 +3309,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>162</v>
@@ -3747,10 +3750,10 @@
         <v>76</v>
       </c>
       <c r="D22" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="E22" s="25" t="s">
         <v>219</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>220</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -3780,16 +3783,16 @@
         <v>47</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O22" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P22" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q22" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -3803,10 +3806,10 @@
         <v>76</v>
       </c>
       <c r="D23" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" s="25" t="s">
         <v>224</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>225</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -3836,16 +3839,16 @@
         <v>47</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O23" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -3859,10 +3862,10 @@
         <v>76</v>
       </c>
       <c r="D24" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E24" s="25" t="s">
         <v>228</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>229</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -3892,16 +3895,16 @@
         <v>47</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O24" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -3915,10 +3918,10 @@
         <v>76</v>
       </c>
       <c r="D25" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>233</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
@@ -3948,16 +3951,16 @@
         <v>47</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O25" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -3971,10 +3974,10 @@
         <v>76</v>
       </c>
       <c r="D26" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>236</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>237</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -4004,16 +4007,16 @@
         <v>47</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O26" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -4101,7 +4104,7 @@
         <v>63</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>107</v>
@@ -4442,21 +4445,21 @@
       </c>
       <c r="H37" s="24">
         <f>SUM(H4:H36)</f>
-        <v>46.720000000000006</v>
+        <v>47.1</v>
       </c>
       <c r="I37" s="24" t="s">
         <v>186</v>
       </c>
       <c r="J37" s="24">
         <f t="shared" ref="J37:L37" si="6">SUM(J4:J36)</f>
-        <v>407.39000000000004</v>
+        <v>411.02999999999992</v>
       </c>
       <c r="K37" s="24" t="s">
         <v>186</v>
       </c>
       <c r="L37" s="24">
         <f t="shared" si="6"/>
-        <v>917.42000000000007</v>
+        <v>925.22</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -4465,21 +4468,21 @@
       </c>
       <c r="H38" s="24">
         <f>H37</f>
-        <v>46.720000000000006</v>
+        <v>47.1</v>
       </c>
       <c r="I38" t="s">
         <v>1</v>
       </c>
       <c r="J38" s="35">
         <f>J37/10</f>
-        <v>40.739000000000004</v>
+        <v>41.102999999999994</v>
       </c>
       <c r="K38" t="s">
         <v>1</v>
       </c>
       <c r="L38" s="35">
         <f>L37/25</f>
-        <v>36.696800000000003</v>
+        <v>37.008800000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4504,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4535,6 +4538,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>244</v>
+      </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
@@ -4551,7 +4557,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
         <v>106</v>
@@ -4559,7 +4565,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed other 5TM checksum bug
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="246">
   <si>
     <t>Number</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>Switch reverse mosfet with schottky</t>
+  </si>
+  <si>
+    <t>Switch 5TM power mosfet with transistor</t>
   </si>
 </sst>
 </file>
@@ -4508,7 +4511,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4546,6 +4549,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>245</v>
+      </c>
       <c r="E5" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
Switched 5TM power to transistor, added schottky
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="250">
   <si>
     <t>Number</t>
   </si>
@@ -349,9 +349,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Reverse voltage protection</t>
-  </si>
-  <si>
     <t>Fairchild Semiconductor</t>
   </si>
   <si>
@@ -481,9 +478,6 @@
     <t>http://www.digikey.com/product-detail/en/MMBT3904/MMBT3904FSCT-ND/458971?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>Q8, Q9</t>
-  </si>
-  <si>
     <t>R15, R16</t>
   </si>
   <si>
@@ -499,9 +493,6 @@
     <t>http://www.digikey.com/product-detail/en/RC0805FR-07130RL/311-130CRCT-ND/730536?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>R17, R18</t>
-  </si>
-  <si>
     <t>ERJ-6ENF1001V</t>
   </si>
   <si>
@@ -679,12 +670,6 @@
     <t>Alt. Source: https://www.adafruit.com/product/85</t>
   </si>
   <si>
-    <t>Q1-Q7, Q10</t>
-  </si>
-  <si>
-    <t>R1-R13, R19-R21</t>
-  </si>
-  <si>
     <t>PPPC032LFBN-RC</t>
   </si>
   <si>
@@ -763,10 +748,37 @@
     <t>J7, J15-J26</t>
   </si>
   <si>
-    <t>Switch reverse mosfet with schottky</t>
-  </si>
-  <si>
-    <t>Switch 5TM power mosfet with transistor</t>
+    <t>Q4, Q6, Q8, Q9</t>
+  </si>
+  <si>
+    <t>R1-R5, R7, R9, R11, R13, R19-R21</t>
+  </si>
+  <si>
+    <t>R6, R8, R17, R18</t>
+  </si>
+  <si>
+    <t>Swap transistor base resistors with 4.4k</t>
+  </si>
+  <si>
+    <t>Comchip Technology</t>
+  </si>
+  <si>
+    <t>CDBA240L-HF</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>641-1697-1-ND</t>
+  </si>
+  <si>
+    <t>DO-214AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.digikey.com/product-detail/en/comchip-technology/CDBA240L-HF/641-1697-1-ND/5226080 </t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q5, Q7, Q10</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1782,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
@@ -1942,7 +1954,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1969,23 +1981,23 @@
         <v>561.5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2016,16 +2028,16 @@
         <v>47</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2643,14 +2655,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
@@ -2693,15 +2705,15 @@
       <c r="E2" s="82"/>
       <c r="F2" s="17"/>
       <c r="G2" s="81" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H2" s="83"/>
       <c r="I2" s="84" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J2" s="83"/>
       <c r="K2" s="81" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="L2" s="83"/>
       <c r="M2" s="81" t="s">
@@ -2734,22 +2746,22 @@
         <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
@@ -2770,13 +2782,13 @@
         <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>33</v>
@@ -2809,13 +2821,13 @@
         <v>47</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O4" s="49" t="s">
         <v>65</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="Q4" s="4"/>
     </row>
@@ -2824,13 +2836,13 @@
         <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>199</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>202</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>34</v>
@@ -2863,13 +2875,13 @@
         <v>47</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="O5" s="29" t="s">
         <v>65</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
@@ -3094,7 +3106,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>92</v>
@@ -3106,28 +3118,28 @@
         <v>94</v>
       </c>
       <c r="F10" s="4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G10" s="69">
         <v>0.1</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="3"/>
-        <v>1.6</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I10" s="74">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
         <f t="shared" si="4"/>
-        <v>3.3600000000000003</v>
+        <v>2.52</v>
       </c>
       <c r="K10" s="74">
         <v>1.52E-2</v>
       </c>
       <c r="L10" s="20">
         <f t="shared" si="5"/>
-        <v>6.08</v>
+        <v>4.5600000000000005</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>47</v>
@@ -3148,7 +3160,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>84</v>
@@ -3258,13 +3270,13 @@
         <v>63</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>22</v>
@@ -3297,13 +3309,13 @@
         <v>47</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
@@ -3312,13 +3324,13 @@
         <v>63</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>23</v>
@@ -3351,13 +3363,13 @@
         <v>47</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
@@ -3366,52 +3378,52 @@
         <v>63</v>
       </c>
       <c r="B15" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>159</v>
-      </c>
       <c r="D15" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F15" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G15" s="69">
         <v>0.1</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I15" s="74">
         <v>0.04</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="K15" s="74">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="L15" s="20">
         <f t="shared" si="2"/>
-        <v>1.44</v>
+        <v>2.88</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O15" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
@@ -3420,16 +3432,16 @@
         <v>63</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>92</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -3459,13 +3471,13 @@
         <v>47</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O16" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
@@ -3474,33 +3486,33 @@
         <v>63</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>150</v>
+        <v>239</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>147</v>
-      </c>
       <c r="F17" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17" s="69">
         <v>0.16</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>0.32</v>
+        <v>0.64</v>
       </c>
       <c r="I17" s="74">
         <v>0.14199999999999999</v>
       </c>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
-        <v>2.84</v>
+        <v>5.68</v>
       </c>
       <c r="K17" s="74">
         <f>I17</f>
@@ -3508,19 +3520,19 @@
       </c>
       <c r="L17" s="20">
         <f t="shared" si="2"/>
-        <v>7.1</v>
+        <v>14.2</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="P17" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>149</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
@@ -3529,16 +3541,16 @@
         <v>63</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -3569,13 +3581,13 @@
         <v>47</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="O18" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
@@ -3584,16 +3596,16 @@
         <v>63</v>
       </c>
       <c r="B19" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>192</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
@@ -3623,13 +3635,13 @@
         <v>47</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="O19" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
@@ -3638,16 +3650,16 @@
         <v>63</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -3678,13 +3690,13 @@
         <v>47</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
@@ -3693,13 +3705,13 @@
         <v>63</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="D21" s="55" t="s">
         <v>117</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>118</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>24</v>
@@ -3732,13 +3744,13 @@
         <v>15</v>
       </c>
       <c r="N21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O21" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="O21" s="29" t="s">
+      <c r="P21" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
@@ -3753,10 +3765,10 @@
         <v>76</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -3786,16 +3798,16 @@
         <v>47</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="O22" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -3809,10 +3821,10 @@
         <v>76</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -3842,16 +3854,16 @@
         <v>47</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="O23" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -3865,10 +3877,10 @@
         <v>76</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -3898,16 +3910,16 @@
         <v>47</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="O24" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -3921,10 +3933,10 @@
         <v>76</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
@@ -3954,16 +3966,16 @@
         <v>47</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="O25" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -3977,10 +3989,10 @@
         <v>76</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -4010,16 +4022,16 @@
         <v>47</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="O26" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -4027,12 +4039,12 @@
         <v>105</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="58"/>
       <c r="E27" s="57" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F27" s="59">
         <v>1</v>
@@ -4067,12 +4079,12 @@
         <v>105</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28" s="57"/>
       <c r="D28" s="58"/>
       <c r="E28" s="57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="59">
         <v>1</v>
@@ -4107,33 +4119,33 @@
         <v>63</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>216</v>
+        <v>249</v>
       </c>
       <c r="C29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="E29" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>109</v>
-      </c>
       <c r="F29" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G29" s="69">
         <v>0.22</v>
       </c>
       <c r="H29" s="26">
         <f t="shared" si="0"/>
-        <v>1.76</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I29" s="74">
         <v>0.17799999999999999</v>
       </c>
       <c r="J29" s="20">
         <f t="shared" si="1"/>
-        <v>14.239999999999998</v>
+        <v>8.8999999999999986</v>
       </c>
       <c r="K29" s="74">
         <f>I29</f>
@@ -4141,19 +4153,19 @@
       </c>
       <c r="L29" s="20">
         <f t="shared" si="2"/>
-        <v>35.6</v>
+        <v>22.249999999999996</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="O29" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="O29" s="29" t="s">
+      <c r="P29" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="Q29" s="4"/>
     </row>
@@ -4162,16 +4174,16 @@
         <v>63</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>92</v>
       </c>
       <c r="D30" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>123</v>
       </c>
       <c r="F30" s="4">
         <v>3</v>
@@ -4201,13 +4213,13 @@
         <v>47</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O30" s="29" t="s">
         <v>90</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q30" s="4"/>
     </row>
@@ -4216,16 +4228,16 @@
         <v>63</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="D31" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="E31" s="25" t="s">
         <v>128</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>129</v>
       </c>
       <c r="F31" s="4">
         <v>1</v>
@@ -4256,13 +4268,13 @@
         <v>15</v>
       </c>
       <c r="N31" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="O31" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="O31" s="29" t="s">
+      <c r="P31" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="P31" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="Q31" s="4"/>
     </row>
@@ -4271,12 +4283,12 @@
         <v>105</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="58"/>
       <c r="E32" s="57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F32" s="59">
         <v>1</v>
@@ -4301,7 +4313,7 @@
       <c r="O32" s="58"/>
       <c r="P32" s="59"/>
       <c r="Q32" s="59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
@@ -4309,16 +4321,16 @@
         <v>63</v>
       </c>
       <c r="B33" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>139</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>140</v>
       </c>
       <c r="D33" s="32" t="s">
         <v>102</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F33" s="64">
         <v>1</v>
@@ -4348,42 +4360,66 @@
         <v>15</v>
       </c>
       <c r="N33" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O33" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="O33" s="32" t="s">
+      <c r="P33" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="P33" s="78" t="s">
-        <v>144</v>
-      </c>
       <c r="Q33" s="64"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="69"/>
+      <c r="C34" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="69">
+        <v>0.4</v>
+      </c>
       <c r="H34" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="74"/>
+        <v>0.4</v>
+      </c>
+      <c r="I34" s="74">
+        <v>0.31</v>
+      </c>
       <c r="J34" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="74"/>
+        <v>3.1</v>
+      </c>
+      <c r="K34" s="74">
+        <v>0.26119999999999999</v>
+      </c>
       <c r="L34" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="3"/>
-      <c r="O34" s="29"/>
-      <c r="P34" s="4"/>
+        <v>6.5299999999999994</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="O34" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="P34" s="19" t="s">
+        <v>248</v>
+      </c>
       <c r="Q34" s="4"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -4444,25 +4480,25 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G37" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H37" s="24">
         <f>SUM(H4:H36)</f>
-        <v>47.1</v>
+        <v>46.96</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J37" s="24">
         <f t="shared" ref="J37:L37" si="6">SUM(J4:J36)</f>
-        <v>411.02999999999992</v>
+        <v>411.59</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L37" s="24">
         <f t="shared" si="6"/>
-        <v>925.22</v>
+        <v>925.42</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -4471,21 +4507,21 @@
       </c>
       <c r="H38" s="24">
         <f>H37</f>
-        <v>47.1</v>
+        <v>46.96</v>
       </c>
       <c r="I38" t="s">
         <v>1</v>
       </c>
       <c r="J38" s="35">
         <f>J37/10</f>
-        <v>41.102999999999994</v>
+        <v>41.158999999999999</v>
       </c>
       <c r="K38" t="s">
         <v>1</v>
       </c>
       <c r="L38" s="35">
         <f>L37/25</f>
-        <v>37.008800000000001</v>
+        <v>37.016799999999996</v>
       </c>
     </row>
   </sheetData>
@@ -4500,6 +4536,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P33" r:id="rId1"/>
+    <hyperlink ref="P34" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4511,7 +4548,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4524,54 +4561,48 @@
         <v>36</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>244</v>
-      </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>245</v>
-      </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>242</v>
+      </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E7" t="s">
-        <v>106</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Started routing, part changes
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="249">
   <si>
     <t>Number</t>
   </si>
@@ -493,21 +493,6 @@
     <t>http://www.digikey.com/product-detail/en/RC0805FR-07130RL/311-130CRCT-ND/730536?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>ERJ-6ENF1001V</t>
-  </si>
-  <si>
-    <t>1k 1% 1/8W Resistor</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>541-1.00KCCT-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/CRCW08051K00FKEA/541-1.00KCCT-ND/1180783?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
-  </si>
-  <si>
     <t>Lite-On Inc.</t>
   </si>
   <si>
@@ -733,33 +718,18 @@
     <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC101LFBN-RC/S7043-ND/810182</t>
   </si>
   <si>
-    <t>Fan screwterm and transistor, flyback diode</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
     <t>LED2</t>
   </si>
   <si>
-    <t>Test fan with transistor</t>
-  </si>
-  <si>
     <t>J7, J15-J26</t>
   </si>
   <si>
-    <t>Q4, Q6, Q8, Q9</t>
-  </si>
-  <si>
     <t>R1-R5, R7, R9, R11, R13, R19-R21</t>
   </si>
   <si>
-    <t>R6, R8, R17, R18</t>
-  </si>
-  <si>
-    <t>Swap transistor base resistors with 4.4k</t>
-  </si>
-  <si>
     <t>Comchip Technology</t>
   </si>
   <si>
@@ -779,6 +749,33 @@
   </si>
   <si>
     <t>Q1, Q2, Q5, Q7, Q10</t>
+  </si>
+  <si>
+    <t>Battery Resistor Divider</t>
+  </si>
+  <si>
+    <t>4.3k 1% 1/8W Resistor</t>
+  </si>
+  <si>
+    <t>RC0805FR-074K3L</t>
+  </si>
+  <si>
+    <t>311-4.30KCRCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0805FR-074K3L/311-4.30KCRCT-ND/730862?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>DS1, DS2</t>
+  </si>
+  <si>
+    <t>R6, R8, R10, R17, R18</t>
+  </si>
+  <si>
+    <t>Q3, Q4, Q6, Q8, Q9</t>
+  </si>
+  <si>
+    <t>Fan Vcc Switcher?</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
@@ -1954,7 +1951,7 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1981,23 +1978,23 @@
         <v>561.5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2028,16 +2025,16 @@
         <v>47</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2655,8 +2652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2705,15 +2702,15 @@
       <c r="E2" s="82"/>
       <c r="F2" s="17"/>
       <c r="G2" s="81" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H2" s="83"/>
       <c r="I2" s="84" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J2" s="83"/>
       <c r="K2" s="81" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L2" s="83"/>
       <c r="M2" s="81" t="s">
@@ -2746,22 +2743,22 @@
         <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
@@ -2782,13 +2779,13 @@
         <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>33</v>
@@ -2821,13 +2818,13 @@
         <v>47</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="O4" s="49" t="s">
         <v>65</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="Q4" s="4"/>
     </row>
@@ -2836,13 +2833,13 @@
         <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>34</v>
@@ -2875,13 +2872,13 @@
         <v>47</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="O5" s="29" t="s">
         <v>65</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
@@ -3106,7 +3103,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>92</v>
@@ -3160,7 +3157,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>84</v>
@@ -3270,13 +3267,13 @@
         <v>63</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>22</v>
@@ -3309,13 +3306,13 @@
         <v>47</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
@@ -3324,13 +3321,13 @@
         <v>63</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>159</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>164</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>23</v>
@@ -3363,13 +3360,13 @@
         <v>47</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
@@ -3378,52 +3375,52 @@
         <v>63</v>
       </c>
       <c r="B15" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="E15" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>155</v>
-      </c>
       <c r="F15" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="69">
         <v>0.1</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="74">
-        <v>0.04</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
-        <v>1.6</v>
+        <v>1.05</v>
       </c>
       <c r="K15" s="74">
-        <v>2.8799999999999999E-2</v>
+        <v>1.52E-2</v>
       </c>
       <c r="L15" s="20">
         <f t="shared" si="2"/>
-        <v>2.88</v>
+        <v>1.9</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>157</v>
+        <v>243</v>
       </c>
       <c r="O15" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
@@ -3486,7 +3483,7 @@
         <v>63</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>106</v>
@@ -3498,21 +3495,21 @@
         <v>146</v>
       </c>
       <c r="F17" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G17" s="69">
         <v>0.16</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="74">
         <v>0.14199999999999999</v>
       </c>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
-        <v>5.68</v>
+        <v>7.1</v>
       </c>
       <c r="K17" s="74">
         <f>I17</f>
@@ -3520,7 +3517,7 @@
       </c>
       <c r="L17" s="20">
         <f t="shared" si="2"/>
-        <v>14.2</v>
+        <v>17.75</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>47</v>
@@ -3541,16 +3538,16 @@
         <v>63</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -3581,13 +3578,13 @@
         <v>47</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="O18" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
@@ -3596,16 +3593,16 @@
         <v>63</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
@@ -3635,13 +3632,13 @@
         <v>47</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="O19" s="32" t="s">
         <v>90</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
@@ -3650,16 +3647,16 @@
         <v>63</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>126</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -3690,13 +3687,13 @@
         <v>47</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
@@ -3765,10 +3762,10 @@
         <v>76</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -3798,16 +3795,16 @@
         <v>47</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="O22" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -3821,10 +3818,10 @@
         <v>76</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -3854,16 +3851,16 @@
         <v>47</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="O23" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -3877,10 +3874,10 @@
         <v>76</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -3910,16 +3907,16 @@
         <v>47</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="O24" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -3933,10 +3930,10 @@
         <v>76</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
@@ -3966,16 +3963,16 @@
         <v>47</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="O25" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -3989,10 +3986,10 @@
         <v>76</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -4022,16 +4019,16 @@
         <v>47</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="O26" s="29" t="s">
         <v>103</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -4039,12 +4036,12 @@
         <v>105</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="58"/>
       <c r="E27" s="57" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F27" s="59">
         <v>1</v>
@@ -4119,7 +4116,7 @@
         <v>63</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>106</v>
@@ -4374,51 +4371,53 @@
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="25" t="s">
+        <v>245</v>
+      </c>
       <c r="C34" s="25" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F34" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="69">
         <v>0.4</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I34" s="74">
         <v>0.31</v>
       </c>
       <c r="J34" s="20">
         <f t="shared" si="1"/>
-        <v>3.1</v>
+        <v>6.2</v>
       </c>
       <c r="K34" s="74">
         <v>0.26119999999999999</v>
       </c>
       <c r="L34" s="20">
         <f t="shared" si="2"/>
-        <v>6.5299999999999994</v>
+        <v>13.059999999999999</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="O34" s="29" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="P34" s="19" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="Q34" s="4"/>
     </row>
@@ -4480,25 +4479,25 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G37" s="24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H37" s="24">
         <f>SUM(H4:H36)</f>
-        <v>46.96</v>
+        <v>47.620000000000005</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="J37" s="24">
         <f t="shared" ref="J37:L37" si="6">SUM(J4:J36)</f>
-        <v>411.59</v>
+        <v>415.55999999999995</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L37" s="24">
         <f t="shared" si="6"/>
-        <v>925.42</v>
+        <v>934.51999999999987</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -4507,21 +4506,21 @@
       </c>
       <c r="H38" s="24">
         <f>H37</f>
-        <v>46.96</v>
+        <v>47.620000000000005</v>
       </c>
       <c r="I38" t="s">
         <v>1</v>
       </c>
       <c r="J38" s="35">
         <f>J37/10</f>
-        <v>41.158999999999999</v>
+        <v>41.555999999999997</v>
       </c>
       <c r="K38" t="s">
         <v>1</v>
       </c>
       <c r="L38" s="35">
         <f>L37/25</f>
-        <v>37.016799999999996</v>
+        <v>37.380799999999994</v>
       </c>
     </row>
   </sheetData>
@@ -4548,7 +4547,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4566,7 +4565,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -4578,31 +4577,24 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>240</v>
+      </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
       <c r="E5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>242</v>
-      </c>
       <c r="E6" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added gerbers and centroid files
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="257">
   <si>
     <t>Number</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>I2C Level Shifting</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
     <t>To Test</t>
   </si>
   <si>
-    <t>Solar panel Open Voltage - change reverse mosfet if necessary</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -430,9 +424,6 @@
     <t>1x3 TH Female Header</t>
   </si>
   <si>
-    <t>Li200 Resistor Values</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -589,18 +580,12 @@
     <t>http://www.digikey.com/product-detail/en/08055A102JAT2A/478-1328-1-ND/564360?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>Resistors on SD Card</t>
-  </si>
-  <si>
     <t>J14</t>
   </si>
   <si>
     <t>1x1 TH Female Header</t>
   </si>
   <si>
-    <t>Solar Panel Battery voltage for resistor divider</t>
-  </si>
-  <si>
     <t>On Shore Technology Inc.</t>
   </si>
   <si>
@@ -769,9 +754,6 @@
     <t>Q3, Q4, Q6, Q8, Q9</t>
   </si>
   <si>
-    <t>Fan Vcc Switcher?</t>
-  </si>
-  <si>
     <t>R23, R24</t>
   </si>
   <si>
@@ -787,10 +769,37 @@
     <t>http://www.digikey.com/product-detail/en/RC0805FR-0775KL/311-75.0KCRCT-ND/731080?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>LED Artwork?</t>
-  </si>
-  <si>
-    <t>Double Check LiCor Polarity</t>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW080556K0FKEA</t>
+  </si>
+  <si>
+    <t>56k 1% 1/8W Resistor</t>
+  </si>
+  <si>
+    <t>541-56.0KCCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CRCW080556K0FKEA/541-56.0KCCT-ND/1180982?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>RC0805FR-0716KL</t>
+  </si>
+  <si>
+    <t>311-16.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>16k 1% 1/8W Resistor</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0805FR-0716KL/311-16.0KCRCT-ND/730567?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1264,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1347,6 +1356,7 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1754,35 +1764,35 @@
       <c r="A1" s="47"/>
       <c r="B1" s="1"/>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="83"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="81" t="s">
+      <c r="G2" s="84"/>
+      <c r="H2" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="83"/>
-      <c r="J2" s="81" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="79" t="s">
+      <c r="K2" s="86"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="80" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1791,10 +1801,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
@@ -1818,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>10</v>
@@ -1826,7 +1836,7 @@
       <c r="M3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="80"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -1870,13 +1880,13 @@
         <v>21</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1905,23 +1915,23 @@
         <v>623.75</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="M5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="44" t="s">
         <v>38</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1950,23 +1960,23 @@
         <v>323.75</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="44" t="s">
         <v>42</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1993,23 +2003,23 @@
         <v>561.5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2037,19 +2047,19 @@
         <v>43.875</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2665,10 +2675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2693,117 +2703,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="52" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="81" t="s">
-        <v>161</v>
-      </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="J2" s="83"/>
-      <c r="K2" s="81" t="s">
-        <v>163</v>
-      </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="81" t="s">
+      <c r="G2" s="82" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="84"/>
+      <c r="K2" s="82" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="84"/>
+      <c r="M2" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="79" t="s">
+      <c r="N2" s="86"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="80" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="E3" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>10</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q3" s="80"/>
+        <v>96</v>
+      </c>
+      <c r="Q3" s="81"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="46">
         <v>13</v>
@@ -2812,52 +2822,52 @@
         <v>0.38</v>
       </c>
       <c r="H4" s="38">
-        <f t="shared" ref="H4:H36" si="0">F4*G4</f>
+        <f t="shared" ref="H4:H37" si="0">F4*G4</f>
         <v>4.9400000000000004</v>
       </c>
       <c r="I4" s="73">
         <v>0.36399999999999999</v>
       </c>
       <c r="J4" s="43">
-        <f t="shared" ref="J4:J36" si="1">F4*I4*10</f>
+        <f t="shared" ref="J4:J37" si="1">F4*I4*10</f>
         <v>47.32</v>
       </c>
       <c r="K4" s="73">
         <v>0.312</v>
       </c>
       <c r="L4" s="43">
-        <f t="shared" ref="L4:L36" si="2">F4*K4*25</f>
+        <f t="shared" ref="L4:L37" si="2">F4*K4*25</f>
         <v>101.4</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="O4" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -2884,34 +2894,34 @@
         <v>56.16</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -2941,31 +2951,31 @@
         <v>15</v>
       </c>
       <c r="N6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="P6" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="58" t="s">
+      <c r="E7" s="57" t="s">
         <v>78</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>79</v>
       </c>
       <c r="F7" s="59">
         <v>1</v>
@@ -2992,31 +3002,31 @@
         <v>2.81</v>
       </c>
       <c r="M7" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="P7" s="62" t="s">
         <v>81</v>
-      </c>
-      <c r="P7" s="62" t="s">
-        <v>82</v>
       </c>
       <c r="Q7" s="59"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>71</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>25</v>
@@ -3061,16 +3071,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>14</v>
@@ -3100,34 +3110,34 @@
         <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O9" s="32" t="s">
         <v>16</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="25" t="s">
         <v>93</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>94</v>
       </c>
       <c r="F10" s="4">
         <v>12</v>
@@ -3154,34 +3164,34 @@
         <v>4.5600000000000005</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O10" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="O10" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="P10" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>87</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>88</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -3209,31 +3219,31 @@
         <v>15.6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O11" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="P11" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>74</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>75</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>17</v>
@@ -3264,31 +3274,31 @@
         <v>13.625000000000002</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="O12" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>22</v>
@@ -3318,31 +3328,31 @@
         <v>3.62</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>23</v>
@@ -3372,34 +3382,34 @@
         <v>3.62</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
@@ -3426,34 +3436,34 @@
         <v>1.9</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -3480,34 +3490,34 @@
         <v>0.76</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F17" s="4">
         <v>5</v>
@@ -3535,34 +3545,34 @@
         <v>17.75</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O17" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -3590,34 +3600,34 @@
         <v>2.1999999999999997</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="O18" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>180</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
@@ -3644,34 +3654,34 @@
         <v>1.32</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O19" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -3699,31 +3709,31 @@
         <v>126.8</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="55" t="s">
         <v>114</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>116</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>24</v>
@@ -3756,31 +3766,31 @@
         <v>15</v>
       </c>
       <c r="N21" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="O21" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="P21" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="O21" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>119</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -3807,36 +3817,36 @@
         <v>14.92</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="O22" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -3863,36 +3873,36 @@
         <v>11.690000000000001</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -3919,36 +3929,36 @@
         <v>12.72</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
@@ -3975,36 +3985,36 @@
         <v>32.18</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="O25" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -4031,32 +4041,32 @@
         <v>16.189999999999998</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" s="57" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="58"/>
       <c r="E27" s="57" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F27" s="59">
         <v>1</v>
@@ -4079,24 +4089,24 @@
       <c r="M27" s="56"/>
       <c r="N27" s="57"/>
       <c r="O27" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P27" s="62"/>
       <c r="Q27" s="59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C28" s="57"/>
       <c r="D28" s="58"/>
       <c r="E28" s="57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F28" s="59">
         <v>1</v>
@@ -4119,28 +4129,28 @@
       <c r="M28" s="56"/>
       <c r="N28" s="57"/>
       <c r="O28" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P28" s="62"/>
       <c r="Q28" s="59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C29" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="E29" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>108</v>
       </c>
       <c r="F29" s="4">
         <v>5</v>
@@ -4168,34 +4178,34 @@
         <v>22.249999999999996</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O29" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="O29" s="29" t="s">
+      <c r="P29" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F30" s="4">
         <v>3</v>
@@ -4222,34 +4232,34 @@
         <v>2.67</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="E31" s="25" t="s">
         <v>125</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>127</v>
       </c>
       <c r="F31" s="4">
         <v>1</v>
@@ -4280,27 +4290,27 @@
         <v>15</v>
       </c>
       <c r="N31" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="P31" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="O31" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="P31" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" s="57" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="58"/>
       <c r="E32" s="57" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F32" s="59">
         <v>1</v>
@@ -4325,24 +4335,24 @@
       <c r="O32" s="58"/>
       <c r="P32" s="59"/>
       <c r="Q32" s="59" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F33" s="64">
         <v>1</v>
@@ -4372,31 +4382,31 @@
         <v>15</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O33" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P33" s="78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q33" s="64"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F34" s="4">
         <v>2</v>
@@ -4423,34 +4433,34 @@
         <v>13.059999999999999</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="O34" s="29" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="P34" s="19" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Q34" s="4"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F35" s="4">
         <v>2</v>
@@ -4477,91 +4487,171 @@
         <v>0.76</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N35" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="O35" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="P35" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="E36" s="25" t="s">
         <v>250</v>
       </c>
-      <c r="O35" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="P35" s="19" t="s">
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="26">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="74">
+        <v>0.04</v>
+      </c>
+      <c r="J36" s="20">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="K36" s="74">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="L36" s="20">
+        <f t="shared" si="2"/>
+        <v>0.72</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N36" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="Q35" s="4"/>
-    </row>
-    <row r="36" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="77"/>
-      <c r="J36" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G37" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="H37" s="24">
-        <f>SUM(H4:H36)</f>
-        <v>47.820000000000007</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="J37" s="24">
-        <f t="shared" ref="J37:L37" si="6">SUM(J4:J36)</f>
-        <v>415.97999999999996</v>
-      </c>
-      <c r="K37" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="L37" s="24">
+      <c r="O36" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="P36" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q36" s="4"/>
+    </row>
+    <row r="37" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="72">
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="15">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="77">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="J37" s="22">
+        <f t="shared" si="1"/>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="K37" s="77">
+        <v>1.52E-2</v>
+      </c>
+      <c r="L37" s="22">
+        <f t="shared" si="2"/>
+        <v>0.38</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="O37" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="P37" s="79" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q37" s="7"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G38" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="24">
+        <f>SUM(H4:H37)</f>
+        <v>48.02000000000001</v>
+      </c>
+      <c r="I38" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="J38" s="24">
+        <f t="shared" ref="J38:L38" si="6">SUM(J4:J37)</f>
+        <v>416.58999999999992</v>
+      </c>
+      <c r="K38" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="L38" s="24">
         <f t="shared" si="6"/>
-        <v>935.27999999999986</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G38" t="s">
+        <v>936.37999999999988</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
         <v>1</v>
       </c>
-      <c r="H38" s="24">
-        <f>H37</f>
-        <v>47.820000000000007</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="H39" s="24">
+        <f>H38</f>
+        <v>48.02000000000001</v>
+      </c>
+      <c r="I39" t="s">
         <v>1</v>
       </c>
-      <c r="J38" s="35">
-        <f>J37/10</f>
-        <v>41.597999999999999</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="J39" s="35">
+        <f>J38/10</f>
+        <v>41.658999999999992</v>
+      </c>
+      <c r="K39" t="s">
         <v>1</v>
       </c>
-      <c r="L38" s="35">
-        <f>L37/25</f>
-        <v>37.411199999999994</v>
+      <c r="L39" s="35">
+        <f>L38/25</f>
+        <v>37.455199999999998</v>
       </c>
     </row>
   </sheetData>
@@ -4578,6 +4668,7 @@
     <hyperlink ref="P33" r:id="rId1"/>
     <hyperlink ref="P34" r:id="rId2"/>
     <hyperlink ref="P35" r:id="rId3"/>
+    <hyperlink ref="P37" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4589,7 +4680,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4599,46 +4690,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>253</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Soldermask changes and started assembly quotes
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
-    <sheet name="To Add" sheetId="2" r:id="rId3"/>
+    <sheet name="Current Quotes" sheetId="4" r:id="rId3"/>
+    <sheet name="To Add" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="276">
   <si>
     <t>Number</t>
   </si>
@@ -800,20 +801,85 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/RC0805FR-0716KL/311-16.0KCRCT-ND/730567?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
+  </si>
+  <si>
+    <t>Total Placements:</t>
+  </si>
+  <si>
+    <t>Through Hole Placements:</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Screaming Circuits</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Cost Quoted</t>
+  </si>
+  <si>
+    <t>Total Turn Time</t>
+  </si>
+  <si>
+    <t>20 Day</t>
+  </si>
+  <si>
+    <t>10 Day Full Proto</t>
+  </si>
+  <si>
+    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student. Requires boards from OshPark!</t>
+  </si>
+  <si>
+    <t>Add approximately $148.8 for power supply, SD Card holder; 10% Discount for being a student. Requires panelization and boards from OshPark!</t>
+  </si>
+  <si>
+    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student. Requires panelization and boards from OshPark!</t>
+  </si>
+  <si>
+    <t>Osh Park</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>12 Calendar Days</t>
+  </si>
+  <si>
+    <t>Not Panelized! Cost will change with panelization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1242,29 +1308,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1286,7 +1353,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1294,7 +1361,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -1312,7 +1379,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
@@ -1323,7 +1390,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1339,7 +1406,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1355,8 +1422,14 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="17" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1381,8 +1454,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
+    <cellStyle name="Currency" xfId="20" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1769,30 +1845,30 @@
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="83"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="85" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="82" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="82" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="80" t="s">
+      <c r="K2" s="92"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="86" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1836,7 +1912,7 @@
       <c r="M3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="81"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2678,7 +2754,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2703,10 +2779,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="93"/>
       <c r="C1" s="52" t="s">
         <v>66</v>
       </c>
@@ -2718,33 +2794,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="88" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85" t="s">
+      <c r="H2" s="90"/>
+      <c r="I2" s="91" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="82" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="84"/>
-      <c r="M2" s="82" t="s">
+      <c r="L2" s="90"/>
+      <c r="M2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="86"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="80" t="s">
+      <c r="N2" s="92"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="86" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2797,7 +2873,7 @@
       <c r="P3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="81"/>
+      <c r="Q3" s="87"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -4609,6 +4685,13 @@
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E38" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F38">
+        <f>SUM(F4:F37)</f>
+        <v>80</v>
+      </c>
       <c r="G38" s="24" t="s">
         <v>174</v>
       </c>
@@ -4632,6 +4715,13 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E39" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="F39">
+        <f>SUM(F4:F6,F21,F22:F26)</f>
+        <v>25</v>
+      </c>
       <c r="G39" t="s">
         <v>1</v>
       </c>
@@ -4677,9 +4767,168 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="84" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="84" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>266</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="80">
+        <v>42607</v>
+      </c>
+      <c r="C3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3" s="84">
+        <v>1368.93</v>
+      </c>
+      <c r="G3" s="84">
+        <f>F3/E3</f>
+        <v>114.0775</v>
+      </c>
+      <c r="H3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="80">
+        <v>42607</v>
+      </c>
+      <c r="C4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" s="84">
+        <v>1902.4</v>
+      </c>
+      <c r="G4" s="84">
+        <f>F4/E4</f>
+        <v>95.12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="80">
+        <v>42607</v>
+      </c>
+      <c r="C5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5" s="84">
+        <v>1720.43</v>
+      </c>
+      <c r="G5" s="84">
+        <f>F5/E5</f>
+        <v>143.36916666666667</v>
+      </c>
+      <c r="H5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="80">
+        <v>42607</v>
+      </c>
+      <c r="C6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="95">
+        <v>49.25</v>
+      </c>
+      <c r="G6" s="84">
+        <f>F6/E6</f>
+        <v>16.416666666666668</v>
+      </c>
+      <c r="H6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added assembly quotes and panelized gerbers
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="284">
   <si>
     <t>Number</t>
   </si>
@@ -858,14 +858,37 @@
   </si>
   <si>
     <t>Not Panelized! Cost will change with panelization</t>
+  </si>
+  <si>
+    <t>4PCB</t>
+  </si>
+  <si>
+    <t>Assembly+Printing</t>
+  </si>
+  <si>
+    <t>Cost Quoted+Extra Parts/Quantities (See formula for details)</t>
+  </si>
+  <si>
+    <t>10 Day</t>
+  </si>
+  <si>
+    <t>Includes everything</t>
+  </si>
+  <si>
+    <t>26 Day</t>
+  </si>
+  <si>
+    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student</t>
+  </si>
+  <si>
+    <t>Quote is for 3 panels containing 4 pcbs each</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
@@ -1331,7 +1354,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1430,6 +1453,9 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1454,8 +1480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Currency" xfId="20" builtinId="4"/>
@@ -1845,30 +1869,30 @@
       <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="92"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="91" t="s">
+      <c r="E2" s="93"/>
+      <c r="F2" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="88" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="88" t="s">
+      <c r="I2" s="93"/>
+      <c r="J2" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="86" t="s">
+      <c r="K2" s="95"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="89" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1912,7 +1936,7 @@
       <c r="M3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="87"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2779,10 +2803,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="93"/>
+      <c r="B1" s="96"/>
       <c r="C1" s="52" t="s">
         <v>66</v>
       </c>
@@ -2794,33 +2818,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="91" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="91" t="s">
+      <c r="H2" s="93"/>
+      <c r="I2" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="88" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="91" t="s">
         <v>160</v>
       </c>
-      <c r="L2" s="90"/>
-      <c r="M2" s="88" t="s">
+      <c r="L2" s="93"/>
+      <c r="M2" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="92"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="86" t="s">
+      <c r="N2" s="95"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="89" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2873,7 +2897,7 @@
       <c r="P3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="87"/>
+      <c r="Q3" s="90"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -4767,29 +4791,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="84" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="84" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="87" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.83203125" style="84" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="84" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="118.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="86" t="s">
         <v>260</v>
       </c>
       <c r="C2" s="81" t="s">
@@ -4801,17 +4826,20 @@
       <c r="E2" s="81" t="s">
         <v>262</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="88" t="s">
         <v>265</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="83" t="s">
+        <v>278</v>
+      </c>
+      <c r="H2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="82" t="s">
+      <c r="I2" s="82" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>263</v>
       </c>
@@ -4827,18 +4855,22 @@
       <c r="E3">
         <v>12</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="87">
         <v>1368.93</v>
       </c>
-      <c r="G3" s="84">
-        <f>F3/E3</f>
-        <v>114.0775</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G3" s="87">
+        <f>F3+89.28+G7</f>
+        <v>1700.71</v>
+      </c>
+      <c r="H3" s="84">
+        <f>G3/E3</f>
+        <v>141.72583333333333</v>
+      </c>
+      <c r="I3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>263</v>
       </c>
@@ -4854,18 +4886,22 @@
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4" s="84">
+      <c r="F4" s="87">
         <v>1902.4</v>
       </c>
-      <c r="G4" s="84">
-        <f>F4/E4</f>
-        <v>95.12</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="87">
+        <f>F4+148.8+G7*2</f>
+        <v>2536.2000000000003</v>
+      </c>
+      <c r="H4" s="84">
+        <f t="shared" ref="H4:H5" si="0">G4/E4</f>
+        <v>126.81000000000002</v>
+      </c>
+      <c r="I4" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -4881,42 +4917,202 @@
       <c r="E5">
         <v>12</v>
       </c>
-      <c r="F5" s="84">
+      <c r="F5" s="87">
         <v>1720.43</v>
       </c>
-      <c r="G5" s="84">
-        <f>F5/E5</f>
-        <v>143.36916666666667</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="87">
+        <f>F5+89.28+F8*4</f>
+        <v>2006.71</v>
+      </c>
+      <c r="H5" s="84">
+        <f t="shared" si="0"/>
+        <v>167.22583333333333</v>
+      </c>
+      <c r="I5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="80">
+        <v>42611</v>
+      </c>
+      <c r="C6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6" s="87">
+        <v>2331.33</v>
+      </c>
+      <c r="G6" s="87">
+        <f>F6+90.28</f>
+        <v>2421.61</v>
+      </c>
+      <c r="H6" s="84">
+        <f>G6/E6</f>
+        <v>201.80083333333334</v>
+      </c>
+      <c r="I6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>272</v>
       </c>
-      <c r="B6" s="80">
+      <c r="B7" s="80">
+        <v>42612</v>
+      </c>
+      <c r="C7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7" s="87">
+        <v>242.5</v>
+      </c>
+      <c r="G7" s="87">
+        <f>F7</f>
+        <v>242.5</v>
+      </c>
+      <c r="H7" s="84">
+        <f>G7/E7</f>
+        <v>20.208333333333332</v>
+      </c>
+      <c r="I7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="80">
         <v>42607</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>273</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>274</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="F6" s="95">
+      <c r="F8" s="87">
         <v>49.25</v>
       </c>
-      <c r="G6" s="84">
-        <f>F6/E6</f>
+      <c r="G8" s="87"/>
+      <c r="H8" s="84">
+        <f>F8/E8</f>
         <v>16.416666666666668</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I8" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="80">
+        <v>42611</v>
+      </c>
+      <c r="C9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" s="87">
+        <v>2528.4899999999998</v>
+      </c>
+      <c r="G9" s="87">
+        <f>F9</f>
+        <v>2528.4899999999998</v>
+      </c>
+      <c r="H9" s="84">
+        <f>G9/E9</f>
+        <v>252.84899999999999</v>
+      </c>
+      <c r="I9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="80">
+        <v>42611</v>
+      </c>
+      <c r="C10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10" s="87">
+        <v>3372.79</v>
+      </c>
+      <c r="G10" s="87">
+        <f t="shared" ref="G10:G11" si="1">F10</f>
+        <v>3372.79</v>
+      </c>
+      <c r="H10" s="84">
+        <f t="shared" ref="H10:H11" si="2">G10/E10</f>
+        <v>168.6395</v>
+      </c>
+      <c r="I10" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" s="80">
+        <v>42611</v>
+      </c>
+      <c r="C11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11" s="87">
+        <v>3826.44</v>
+      </c>
+      <c r="G11" s="87">
+        <f t="shared" si="1"/>
+        <v>3826.44</v>
+      </c>
+      <c r="H11" s="84">
+        <f t="shared" si="2"/>
+        <v>153.05760000000001</v>
+      </c>
+      <c r="I11" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM, design finalized for assembly
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
     <sheet name="Current Quotes" sheetId="4" r:id="rId3"/>
-    <sheet name="To Add" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="294">
   <si>
     <t>Number</t>
   </si>
@@ -92,12 +91,6 @@
     <t>CR1220 Battery</t>
   </si>
   <si>
-    <t>614-CR1220</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/Search/ProductDetail.aspx?qs=sGAEpiMZZMtz8P%2feuiupSd2F%2fX%2ffEmeEyLDGD5JMOeY%3d</t>
-  </si>
-  <si>
     <t>Green LED</t>
   </si>
   <si>
@@ -137,9 +130,6 @@
     <t>Possible different source? Check footprint carefully if so</t>
   </si>
   <si>
-    <t>To Add Rough List</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -365,9 +355,6 @@
     <t>http://www.digikey.com/product-detail/en/BSS138/BSS138CT-ND/244294?curr=usd&amp;WT.z_cid=ref_octopart_dkc_buynow&amp;site=us</t>
   </si>
   <si>
-    <t>To Test</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -882,6 +869,48 @@
   </si>
   <si>
     <t>Quote is for 3 panels containing 4 pcbs each</t>
+  </si>
+  <si>
+    <t>P033-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/panasonic-bsg/CR1220/P033-ND/269740</t>
+  </si>
+  <si>
+    <t>Printed Circuit Board (PCB)</t>
+  </si>
+  <si>
+    <t>Actual (Paid) Cost</t>
+  </si>
+  <si>
+    <t>Quantity:</t>
+  </si>
+  <si>
+    <t>Shipping costs and taxes not included!</t>
+  </si>
+  <si>
+    <t>3.38"x2.90" standard. 7.46"x6.51" panelized. 4x/panel. Osh Park prices $5/in^2 for 3. Actual cost has super swift service added. Medium run not considered</t>
+  </si>
+  <si>
+    <t>PCB Assembly</t>
+  </si>
+  <si>
+    <t>http://www.oshpark.com</t>
+  </si>
+  <si>
+    <t>http://www.screamingcircuits.com</t>
+  </si>
+  <si>
+    <t>Ideal costs are hard to calculate without quote. Student discount included</t>
+  </si>
+  <si>
+    <t>PCB Turnkey Parts</t>
+  </si>
+  <si>
+    <t>Ideal costs are hard to calculate without quote. See Shield Parts sheet for part breakdown without "Turnkey Tax"</t>
+  </si>
+  <si>
+    <t>12V Battery</t>
   </si>
 </sst>
 </file>
@@ -949,7 +978,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1326,6 +1355,19 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1354,7 +1396,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1402,7 +1444,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
@@ -1414,7 +1455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1480,6 +1520,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Currency" xfId="20" builtinId="4"/>
@@ -1836,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1848,69 +1898,81 @@
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="156.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="156.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="127.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46"/>
       <c r="B1" s="1"/>
       <c r="D1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="30"/>
-    </row>
-    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+        <v>285</v>
+      </c>
+      <c r="J1" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="92"/>
+      <c r="B2" s="90"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="E2" s="91"/>
+      <c r="F2" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="93"/>
-      <c r="H2" s="91" t="s">
+      <c r="G2" s="91"/>
+      <c r="H2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="93"/>
-      <c r="J2" s="91" t="s">
+      <c r="I2" s="91"/>
+      <c r="J2" s="97" t="s">
+        <v>283</v>
+      </c>
+      <c r="K2" s="98"/>
+      <c r="L2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="92"/>
       <c r="M2" s="93"/>
-      <c r="N2" s="89" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="90"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>30</v>
+      <c r="B3" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>1</v>
@@ -1924,69 +1986,84 @@
       <c r="I3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="31" t="s">
+      <c r="M3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="90"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" s="88"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="45">
         <v>1</v>
       </c>
       <c r="D4" s="37">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="E4" s="38">
         <f t="shared" ref="E4:E30" si="0">C4*D4</f>
-        <v>0.82</v>
-      </c>
-      <c r="F4" s="42">
-        <v>0.78</v>
-      </c>
-      <c r="G4" s="43">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="41">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="G4" s="42">
         <f t="shared" ref="G4:G30" si="1">C4*F4*10</f>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0.75</v>
-      </c>
-      <c r="I4" s="43">
+        <v>8.120000000000001</v>
+      </c>
+      <c r="H4" s="41">
+        <f>F4</f>
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="I4" s="42">
         <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
-        <v>18.75</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="29" t="s">
+        <v>20.3</v>
+      </c>
+      <c r="J4" s="95">
+        <f>F4</f>
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="K4" s="95">
+        <f>J4*$K$1</f>
+        <v>9.7439999999999998</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -2014,24 +2091,32 @@
         <f t="shared" si="2"/>
         <v>623.75</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="29" t="s">
+      <c r="J5" s="95">
+        <f>F5</f>
+        <v>24.95</v>
+      </c>
+      <c r="K5" s="95">
+        <f t="shared" ref="K5:K30" si="3">J5*$K$1</f>
+        <v>299.39999999999998</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -2059,24 +2144,32 @@
         <f t="shared" si="2"/>
         <v>323.75</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="32" t="s">
+      <c r="J6" s="95">
+        <f>F6</f>
+        <v>12.95</v>
+      </c>
+      <c r="K6" s="95">
+        <f t="shared" si="3"/>
+        <v>155.39999999999998</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -2102,24 +2195,32 @@
         <f t="shared" si="2"/>
         <v>561.5</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" s="32" t="s">
+      <c r="J7" s="95">
+        <f>F7</f>
+        <v>23.7</v>
+      </c>
+      <c r="K7" s="95">
+        <f t="shared" si="3"/>
+        <v>284.39999999999998</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="N7" s="44"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="P7" s="43"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -2146,101 +2247,188 @@
         <f t="shared" si="2"/>
         <v>43.875</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="L8" s="32" t="s">
+      <c r="J8" s="95">
+        <f>F8</f>
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="K8" s="95">
+        <f t="shared" si="3"/>
+        <v>21.06</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="N8" s="44" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="P8" s="43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="39">
+        <f>9.802*5/3</f>
+        <v>16.336666666666666</v>
+      </c>
       <c r="E9" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="21"/>
+        <v>16.336666666666666</v>
+      </c>
+      <c r="F9" s="21">
+        <f>D9</f>
+        <v>16.336666666666666</v>
+      </c>
       <c r="G9" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="21"/>
+        <v>163.36666666666667</v>
+      </c>
+      <c r="H9" s="21">
+        <f>D9</f>
+        <v>16.336666666666666</v>
+      </c>
       <c r="I9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="44"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>408.41666666666663</v>
+      </c>
+      <c r="J9" s="95">
+        <f>331.5/12</f>
+        <v>27.625</v>
+      </c>
+      <c r="K9" s="95">
+        <f t="shared" si="3"/>
+        <v>331.5</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="P9" s="43" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="26">
+      <c r="B10" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="99"/>
+      <c r="E10" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="20">
+      <c r="F10" s="100"/>
+      <c r="G10" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="20">
+      <c r="H10" s="100"/>
+      <c r="I10" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="44"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J10" s="95">
+        <f>(943.1-94.31)/12</f>
+        <v>70.732500000000002</v>
+      </c>
+      <c r="K10" s="95">
+        <f t="shared" si="3"/>
+        <v>848.79</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="P10" s="43" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="26">
+      <c r="B11" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="99"/>
+      <c r="E11" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="20">
+      <c r="F11" s="100"/>
+      <c r="G11" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="20">
+      <c r="H11" s="100"/>
+      <c r="I11" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="44"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J11" s="95">
+        <f>703.13/12</f>
+        <v>58.594166666666666</v>
+      </c>
+      <c r="K11" s="95">
+        <f t="shared" si="3"/>
+        <v>703.13</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="P11" s="43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
       <c r="D12" s="39"/>
       <c r="E12" s="26">
         <f t="shared" si="0"/>
@@ -2256,13 +2444,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="44"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J12" s="95"/>
+      <c r="K12" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="43"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25"/>
       <c r="C13" s="4"/>
@@ -2281,13 +2474,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="44"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J13" s="95"/>
+      <c r="K13" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25"/>
       <c r="C14" s="4"/>
@@ -2306,13 +2504,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="44"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J14" s="95"/>
+      <c r="K14" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25"/>
       <c r="C15" s="4"/>
@@ -2331,13 +2534,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="44"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J15" s="95"/>
+      <c r="K15" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="43"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25"/>
       <c r="C16" s="4"/>
@@ -2356,13 +2564,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="44"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J16" s="95"/>
+      <c r="K16" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
       <c r="C17" s="4"/>
@@ -2381,13 +2594,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="44"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J17" s="95"/>
+      <c r="K17" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="4"/>
@@ -2406,13 +2624,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="44"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J18" s="95"/>
+      <c r="K18" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="43"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="25"/>
       <c r="C19" s="4"/>
@@ -2431,13 +2654,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="44"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J19" s="95"/>
+      <c r="K19" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="4"/>
@@ -2456,13 +2684,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="44"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J20" s="95"/>
+      <c r="K20" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="4"/>
@@ -2481,13 +2714,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="44"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J21" s="95"/>
+      <c r="K21" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25"/>
       <c r="C22" s="4"/>
@@ -2506,13 +2744,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="44"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J22" s="95"/>
+      <c r="K22" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="43"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25"/>
       <c r="C23" s="4"/>
@@ -2531,13 +2774,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="44"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J23" s="95"/>
+      <c r="K23" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="43"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25"/>
       <c r="C24" s="4"/>
@@ -2556,13 +2804,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="44"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J24" s="95"/>
+      <c r="K24" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="43"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25"/>
       <c r="C25" s="4"/>
@@ -2581,13 +2834,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="2"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="44"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J25" s="95"/>
+      <c r="K25" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="43"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -2606,13 +2864,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="2"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="44"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J26" s="95"/>
+      <c r="K26" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="43"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
@@ -2631,13 +2894,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="44"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J27" s="95"/>
+      <c r="K27" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="43"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
@@ -2656,13 +2924,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="44"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J28" s="95"/>
+      <c r="K28" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="43"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
@@ -2681,13 +2954,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="44"/>
-    </row>
-    <row r="30" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="95"/>
+      <c r="K29" s="95">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="43"/>
+    </row>
+    <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -2706,70 +2984,96 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="45"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J30" s="96"/>
+      <c r="K30" s="96">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="44"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>65.62</v>
+        <v>82.036666666666662</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
-        <f t="shared" ref="G31:I31" si="3">SUM(G4:G30)</f>
-        <v>641.34999999999991</v>
+        <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
+        <v>805.03666666666663</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
-        <f t="shared" si="3"/>
-        <v>1571.625</v>
-      </c>
-      <c r="L31" s="30"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1981.5916666666667</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="24">
+        <f>SUM(K4:K30)</f>
+        <v>2653.424</v>
+      </c>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>65.62</v>
+        <v>82.036666666666662</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>64.134999999999991</v>
+        <v>80.50366666666666</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>62.865000000000002</v>
-      </c>
-      <c r="L32" s="30"/>
+        <v>79.263666666666666</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="35">
+        <f>K31/K1</f>
+        <v>221.11866666666666</v>
+      </c>
+      <c r="N32" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="N2:N3"/>
+  <mergeCells count="7">
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O9" r:id="rId1"/>
+    <hyperlink ref="O10" r:id="rId2"/>
+    <hyperlink ref="O11" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2778,7 +3082,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2786,7 +3090,7 @@
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="54" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="52" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -2803,190 +3107,190 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="52" t="s">
-        <v>66</v>
+      <c r="A1" s="94" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="50" t="s">
+        <v>63</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="91" t="s">
-        <v>158</v>
-      </c>
-      <c r="H2" s="93"/>
-      <c r="I2" s="94" t="s">
-        <v>159</v>
-      </c>
-      <c r="J2" s="93"/>
-      <c r="K2" s="91" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="93"/>
-      <c r="M2" s="91" t="s">
+      <c r="G2" s="89" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="91"/>
+      <c r="K2" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="L2" s="91"/>
+      <c r="M2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="95"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="89" t="s">
-        <v>29</v>
+      <c r="N2" s="93"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="87" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>10</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q3" s="90"/>
+        <v>93</v>
+      </c>
+      <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>182</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="46">
+        <v>30</v>
+      </c>
+      <c r="F4" s="45">
         <v>13</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="66">
         <v>0.38</v>
       </c>
       <c r="H4" s="38">
         <f t="shared" ref="H4:H37" si="0">F4*G4</f>
         <v>4.9400000000000004</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="71">
         <v>0.36399999999999999</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f t="shared" ref="J4:J37" si="1">F4*I4*10</f>
         <v>47.32</v>
       </c>
-      <c r="K4" s="73">
+      <c r="K4" s="71">
         <v>0.312</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="42">
         <f t="shared" ref="L4:L37" si="2">F4*K4*25</f>
         <v>101.4</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="O4" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="50" t="s">
-        <v>190</v>
+        <v>183</v>
+      </c>
+      <c r="O4" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="49" t="s">
+        <v>186</v>
       </c>
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="69">
+      <c r="G5" s="67">
         <v>0.67</v>
       </c>
       <c r="H5" s="26">
         <f t="shared" si="0"/>
         <v>2.68</v>
       </c>
-      <c r="I5" s="74">
+      <c r="I5" s="72">
         <v>0.624</v>
       </c>
       <c r="J5" s="20">
         <f t="shared" si="1"/>
         <v>24.96</v>
       </c>
-      <c r="K5" s="74">
+      <c r="K5" s="72">
         <v>0.56159999999999999</v>
       </c>
       <c r="L5" s="20">
@@ -2994,53 +3298,53 @@
         <v>56.16</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="69">
+      <c r="G6" s="67">
         <v>6.2</v>
       </c>
       <c r="H6" s="26">
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
-      <c r="I6" s="74">
+      <c r="I6" s="72">
         <v>5.7</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="K6" s="74">
+      <c r="K6" s="72">
         <v>5.43</v>
       </c>
       <c r="L6" s="20">
@@ -3051,104 +3355,104 @@
         <v>15</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="59">
+      <c r="A7" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="57">
         <v>1</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="68">
         <v>0.22</v>
       </c>
-      <c r="H7" s="60">
+      <c r="H7" s="58">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="I7" s="75">
+      <c r="I7" s="73">
         <v>0.153</v>
       </c>
-      <c r="J7" s="61">
+      <c r="J7" s="59">
         <f t="shared" si="1"/>
         <v>1.53</v>
       </c>
-      <c r="K7" s="75">
+      <c r="K7" s="73">
         <v>0.1124</v>
       </c>
-      <c r="L7" s="61">
+      <c r="L7" s="59">
         <f t="shared" si="2"/>
         <v>2.81</v>
       </c>
-      <c r="M7" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="P7" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" s="59"/>
+      <c r="M7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="57"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="67">
         <v>1.74</v>
       </c>
       <c r="H8" s="26">
         <f t="shared" ref="H8:H13" si="3">F8*G8</f>
         <v>1.74</v>
       </c>
-      <c r="I8" s="74">
+      <c r="I8" s="72">
         <v>1.74</v>
       </c>
       <c r="J8" s="20">
         <f t="shared" ref="J8:J13" si="4">F8*I8*10</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="72">
         <v>1.49</v>
       </c>
       <c r="L8" s="20">
@@ -3156,31 +3460,31 @@
         <v>37.25</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>14</v>
@@ -3188,21 +3492,21 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="69">
+      <c r="G9" s="67">
         <v>9.9700000000000006</v>
       </c>
       <c r="H9" s="26">
         <f t="shared" si="3"/>
         <v>9.9700000000000006</v>
       </c>
-      <c r="I9" s="74">
+      <c r="I9" s="72">
         <v>9.41</v>
       </c>
       <c r="J9" s="20">
         <f t="shared" si="4"/>
         <v>94.1</v>
       </c>
-      <c r="K9" s="74">
+      <c r="K9" s="72">
         <v>7.5275999999999996</v>
       </c>
       <c r="L9" s="20">
@@ -3210,53 +3514,53 @@
         <v>188.19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O9" s="32" t="s">
         <v>16</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" s="4">
         <v>12</v>
       </c>
-      <c r="G10" s="69">
+      <c r="G10" s="67">
         <v>0.1</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="72">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J10" s="20">
         <f t="shared" si="4"/>
         <v>2.52</v>
       </c>
-      <c r="K10" s="74">
+      <c r="K10" s="72">
         <v>1.52E-2</v>
       </c>
       <c r="L10" s="20">
@@ -3264,53 +3568,53 @@
         <v>4.5600000000000005</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C11" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>86</v>
-      </c>
       <c r="E11" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11" s="69">
+      <c r="G11" s="67">
         <v>0.25</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="I11" s="74">
+      <c r="I11" s="72">
         <v>0.20799999999999999</v>
       </c>
       <c r="J11" s="20">
         <f t="shared" si="4"/>
         <v>6.24</v>
       </c>
-      <c r="K11" s="74">
+      <c r="K11" s="72">
         <f>I11</f>
         <v>0.20799999999999999</v>
       </c>
@@ -3319,31 +3623,31 @@
         <v>15.6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>17</v>
@@ -3351,21 +3655,21 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="69">
+      <c r="G12" s="67">
         <v>0.57999999999999996</v>
       </c>
       <c r="H12" s="26">
         <f t="shared" si="3"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="I12" s="74">
+      <c r="I12" s="72">
         <v>0.54500000000000004</v>
       </c>
       <c r="J12" s="20">
         <f t="shared" si="4"/>
         <v>5.45</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="72">
         <f>I12</f>
         <v>0.54500000000000004</v>
       </c>
@@ -3374,53 +3678,53 @@
         <v>13.625000000000002</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O12" s="32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="69">
+      <c r="G13" s="67">
         <v>0.27</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" si="3"/>
         <v>0.27</v>
       </c>
-      <c r="I13" s="74">
+      <c r="I13" s="72">
         <v>0.19600000000000001</v>
       </c>
       <c r="J13" s="20">
         <f t="shared" si="4"/>
         <v>1.96</v>
       </c>
-      <c r="K13" s="74">
+      <c r="K13" s="72">
         <v>0.14480000000000001</v>
       </c>
       <c r="L13" s="20">
@@ -3428,53 +3732,53 @@
         <v>3.62</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="69">
+      <c r="G14" s="67">
         <v>0.27</v>
       </c>
       <c r="H14" s="26">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="72">
         <v>0.19600000000000001</v>
       </c>
       <c r="J14" s="20">
         <f t="shared" si="1"/>
         <v>1.96</v>
       </c>
-      <c r="K14" s="74">
+      <c r="K14" s="72">
         <v>0.14480000000000001</v>
       </c>
       <c r="L14" s="20">
@@ -3482,53 +3786,53 @@
         <v>3.62</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O14" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14" s="19" t="s">
         <v>153</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>157</v>
       </c>
       <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F15" s="4">
         <v>5</v>
       </c>
-      <c r="G15" s="69">
+      <c r="G15" s="67">
         <v>0.1</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="72">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
-      <c r="K15" s="74">
+      <c r="K15" s="72">
         <v>1.52E-2</v>
       </c>
       <c r="L15" s="20">
@@ -3536,53 +3840,53 @@
         <v>1.9</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
       </c>
-      <c r="G16" s="69">
+      <c r="G16" s="67">
         <v>0.1</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="72">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J16" s="20">
         <f t="shared" si="1"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="K16" s="74">
+      <c r="K16" s="72">
         <v>1.52E-2</v>
       </c>
       <c r="L16" s="20">
@@ -3590,53 +3894,53 @@
         <v>0.76</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F17" s="4">
         <v>5</v>
       </c>
-      <c r="G17" s="69">
+      <c r="G17" s="67">
         <v>0.16</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="I17" s="74">
+      <c r="I17" s="72">
         <v>0.14199999999999999</v>
       </c>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
         <v>7.1</v>
       </c>
-      <c r="K17" s="74">
+      <c r="K17" s="72">
         <f>I17</f>
         <v>0.14199999999999999</v>
       </c>
@@ -3645,53 +3949,53 @@
         <v>17.75</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="O17" s="32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="69">
+      <c r="G18" s="67">
         <v>0.11</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="72">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="J18" s="20">
         <f t="shared" si="1"/>
         <v>0.87999999999999989</v>
       </c>
-      <c r="K18" s="74">
+      <c r="K18" s="72">
         <f>I18</f>
         <v>8.7999999999999995E-2</v>
       </c>
@@ -3700,53 +4004,53 @@
         <v>2.1999999999999997</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="O18" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="G19" s="69">
+      <c r="G19" s="67">
         <v>0.1</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I19" s="74">
+      <c r="I19" s="72">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="J19" s="20">
         <f t="shared" si="1"/>
         <v>0.73</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="72">
         <v>5.28E-2</v>
       </c>
       <c r="L19" s="20">
@@ -3754,53 +4058,53 @@
         <v>1.32</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="O19" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="Q19" s="4"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="69">
+      <c r="G20" s="67">
         <v>5.65</v>
       </c>
       <c r="H20" s="26">
         <f t="shared" si="0"/>
         <v>5.65</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="72">
         <v>5.0720000000000001</v>
       </c>
       <c r="J20" s="20">
         <f t="shared" si="1"/>
         <v>50.72</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="72">
         <f>I20</f>
         <v>5.0720000000000001</v>
       </c>
@@ -3809,53 +4113,53 @@
         <v>126.8</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>110</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="69">
+      <c r="G21" s="67">
         <v>0.56000000000000005</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="72">
         <v>0.54200000000000004</v>
       </c>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
         <v>5.42</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="72">
         <v>0.53100000000000003</v>
       </c>
       <c r="L21" s="20">
@@ -3866,50 +4170,50 @@
         <v>15</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O21" s="29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="69">
+      <c r="G22" s="67">
         <v>0.82</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="72">
         <v>0.64</v>
       </c>
       <c r="J22" s="20">
         <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
-      <c r="K22" s="74">
+      <c r="K22" s="72">
         <v>0.5968</v>
       </c>
       <c r="L22" s="20">
@@ -3917,55 +4221,55 @@
         <v>14.92</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="O22" s="29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="69">
+      <c r="G23" s="67">
         <v>0.65</v>
       </c>
       <c r="H23" s="26">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="I23" s="74">
+      <c r="I23" s="72">
         <v>0.502</v>
       </c>
       <c r="J23" s="20">
         <f t="shared" si="1"/>
         <v>5.0199999999999996</v>
       </c>
-      <c r="K23" s="74">
+      <c r="K23" s="72">
         <v>0.46760000000000002</v>
       </c>
       <c r="L23" s="20">
@@ -3973,55 +4277,55 @@
         <v>11.690000000000001</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="O23" s="29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="69">
+      <c r="G24" s="67">
         <v>0.7</v>
       </c>
       <c r="H24" s="26">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="I24" s="74">
+      <c r="I24" s="72">
         <v>0.54600000000000004</v>
       </c>
       <c r="J24" s="20">
         <f t="shared" si="1"/>
         <v>5.4600000000000009</v>
       </c>
-      <c r="K24" s="74">
+      <c r="K24" s="72">
         <v>0.50880000000000003</v>
       </c>
       <c r="L24" s="20">
@@ -4029,55 +4333,55 @@
         <v>12.72</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="69">
+      <c r="G25" s="67">
         <v>0.89</v>
       </c>
       <c r="H25" s="26">
         <f t="shared" si="0"/>
         <v>1.78</v>
       </c>
-      <c r="I25" s="74">
+      <c r="I25" s="72">
         <v>0.69</v>
       </c>
       <c r="J25" s="20">
         <f t="shared" si="1"/>
         <v>13.799999999999999</v>
       </c>
-      <c r="K25" s="74">
+      <c r="K25" s="72">
         <v>0.64359999999999995</v>
       </c>
       <c r="L25" s="20">
@@ -4085,55 +4389,55 @@
         <v>32.18</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O25" s="29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
       </c>
-      <c r="G26" s="69">
+      <c r="G26" s="67">
         <v>0.84</v>
       </c>
       <c r="H26" s="26">
         <f t="shared" si="0"/>
         <v>0.84</v>
       </c>
-      <c r="I26" s="74">
+      <c r="I26" s="72">
         <v>0.69899999999999995</v>
       </c>
       <c r="J26" s="20">
         <f t="shared" si="1"/>
         <v>6.9899999999999993</v>
       </c>
-      <c r="K26" s="74">
+      <c r="K26" s="72">
         <v>0.64759999999999995</v>
       </c>
       <c r="L26" s="20">
@@ -4141,135 +4445,135 @@
         <v>16.189999999999998</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="57" t="s">
-        <v>184</v>
-      </c>
-      <c r="F27" s="59">
+      <c r="A27" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="55" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" s="57">
         <v>1</v>
       </c>
-      <c r="G27" s="70"/>
-      <c r="H27" s="60">
+      <c r="G27" s="68"/>
+      <c r="H27" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="75"/>
-      <c r="J27" s="61">
+      <c r="I27" s="73"/>
+      <c r="J27" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K27" s="75"/>
-      <c r="L27" s="61">
+      <c r="K27" s="73"/>
+      <c r="L27" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M27" s="56"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="59" t="s">
-        <v>103</v>
+      <c r="M27" s="54"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="57" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="59">
+      <c r="A28" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="57">
         <v>1</v>
       </c>
-      <c r="G28" s="70"/>
-      <c r="H28" s="60">
+      <c r="G28" s="68"/>
+      <c r="H28" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="75"/>
-      <c r="J28" s="61">
+      <c r="I28" s="73"/>
+      <c r="J28" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="75"/>
-      <c r="L28" s="61">
+      <c r="K28" s="73"/>
+      <c r="L28" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M28" s="56"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="59" t="s">
-        <v>103</v>
+      <c r="M28" s="54"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="57" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F29" s="4">
         <v>5</v>
       </c>
-      <c r="G29" s="69">
+      <c r="G29" s="67">
         <v>0.22</v>
       </c>
       <c r="H29" s="26">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I29" s="74">
+      <c r="I29" s="72">
         <v>0.17799999999999999</v>
       </c>
       <c r="J29" s="20">
         <f t="shared" si="1"/>
         <v>8.8999999999999986</v>
       </c>
-      <c r="K29" s="74">
+      <c r="K29" s="72">
         <f>I29</f>
         <v>0.17799999999999999</v>
       </c>
@@ -4278,53 +4582,53 @@
         <v>22.249999999999996</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O29" s="29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F30" s="4">
         <v>3</v>
       </c>
-      <c r="G30" s="69">
+      <c r="G30" s="67">
         <v>0.1</v>
       </c>
       <c r="H30" s="26">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="I30" s="74">
+      <c r="I30" s="72">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="J30" s="20">
         <f t="shared" si="1"/>
         <v>1.53</v>
       </c>
-      <c r="K30" s="74">
+      <c r="K30" s="72">
         <v>3.56E-2</v>
       </c>
       <c r="L30" s="20">
@@ -4332,53 +4636,53 @@
         <v>2.67</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P30" s="19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F31" s="4">
         <v>1</v>
       </c>
-      <c r="G31" s="69">
+      <c r="G31" s="67">
         <v>1.61</v>
       </c>
       <c r="H31" s="26">
         <f t="shared" si="0"/>
         <v>1.61</v>
       </c>
-      <c r="I31" s="74">
+      <c r="I31" s="72">
         <v>1.37</v>
       </c>
       <c r="J31" s="20">
         <f t="shared" si="1"/>
         <v>13.700000000000001</v>
       </c>
-      <c r="K31" s="74">
+      <c r="K31" s="72">
         <f>I31</f>
         <v>1.37</v>
       </c>
@@ -4390,142 +4694,142 @@
         <v>15</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O31" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="P31" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="P31" s="19" t="s">
+      <c r="C32" s="55"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="Q31" s="4"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="57" t="s">
+      <c r="F32" s="57">
+        <v>1</v>
+      </c>
+      <c r="G32" s="68"/>
+      <c r="H32" s="58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="73"/>
+      <c r="J32" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="73"/>
+      <c r="L32" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="54"/>
+      <c r="N32" s="55"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="57" t="s">
+      <c r="D33" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="F32" s="59">
+      <c r="F33" s="62">
         <v>1</v>
       </c>
-      <c r="G32" s="70"/>
-      <c r="H32" s="60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="75"/>
-      <c r="J32" s="61">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K32" s="75"/>
-      <c r="L32" s="61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="56"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="64">
-        <v>1</v>
-      </c>
-      <c r="G33" s="71">
+      <c r="G33" s="69">
         <v>2.2799999999999998</v>
       </c>
-      <c r="H33" s="65">
+      <c r="H33" s="63">
         <f t="shared" si="0"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="I33" s="76">
+      <c r="I33" s="74">
         <v>2.08</v>
       </c>
-      <c r="J33" s="66">
+      <c r="J33" s="64">
         <f t="shared" si="1"/>
         <v>20.8</v>
       </c>
-      <c r="K33" s="76">
+      <c r="K33" s="74">
         <v>1.92</v>
       </c>
-      <c r="L33" s="66">
+      <c r="L33" s="64">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="M33" s="63" t="s">
+      <c r="M33" s="61" t="s">
         <v>15</v>
       </c>
       <c r="N33" s="25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O33" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="P33" s="78" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q33" s="64"/>
+        <v>134</v>
+      </c>
+      <c r="P33" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q33" s="62"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F34" s="4">
         <v>2</v>
       </c>
-      <c r="G34" s="69">
+      <c r="G34" s="67">
         <v>0.4</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="I34" s="74">
+      <c r="I34" s="72">
         <v>0.31</v>
       </c>
       <c r="J34" s="20">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
-      <c r="K34" s="74">
+      <c r="K34" s="72">
         <v>0.26119999999999999</v>
       </c>
       <c r="L34" s="20">
@@ -4533,53 +4837,53 @@
         <v>13.059999999999999</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="O34" s="29" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="P34" s="19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="Q34" s="4"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F35" s="4">
         <v>2</v>
       </c>
-      <c r="G35" s="69">
+      <c r="G35" s="67">
         <v>0.1</v>
       </c>
       <c r="H35" s="26">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I35" s="74">
+      <c r="I35" s="72">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J35" s="20">
         <f t="shared" si="1"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="K35" s="74">
+      <c r="K35" s="72">
         <v>1.52E-2</v>
       </c>
       <c r="L35" s="20">
@@ -4587,53 +4891,53 @@
         <v>0.76</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="O35" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P35" s="19" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="Q35" s="4"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B36" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="25" t="s">
         <v>246</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>250</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
       </c>
-      <c r="G36" s="69">
+      <c r="G36" s="67">
         <v>0.1</v>
       </c>
       <c r="H36" s="26">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I36" s="74">
+      <c r="I36" s="72">
         <v>0.04</v>
       </c>
       <c r="J36" s="20">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="K36" s="74">
+      <c r="K36" s="72">
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="L36" s="20">
@@ -4641,53 +4945,53 @@
         <v>0.72</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="O36" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P36" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="Q36" s="4"/>
     </row>
     <row r="37" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
-      <c r="G37" s="72">
+      <c r="G37" s="70">
         <v>0.1</v>
       </c>
       <c r="H37" s="15">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I37" s="77">
+      <c r="I37" s="75">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J37" s="22">
         <f t="shared" si="1"/>
         <v>0.21000000000000002</v>
       </c>
-      <c r="K37" s="77">
+      <c r="K37" s="75">
         <v>1.52E-2</v>
       </c>
       <c r="L37" s="22">
@@ -4695,52 +4999,52 @@
         <v>0.38</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="O37" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="P37" s="79" t="s">
-        <v>256</v>
+        <v>86</v>
+      </c>
+      <c r="P37" s="77" t="s">
+        <v>252</v>
       </c>
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E38" s="25" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F38">
         <f>SUM(F4:F37)</f>
         <v>80</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H38" s="24">
         <f>SUM(H4:H37)</f>
         <v>48.02000000000001</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J38" s="24">
-        <f t="shared" ref="J38:L38" si="6">SUM(J4:J37)</f>
+        <f>SUM(J4:J37)</f>
         <v>416.58999999999992</v>
       </c>
       <c r="K38" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L38" s="24">
-        <f t="shared" si="6"/>
+        <f>SUM(L4:L37)</f>
         <v>936.37999999999988</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E39" s="25" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F39">
         <f>SUM(F4:F6,F21,F22:F26)</f>
@@ -4793,356 +5097,327 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="78" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="87" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.83203125" style="84" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="84" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="85" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.83203125" style="82" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="82" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="118.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2" s="86" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" s="81" t="s">
+      <c r="A2" s="79" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="84" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" s="86" t="s">
         <v>261</v>
       </c>
-      <c r="D2" s="81" t="s">
-        <v>266</v>
-      </c>
-      <c r="E2" s="81" t="s">
-        <v>262</v>
-      </c>
-      <c r="F2" s="88" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="83" t="s">
-        <v>278</v>
-      </c>
-      <c r="H2" s="85" t="s">
+      <c r="G2" s="81" t="s">
+        <v>274</v>
+      </c>
+      <c r="H2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="82" t="s">
-        <v>29</v>
+      <c r="I2" s="80" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="78">
+        <v>42607</v>
+      </c>
+      <c r="C3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" t="s">
         <v>263</v>
-      </c>
-      <c r="B3" s="80">
-        <v>42607</v>
-      </c>
-      <c r="C3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D3" t="s">
-        <v>267</v>
       </c>
       <c r="E3">
         <v>12</v>
       </c>
-      <c r="F3" s="87">
+      <c r="F3" s="85">
         <v>1368.93</v>
       </c>
-      <c r="G3" s="87">
+      <c r="G3" s="85">
         <f>F3+89.28+G7</f>
         <v>1700.71</v>
       </c>
-      <c r="H3" s="84">
+      <c r="H3" s="82">
         <f>G3/E3</f>
         <v>141.72583333333333</v>
       </c>
       <c r="I3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" s="78">
+        <v>42607</v>
+      </c>
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" t="s">
         <v>263</v>
-      </c>
-      <c r="B4" s="80">
-        <v>42607</v>
-      </c>
-      <c r="C4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" t="s">
-        <v>267</v>
       </c>
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4" s="87">
+      <c r="F4" s="85">
         <v>1902.4</v>
       </c>
-      <c r="G4" s="87">
+      <c r="G4" s="85">
         <f>F4+148.8+G7*2</f>
         <v>2536.2000000000003</v>
       </c>
-      <c r="H4" s="84">
+      <c r="H4" s="82">
         <f t="shared" ref="H4:H5" si="0">G4/E4</f>
         <v>126.81000000000002</v>
       </c>
       <c r="I4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B5" s="80">
+        <v>259</v>
+      </c>
+      <c r="B5" s="78">
         <v>42607</v>
       </c>
       <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" t="s">
         <v>264</v>
-      </c>
-      <c r="D5" t="s">
-        <v>268</v>
       </c>
       <c r="E5">
         <v>12</v>
       </c>
-      <c r="F5" s="87">
+      <c r="F5" s="85">
         <v>1720.43</v>
       </c>
-      <c r="G5" s="87">
+      <c r="G5" s="85">
         <f>F5+89.28+F8*4</f>
         <v>2006.71</v>
       </c>
-      <c r="H5" s="84">
+      <c r="H5" s="82">
         <f t="shared" si="0"/>
         <v>167.22583333333333</v>
       </c>
       <c r="I5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B6" s="80">
+        <v>259</v>
+      </c>
+      <c r="B6" s="78">
         <v>42611</v>
       </c>
       <c r="C6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" t="s">
         <v>277</v>
-      </c>
-      <c r="D6" t="s">
-        <v>281</v>
       </c>
       <c r="E6">
         <v>12</v>
       </c>
-      <c r="F6" s="87">
+      <c r="F6" s="85">
         <v>2331.33</v>
       </c>
-      <c r="G6" s="87">
+      <c r="G6" s="85">
         <f>F6+90.28</f>
         <v>2421.61</v>
       </c>
-      <c r="H6" s="84">
+      <c r="H6" s="82">
         <f>G6/E6</f>
         <v>201.80083333333334</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" s="80">
+        <v>268</v>
+      </c>
+      <c r="B7" s="78">
         <v>42612</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
-      <c r="F7" s="87">
+      <c r="F7" s="85">
         <v>242.5</v>
       </c>
-      <c r="G7" s="87">
+      <c r="G7" s="85">
         <f>F7</f>
         <v>242.5</v>
       </c>
-      <c r="H7" s="84">
+      <c r="H7" s="82">
         <f>G7/E7</f>
         <v>20.208333333333332</v>
       </c>
       <c r="I7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="80">
+        <v>268</v>
+      </c>
+      <c r="B8" s="78">
         <v>42607</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="85">
         <v>49.25</v>
       </c>
-      <c r="G8" s="87"/>
-      <c r="H8" s="84">
+      <c r="G8" s="85"/>
+      <c r="H8" s="82">
         <f>F8/E8</f>
         <v>16.416666666666668</v>
       </c>
       <c r="I8" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" s="80">
+        <v>272</v>
+      </c>
+      <c r="B9" s="78">
         <v>42611</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
-      <c r="F9" s="87">
+      <c r="F9" s="85">
         <v>2528.4899999999998</v>
       </c>
-      <c r="G9" s="87">
+      <c r="G9" s="85">
         <f>F9</f>
         <v>2528.4899999999998</v>
       </c>
-      <c r="H9" s="84">
+      <c r="H9" s="82">
         <f>G9/E9</f>
         <v>252.84899999999999</v>
       </c>
       <c r="I9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>276</v>
-      </c>
-      <c r="B10" s="80">
+        <v>272</v>
+      </c>
+      <c r="B10" s="78">
         <v>42611</v>
       </c>
       <c r="C10" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D10" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E10">
         <v>20</v>
       </c>
-      <c r="F10" s="87">
+      <c r="F10" s="85">
         <v>3372.79</v>
       </c>
-      <c r="G10" s="87">
+      <c r="G10" s="85">
         <f t="shared" ref="G10:G11" si="1">F10</f>
         <v>3372.79</v>
       </c>
-      <c r="H10" s="84">
+      <c r="H10" s="82">
         <f t="shared" ref="H10:H11" si="2">G10/E10</f>
         <v>168.6395</v>
       </c>
       <c r="I10" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B11" s="80">
+        <v>272</v>
+      </c>
+      <c r="B11" s="78">
         <v>42611</v>
       </c>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E11">
         <v>25</v>
       </c>
-      <c r="F11" s="87">
+      <c r="F11" s="85">
         <v>3826.44</v>
       </c>
-      <c r="G11" s="87">
+      <c r="G11" s="85">
         <f t="shared" si="1"/>
         <v>3826.44</v>
       </c>
-      <c r="H11" s="84">
+      <c r="H11" s="82">
         <f t="shared" si="2"/>
         <v>153.05760000000001</v>
       </c>
       <c r="I11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51"/>
+        <v>276</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
File reorganization, README update, Time_Set added
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="304">
   <si>
     <t>Number</t>
   </si>
@@ -911,13 +911,44 @@
   </si>
   <si>
     <t>12V Battery</t>
+  </si>
+  <si>
+    <t>Seahorse SE-120 Waterproof Case</t>
+  </si>
+  <si>
+    <t>Fuerte Cases</t>
+  </si>
+  <si>
+    <t>SE-120</t>
+  </si>
+  <si>
+    <t>http://seahorsecases.com/Merchant2/merchant.mvc?Screen=PROD&amp;Store_Code=S&amp;Product_Code=SE-120&amp;Category_Code=SE_CASES</t>
+  </si>
+  <si>
+    <t>Available from other sources</t>
+  </si>
+  <si>
+    <t>Radiation Shield</t>
+  </si>
+  <si>
+    <t>Ambient Weather</t>
+  </si>
+  <si>
+    <t>SRS100LX</t>
+  </si>
+  <si>
+    <t>http://www.ambientweather.com/amwesrpatean.html</t>
+  </si>
+  <si>
+    <t>Sometimes available from other sources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
@@ -1396,7 +1427,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1496,6 +1527,10 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1517,19 +1552,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Currency" xfId="20" builtinId="4"/>
@@ -1889,13 +1921,13 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -1927,34 +1959,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="90"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="97" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="89" t="s">
+      <c r="K2" s="99"/>
+      <c r="L2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="87" t="s">
+      <c r="M2" s="97"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2004,7 +2036,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="88"/>
+      <c r="P3" s="92"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2036,11 +2068,11 @@
         <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
         <v>20.3</v>
       </c>
-      <c r="J4" s="95">
+      <c r="J4" s="87">
         <f>F4</f>
         <v>0.81200000000000006</v>
       </c>
-      <c r="K4" s="95">
+      <c r="K4" s="87">
         <f>J4*$K$1</f>
         <v>9.7439999999999998</v>
       </c>
@@ -2091,11 +2123,11 @@
         <f t="shared" si="2"/>
         <v>623.75</v>
       </c>
-      <c r="J5" s="95">
+      <c r="J5" s="87">
         <f>F5</f>
         <v>24.95</v>
       </c>
-      <c r="K5" s="95">
+      <c r="K5" s="87">
         <f t="shared" ref="K5:K30" si="3">J5*$K$1</f>
         <v>299.39999999999998</v>
       </c>
@@ -2144,11 +2176,11 @@
         <f t="shared" si="2"/>
         <v>323.75</v>
       </c>
-      <c r="J6" s="95">
+      <c r="J6" s="87">
         <f>F6</f>
         <v>12.95</v>
       </c>
-      <c r="K6" s="95">
+      <c r="K6" s="87">
         <f t="shared" si="3"/>
         <v>155.39999999999998</v>
       </c>
@@ -2195,11 +2227,11 @@
         <f t="shared" si="2"/>
         <v>561.5</v>
       </c>
-      <c r="J7" s="95">
+      <c r="J7" s="87">
         <f>F7</f>
         <v>23.7</v>
       </c>
-      <c r="K7" s="95">
+      <c r="K7" s="87">
         <f t="shared" si="3"/>
         <v>284.39999999999998</v>
       </c>
@@ -2247,11 +2279,11 @@
         <f t="shared" si="2"/>
         <v>43.875</v>
       </c>
-      <c r="J8" s="95">
+      <c r="J8" s="87">
         <f>F8</f>
         <v>1.7549999999999999</v>
       </c>
-      <c r="K8" s="95">
+      <c r="K8" s="87">
         <f t="shared" si="3"/>
         <v>21.06</v>
       </c>
@@ -2303,11 +2335,11 @@
         <f t="shared" si="2"/>
         <v>408.41666666666663</v>
       </c>
-      <c r="J9" s="95">
+      <c r="J9" s="87">
         <f>331.5/12</f>
         <v>27.625</v>
       </c>
-      <c r="K9" s="95">
+      <c r="K9" s="87">
         <f t="shared" si="3"/>
         <v>331.5</v>
       </c>
@@ -2335,26 +2367,26 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="99"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="100"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="100"/>
+      <c r="H10" s="90"/>
       <c r="I10" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J10" s="95">
+      <c r="J10" s="87">
         <f>(943.1-94.31)/12</f>
         <v>70.732500000000002</v>
       </c>
-      <c r="K10" s="95">
+      <c r="K10" s="87">
         <f t="shared" si="3"/>
         <v>848.79</v>
       </c>
@@ -2382,26 +2414,26 @@
       <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="99"/>
+      <c r="D11" s="89"/>
       <c r="E11" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="100"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="100"/>
+      <c r="H11" s="90"/>
       <c r="I11" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="95">
+      <c r="J11" s="87">
         <f>703.13/12</f>
         <v>58.594166666666666</v>
       </c>
-      <c r="K11" s="95">
+      <c r="K11" s="87">
         <f t="shared" si="3"/>
         <v>703.13</v>
       </c>
@@ -2444,8 +2476,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="95"/>
-      <c r="K12" s="95">
+      <c r="J12" s="87"/>
+      <c r="K12" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2457,63 +2489,111 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="39"/>
+      <c r="B13" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="39">
+        <v>11.83</v>
+      </c>
       <c r="E13" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="21"/>
+        <v>11.83</v>
+      </c>
+      <c r="F13" s="21">
+        <f>D13</f>
+        <v>11.83</v>
+      </c>
       <c r="G13" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="21"/>
+        <v>118.3</v>
+      </c>
+      <c r="H13" s="21">
+        <f>D13</f>
+        <v>11.83</v>
+      </c>
       <c r="I13" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95">
+        <v>295.75</v>
+      </c>
+      <c r="J13" s="87">
+        <v>11.83</v>
+      </c>
+      <c r="K13" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="43"/>
+        <v>141.96</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="N13" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="39"/>
+      <c r="B14" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="39">
+        <v>39.99</v>
+      </c>
       <c r="E14" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="21"/>
+        <v>39.99</v>
+      </c>
+      <c r="F14" s="21">
+        <f>D14</f>
+        <v>39.99</v>
+      </c>
       <c r="G14" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="21"/>
+        <v>399.90000000000003</v>
+      </c>
+      <c r="H14" s="21">
+        <f>D14</f>
+        <v>39.99</v>
+      </c>
       <c r="I14" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="95"/>
-      <c r="K14" s="95">
+        <v>999.75</v>
+      </c>
+      <c r="J14" s="101">
+        <v>39.99</v>
+      </c>
+      <c r="K14" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="43"/>
+        <v>479.88</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="P14" s="43" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
@@ -2534,8 +2614,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95">
+      <c r="J15" s="87"/>
+      <c r="K15" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2564,8 +2644,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="95"/>
-      <c r="K16" s="95">
+      <c r="J16" s="87"/>
+      <c r="K16" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2594,8 +2674,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95">
+      <c r="J17" s="87"/>
+      <c r="K17" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2624,8 +2704,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J18" s="95"/>
-      <c r="K18" s="95">
+      <c r="J18" s="87"/>
+      <c r="K18" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2654,8 +2734,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95">
+      <c r="J19" s="87"/>
+      <c r="K19" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2684,8 +2764,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="95"/>
-      <c r="K20" s="95">
+      <c r="J20" s="87"/>
+      <c r="K20" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2714,8 +2794,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95">
+      <c r="J21" s="87"/>
+      <c r="K21" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2744,8 +2824,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="95"/>
-      <c r="K22" s="95">
+      <c r="J22" s="87"/>
+      <c r="K22" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2774,8 +2854,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="95"/>
-      <c r="K23" s="95">
+      <c r="J23" s="87"/>
+      <c r="K23" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2804,8 +2884,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95">
+      <c r="J24" s="87"/>
+      <c r="K24" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2834,8 +2914,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95">
+      <c r="J25" s="87"/>
+      <c r="K25" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2864,8 +2944,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J26" s="95"/>
-      <c r="K26" s="95">
+      <c r="J26" s="87"/>
+      <c r="K26" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2894,8 +2974,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95">
+      <c r="J27" s="87"/>
+      <c r="K27" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2924,8 +3004,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="95"/>
-      <c r="K28" s="95">
+      <c r="J28" s="87"/>
+      <c r="K28" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2954,8 +3034,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95">
+      <c r="J29" s="87"/>
+      <c r="K29" s="87">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2984,8 +3064,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="96"/>
-      <c r="K30" s="96">
+      <c r="J30" s="88"/>
+      <c r="K30" s="88">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3001,28 +3081,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>82.036666666666662</v>
+        <v>133.85666666666665</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>805.03666666666663</v>
+        <v>1323.2366666666667</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>1981.5916666666667</v>
+        <v>3277.0916666666667</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>2653.424</v>
+        <v>3275.2640000000001</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3032,28 +3112,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>82.036666666666662</v>
+        <v>133.85666666666665</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>80.50366666666666</v>
+        <v>132.32366666666667</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>79.263666666666666</v>
+        <v>131.08366666666666</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>221.11866666666666</v>
+        <v>272.93866666666668</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -3107,10 +3187,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="94"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="50" t="s">
         <v>63</v>
       </c>
@@ -3122,33 +3202,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92" t="s">
+      <c r="H2" s="95"/>
+      <c r="I2" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="J2" s="91"/>
-      <c r="K2" s="89" t="s">
+      <c r="J2" s="95"/>
+      <c r="K2" s="93" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="91"/>
-      <c r="M2" s="89" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="93"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="87" t="s">
+      <c r="N2" s="97"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3201,7 +3281,7 @@
       <c r="P3" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="Q3" s="88"/>
+      <c r="Q3" s="92"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">

</xml_diff>

<commit_message>
Added calibration constants workbook
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
-    <sheet name="Current Quotes" sheetId="4" r:id="rId3"/>
+    <sheet name="LiCor Leveling Base" sheetId="5" r:id="rId3"/>
+    <sheet name="Current Quotes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="327">
   <si>
     <t>Number</t>
   </si>
@@ -967,19 +968,49 @@
     <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-13106-2. More expensive on Noco website</t>
   </si>
   <si>
-    <t>Bubble Level</t>
-  </si>
-  <si>
-    <t>McMaster</t>
-  </si>
-  <si>
-    <t>2147A61</t>
-  </si>
-  <si>
-    <t>http://www.mcmaster.com/#catalog/122/2302/=14e0x9g</t>
-  </si>
-  <si>
-    <t>Search for part number to be precise</t>
+    <t>Davis Anemometer</t>
+  </si>
+  <si>
+    <t>Hodges Marine</t>
+  </si>
+  <si>
+    <t>DAV6410</t>
+  </si>
+  <si>
+    <t>http://www.hodgesmarine.com/Davis-Anemometer-F-Vantage-Pro2-153-Vantage-p/dav6410.htm</t>
+  </si>
+  <si>
+    <t>Red cells indicate values calculated from quotes</t>
+  </si>
+  <si>
+    <t>LiCor Li200 Pyranometer</t>
+  </si>
+  <si>
+    <t>LiCor</t>
+  </si>
+  <si>
+    <t>Li-200R</t>
+  </si>
+  <si>
+    <t>https://www.licor.com</t>
+  </si>
+  <si>
+    <t>Can order online or with quote. Unsure whether online gets you quantity discount</t>
+  </si>
+  <si>
+    <t>Decagon 5TM Soil Sensor</t>
+  </si>
+  <si>
+    <t>Decagon</t>
+  </si>
+  <si>
+    <t>5TM</t>
+  </si>
+  <si>
+    <t>https://www.decagon.com/en/</t>
+  </si>
+  <si>
+    <t>Need quote to order</t>
   </si>
 </sst>
 </file>
@@ -1466,7 +1497,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1571,6 +1602,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1601,6 +1635,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Currency" xfId="20" builtinId="4"/>
@@ -1959,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,6 +2025,9 @@
       <c r="D1" s="3" t="s">
         <v>283</v>
       </c>
+      <c r="F1" t="s">
+        <v>316</v>
+      </c>
       <c r="J1" t="s">
         <v>282</v>
       </c>
@@ -1998,34 +2037,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="96"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="94" t="s">
+      <c r="D2" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="97" t="s">
+      <c r="E2" s="97"/>
+      <c r="F2" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="96"/>
-      <c r="H2" s="94" t="s">
+      <c r="G2" s="97"/>
+      <c r="H2" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="96"/>
-      <c r="J2" s="99" t="s">
+      <c r="I2" s="97"/>
+      <c r="J2" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="K2" s="100"/>
-      <c r="L2" s="94" t="s">
+      <c r="K2" s="101"/>
+      <c r="L2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="98"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="92" t="s">
+      <c r="M2" s="99"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="93" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2075,7 +2114,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="93"/>
+      <c r="P3" s="94"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2410,20 +2449,29 @@
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="89"/>
+      <c r="D10" s="89">
+        <f>J10*1</f>
+        <v>70.732500000000002</v>
+      </c>
       <c r="E10" s="58">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="90"/>
+        <v>70.732500000000002</v>
+      </c>
+      <c r="F10" s="90">
+        <f>J10</f>
+        <v>70.732500000000002</v>
+      </c>
       <c r="G10" s="59">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="90"/>
+        <v>707.32500000000005</v>
+      </c>
+      <c r="H10" s="90">
+        <f>J10</f>
+        <v>70.732500000000002</v>
+      </c>
       <c r="I10" s="59">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1768.3125</v>
       </c>
       <c r="J10" s="87">
         <f>(943.1-94.31)/12</f>
@@ -2457,20 +2505,29 @@
       <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="89"/>
+      <c r="D11" s="89">
+        <f>J11</f>
+        <v>58.594166666666666</v>
+      </c>
       <c r="E11" s="58">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="90"/>
+        <v>58.594166666666666</v>
+      </c>
+      <c r="F11" s="90">
+        <f>J11</f>
+        <v>58.594166666666666</v>
+      </c>
       <c r="G11" s="59">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="90"/>
+        <v>585.94166666666661</v>
+      </c>
+      <c r="H11" s="90">
+        <f>J11</f>
+        <v>58.594166666666666</v>
+      </c>
       <c r="I11" s="59">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1464.8541666666667</v>
       </c>
       <c r="J11" s="87">
         <f>703.13/12</f>
@@ -2615,7 +2672,7 @@
         <f t="shared" si="2"/>
         <v>999.75</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J14" s="87">
         <v>39.99</v>
       </c>
       <c r="K14" s="87">
@@ -2747,117 +2804,160 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="C17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="39">
-        <v>3.14</v>
+        <v>186</v>
       </c>
       <c r="E17" s="26">
         <f t="shared" si="0"/>
-        <v>3.14</v>
+        <v>372</v>
       </c>
       <c r="F17" s="21">
-        <f>D17</f>
-        <v>3.14</v>
+        <v>167</v>
       </c>
       <c r="G17" s="20">
         <f t="shared" si="1"/>
-        <v>31.400000000000002</v>
+        <v>3340</v>
       </c>
       <c r="H17" s="21">
-        <f>D17</f>
-        <v>3.14</v>
+        <v>167</v>
       </c>
       <c r="I17" s="20">
         <f t="shared" si="2"/>
-        <v>78.5</v>
+        <v>8350</v>
       </c>
       <c r="J17" s="87">
-        <f>D17</f>
-        <v>3.14</v>
+        <f>H17*C17</f>
+        <v>334</v>
       </c>
       <c r="K17" s="87">
         <f t="shared" si="3"/>
-        <v>37.68</v>
+        <v>4008</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="N17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O17" s="19" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="P17" s="43" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
+      <c r="B18" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="39">
+        <v>106.99</v>
+      </c>
       <c r="E18" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="21"/>
+        <v>106.99</v>
+      </c>
+      <c r="F18" s="21">
+        <f>D18</f>
+        <v>106.99</v>
+      </c>
       <c r="G18" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="21"/>
+        <v>1069.8999999999999</v>
+      </c>
+      <c r="H18" s="21">
+        <f>D18</f>
+        <v>106.99</v>
+      </c>
       <c r="I18" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="87"/>
+        <v>2674.75</v>
+      </c>
+      <c r="J18" s="87">
+        <f>D18</f>
+        <v>106.99</v>
+      </c>
       <c r="K18" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="19"/>
+        <v>1283.8799999999999</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="M18" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="N18" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>315</v>
+      </c>
       <c r="P18" s="43"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
+      <c r="B19" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="39">
+        <v>270</v>
+      </c>
       <c r="E19" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="21"/>
+        <v>270</v>
+      </c>
+      <c r="F19" s="21">
+        <v>259.2</v>
+      </c>
       <c r="G19" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="21"/>
+        <v>2592</v>
+      </c>
+      <c r="H19" s="21">
+        <v>259.2</v>
+      </c>
       <c r="I19" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="87"/>
+        <v>6480</v>
+      </c>
+      <c r="J19" s="87">
+        <v>259.2</v>
+      </c>
       <c r="K19" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="43"/>
+        <v>3110.3999999999996</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="M19" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="N19" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="P19" s="43" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
@@ -3195,28 +3295,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>165.89666666666662</v>
+        <v>1041.0733333333333</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>1614.8366666666666</v>
+        <v>9878.6033333333326</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>4006.0916666666667</v>
+        <v>24665.508333333331</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>3625.1839999999997</v>
+        <v>11989.784</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3226,28 +3326,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>165.89666666666662</v>
+        <v>1041.0733333333333</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>161.48366666666666</v>
+        <v>987.8603333333333</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>160.24366666666666</v>
+        <v>986.62033333333329</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>302.09866666666665</v>
+        <v>999.1486666666666</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -3301,10 +3401,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="102"/>
       <c r="C1" s="50" t="s">
         <v>61</v>
       </c>
@@ -3316,33 +3416,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="95" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97" t="s">
+      <c r="H2" s="97"/>
+      <c r="I2" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="96"/>
-      <c r="K2" s="94" t="s">
+      <c r="J2" s="97"/>
+      <c r="K2" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="96"/>
-      <c r="M2" s="94" t="s">
+      <c r="L2" s="97"/>
+      <c r="M2" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="92" t="s">
+      <c r="N2" s="99"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="93" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3395,7 +3495,7 @@
       <c r="P3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="93"/>
+      <c r="Q3" s="94"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -5289,6 +5389,1014 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="156.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="127.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46"/>
+      <c r="B1" s="1"/>
+      <c r="D1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" t="s">
+        <v>282</v>
+      </c>
+      <c r="K1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="96"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="97"/>
+      <c r="F2" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="97"/>
+      <c r="H2" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="97"/>
+      <c r="J2" s="100" t="s">
+        <v>281</v>
+      </c>
+      <c r="K2" s="101"/>
+      <c r="L2" s="95" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="99"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="94"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="26">
+        <f t="shared" ref="E4:E17" si="0">C4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="20">
+        <f t="shared" ref="G4:G17" si="1">C4*F4*10</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="41"/>
+      <c r="I4" s="20">
+        <f t="shared" ref="I4:I17" si="2">C4*H4*25</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87">
+        <f t="shared" ref="K4:K17" si="3">J4*$K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="43"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="43"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="43"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="43"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="43"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="104"/>
+      <c r="G10" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="104"/>
+      <c r="I10" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="43"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="104"/>
+      <c r="G11" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="104"/>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="43"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="43"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="91"/>
+      <c r="K14" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="43"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="26">
+        <f t="shared" ref="E18:E30" si="4">C18*D18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20">
+        <f t="shared" ref="G18:G30" si="5">C18*F18*10</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20">
+        <f t="shared" ref="I18:I30" si="6">C18*H18*25</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87">
+        <f t="shared" ref="K18:K30" si="7">J18*$K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="43"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="87"/>
+      <c r="K21" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="43"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="43"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="87"/>
+      <c r="K24" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="43"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="87"/>
+      <c r="K25" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="43"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="21"/>
+      <c r="I26" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="43"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="43"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="43"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="43"/>
+    </row>
+    <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="44"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="24">
+        <f>SUM(E4:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="24">
+        <f>SUM(G4:G30)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="24">
+        <f>SUM(I4:I30)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="24">
+        <f>SUM(K4:K30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="24">
+        <f>E31</f>
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="35">
+        <f>G31/10</f>
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="35">
+        <f>I31/25</f>
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="35">
+        <f>K31/K1</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Small BOM and documentation changes
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="375">
   <si>
     <t>Number</t>
   </si>
@@ -1016,9 +1016,6 @@
     <t>Wide Range 1/8" Blind Rivet</t>
   </si>
   <si>
-    <t>McMaser</t>
-  </si>
-  <si>
     <t>97530A030</t>
   </si>
   <si>
@@ -1146,6 +1143,18 @@
   </si>
   <si>
     <t>Comes in lengths of 5'. Other lengths available</t>
+  </si>
+  <si>
+    <t>1/4" Washer</t>
+  </si>
+  <si>
+    <t>90108A413</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#90108a413/=14xie31</t>
+  </si>
+  <si>
+    <t>Goes around silicon washer to add thickness for rivet to clamp onto</t>
   </si>
 </sst>
 </file>
@@ -2130,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3135,25 +3144,25 @@
         <v>2.9483999999999999</v>
       </c>
       <c r="L20" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M20" s="29" t="s">
         <v>328</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>329</v>
       </c>
       <c r="N20" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O20" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="P20" s="43" t="s">
         <v>330</v>
-      </c>
-      <c r="P20" s="43" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -3190,25 +3199,25 @@
         <v>3.8049999960000003</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="M21" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="N21" s="29" t="s">
         <v>333</v>
       </c>
-      <c r="N21" s="29" t="s">
+      <c r="O21" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="O21" s="19" t="s">
+      <c r="P21" s="43" t="s">
         <v>335</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -3246,28 +3255,28 @@
         <v>13.152000000000001</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="P22" s="43" t="s">
         <v>339</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C23" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="39">
         <f>7.36/50</f>
@@ -3275,7 +3284,7 @@
       </c>
       <c r="E23" s="26">
         <f t="shared" si="0"/>
-        <v>0.44159999999999999</v>
+        <v>0.2944</v>
       </c>
       <c r="F23" s="21">
         <f>D23</f>
@@ -3283,7 +3292,7 @@
       </c>
       <c r="G23" s="20">
         <f t="shared" si="1"/>
-        <v>4.4160000000000004</v>
+        <v>2.944</v>
       </c>
       <c r="H23" s="21">
         <f>D23</f>
@@ -3291,36 +3300,36 @@
       </c>
       <c r="I23" s="20">
         <f t="shared" si="2"/>
-        <v>11.04</v>
+        <v>7.3599999999999994</v>
       </c>
       <c r="J23" s="87">
         <f>E23</f>
-        <v>0.44159999999999999</v>
+        <v>0.2944</v>
       </c>
       <c r="K23" s="87">
         <f t="shared" si="3"/>
-        <v>5.2991999999999999</v>
+        <v>3.5327999999999999</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N23" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O23" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="P23" s="43" t="s">
         <v>343</v>
-      </c>
-      <c r="P23" s="43" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -3358,50 +3367,76 @@
         <v>119.044400004</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="P24" s="43" t="s">
         <v>366</v>
-      </c>
-      <c r="M24" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="N24" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="O24" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="P24" s="43" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
+      <c r="B25" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+      <c r="D25" s="39">
+        <f>3.3/100</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="E25" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="21"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F25" s="21">
+        <f>D25</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="G25" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="21"/>
+        <v>0.66</v>
+      </c>
+      <c r="H25" s="21">
+        <f>D25</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="I25" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="87"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="J25" s="87">
+        <f>D25</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="K25" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="43"/>
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="P25" s="43" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
@@ -3559,28 +3594,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>1053.0940833333334</v>
+        <v>1053.0128833333333</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>9998.8108333333312</v>
+        <v>9997.9988333333313</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>24966.027083333338</v>
+        <v>24963.997083333339</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>12134.032999999999</v>
+        <v>12132.662600000001</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3590,28 +3625,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>1053.0940833333334</v>
+        <v>1053.0128833333333</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>999.88108333333309</v>
+        <v>999.79988333333313</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>998.64108333333354</v>
+        <v>998.55988333333357</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>1011.1694166666666</v>
+        <v>1011.0552166666668</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -5776,7 +5811,7 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C4" s="45">
         <v>3</v>
@@ -5814,25 +5849,25 @@
         <v>8.0063999999999993</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>345</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>346</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -5870,25 +5905,25 @@
         <v>3.1895999999999995</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -5926,25 +5961,25 @@
         <v>31.049999999999997</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -5982,25 +6017,25 @@
         <v>29.52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
@@ -6038,25 +6073,25 @@
         <v>5.7984</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -6093,23 +6128,23 @@
         <v>37.68</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -6144,19 +6179,19 @@
         <v>3.8000000040000002</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="P10" s="43" t="s">
         <v>370</v>
-      </c>
-      <c r="P10" s="43" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Minor changes and added simple matlab data viewing script
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="388">
   <si>
     <t>Number</t>
   </si>
@@ -905,9 +905,6 @@
     <t>Ideal costs are hard to calculate without quote. See Shield Parts sheet for part breakdown without "Turnkey Tax"</t>
   </si>
   <si>
-    <t>12V Battery</t>
-  </si>
-  <si>
     <t>Seahorse SE-120 Waterproof Case</t>
   </si>
   <si>
@@ -1185,6 +1182,18 @@
   </si>
   <si>
     <t>Can be substituted with other parts</t>
+  </si>
+  <si>
+    <t>BatterySharks</t>
+  </si>
+  <si>
+    <t>12V 5.5Ah Sealed Lead Acid Battery</t>
+  </si>
+  <si>
+    <t>https://www.batterysharks.com/12-Volt-5-5-Amp-Sealed-Lead-Acid-Battery-p/12v-5.5ah_ups12-5.5.htm</t>
+  </si>
+  <si>
+    <t>BatterySharks is US source. The $30 ones were bought in europe, explaining the price</t>
   </si>
 </sst>
 </file>
@@ -2169,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,7 +2209,7 @@
         <v>283</v>
       </c>
       <c r="F1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J1" t="s">
         <v>282</v>
@@ -2396,7 +2405,7 @@
         <v>34</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2451,7 +2460,7 @@
         <v>37</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -2730,41 +2739,61 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="25" t="s">
-        <v>291</v>
+        <v>385</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="39">
+        <v>8.39</v>
+      </c>
       <c r="E12" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="21"/>
+        <v>8.39</v>
+      </c>
+      <c r="F12" s="21">
+        <f>D12</f>
+        <v>8.39</v>
+      </c>
       <c r="G12" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="21"/>
+        <v>83.9</v>
+      </c>
+      <c r="H12" s="21">
+        <f>D12</f>
+        <v>8.39</v>
+      </c>
       <c r="I12" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="87"/>
+        <v>209.75</v>
+      </c>
+      <c r="J12" s="87">
+        <v>32</v>
+      </c>
       <c r="K12" s="87">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="43"/>
+        <v>384</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="P12" s="43" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -2800,25 +2829,25 @@
         <v>141.96</v>
       </c>
       <c r="L13" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="M13" s="32" t="s">
         <v>293</v>
-      </c>
-      <c r="M13" s="32" t="s">
-        <v>294</v>
       </c>
       <c r="N13" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O13" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="P13" s="43" t="s">
         <v>295</v>
-      </c>
-      <c r="P13" s="43" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -2854,25 +2883,25 @@
         <v>479.88</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="M14" s="29" t="s">
         <v>298</v>
-      </c>
-      <c r="M14" s="29" t="s">
-        <v>299</v>
       </c>
       <c r="N14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O14" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="P14" s="43" t="s">
         <v>300</v>
-      </c>
-      <c r="P14" s="43" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -2908,7 +2937,7 @@
         <v>150.72</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M15" s="29">
         <v>2857</v>
@@ -2917,14 +2946,14 @@
         <v>18</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
@@ -2960,25 +2989,25 @@
         <v>161.52000000000001</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M16" s="32" t="s">
         <v>306</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>307</v>
       </c>
       <c r="N16" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O16" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="P16" s="43" t="s">
         <v>308</v>
-      </c>
-      <c r="P16" s="43" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
@@ -3013,25 +3042,25 @@
         <v>4008</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="M17" s="29" t="s">
         <v>323</v>
-      </c>
-      <c r="M17" s="29" t="s">
-        <v>324</v>
       </c>
       <c r="N17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O17" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="P17" s="43" t="s">
         <v>325</v>
-      </c>
-      <c r="P17" s="43" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -3068,23 +3097,23 @@
         <v>1283.8799999999999</v>
       </c>
       <c r="L18" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="M18" s="29" t="s">
         <v>313</v>
-      </c>
-      <c r="M18" s="29" t="s">
-        <v>314</v>
       </c>
       <c r="N18" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P18" s="43"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
@@ -3118,25 +3147,25 @@
         <v>3110.3999999999996</v>
       </c>
       <c r="L19" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M19" s="29" t="s">
         <v>318</v>
-      </c>
-      <c r="M19" s="29" t="s">
-        <v>319</v>
       </c>
       <c r="N19" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O19" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="P19" s="43" t="s">
         <v>320</v>
-      </c>
-      <c r="P19" s="43" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
@@ -3174,25 +3203,25 @@
         <v>2.9483999999999999</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N20" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O20" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="P20" s="43" t="s">
         <v>329</v>
-      </c>
-      <c r="P20" s="43" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -3229,25 +3258,25 @@
         <v>3.8049999960000003</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M21" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="N21" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="N21" s="29" t="s">
+      <c r="O21" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="O21" s="19" t="s">
+      <c r="P21" s="43" t="s">
         <v>334</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -3285,25 +3314,25 @@
         <v>13.152000000000001</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="P22" s="43" t="s">
         <v>338</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C23" s="4">
         <v>2</v>
@@ -3341,25 +3370,25 @@
         <v>3.5327999999999999</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N23" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O23" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P23" s="43" t="s">
         <v>342</v>
-      </c>
-      <c r="P23" s="43" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -3397,25 +3426,25 @@
         <v>119.044400004</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="P24" s="43" t="s">
         <v>365</v>
-      </c>
-      <c r="M24" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="N24" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="O24" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="P24" s="43" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
@@ -3453,25 +3482,25 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="N25" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O25" s="19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="P25" s="43" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
@@ -3509,25 +3538,25 @@
         <v>12.263999999999999</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N26" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P26" s="43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -3564,19 +3593,19 @@
         <v>54.599999999999994</v>
       </c>
       <c r="L27" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="M27" s="29" t="s">
         <v>381</v>
-      </c>
-      <c r="M27" s="29" t="s">
-        <v>382</v>
       </c>
       <c r="N27" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O27" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="P27" s="43" t="s">
         <v>383</v>
-      </c>
-      <c r="P27" s="43" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -3675,28 +3704,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>1059.6068833333334</v>
+        <v>1067.9968833333335</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>10063.938833333332</v>
+        <v>10147.838833333333</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>25128.847083333338</v>
+        <v>25338.597083333338</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>12199.526600000001</v>
+        <v>12583.526600000001</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3706,28 +3735,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>1059.6068833333334</v>
+        <v>1067.9968833333335</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>1006.3938833333332</v>
+        <v>1014.7838833333333</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>1005.1538833333335</v>
+        <v>1013.5438833333335</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>1016.6272166666668</v>
+        <v>1048.6272166666668</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -5892,7 +5921,7 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C4" s="45">
         <v>3</v>
@@ -5930,25 +5959,25 @@
         <v>8.0063999999999993</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="M4" s="29" t="s">
         <v>344</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>345</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -5986,25 +6015,25 @@
         <v>3.1895999999999995</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -6042,25 +6071,25 @@
         <v>31.049999999999997</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -6098,25 +6127,25 @@
         <v>29.52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
@@ -6154,25 +6183,25 @@
         <v>5.7984</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -6209,23 +6238,23 @@
         <v>37.68</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -6260,19 +6289,19 @@
         <v>3.8000000040000002</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="P10" s="43" t="s">
         <v>369</v>
-      </c>
-      <c r="P10" s="43" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added DS2 sonic code
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
     <sheet name="LiCor_Leveling_Base" sheetId="5" r:id="rId3"/>
-    <sheet name="Current Quotes" sheetId="4" r:id="rId4"/>
+    <sheet name="MLX90614 Housing" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="389">
   <si>
     <t>Number</t>
   </si>
@@ -791,81 +791,12 @@
     <t>Through Hole Placements:</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Last Updated</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Screaming Circuits</t>
   </si>
   <si>
-    <t>Assembly</t>
-  </si>
-  <si>
-    <t>Cost Quoted</t>
-  </si>
-  <si>
-    <t>Total Turn Time</t>
-  </si>
-  <si>
-    <t>20 Day</t>
-  </si>
-  <si>
-    <t>10 Day Full Proto</t>
-  </si>
-  <si>
-    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student. Requires boards from OshPark!</t>
-  </si>
-  <si>
-    <t>Add approximately $148.8 for power supply, SD Card holder; 10% Discount for being a student. Requires panelization and boards from OshPark!</t>
-  </si>
-  <si>
-    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student. Requires panelization and boards from OshPark!</t>
-  </si>
-  <si>
     <t>Osh Park</t>
   </si>
   <si>
-    <t>Printing</t>
-  </si>
-  <si>
-    <t>12 Calendar Days</t>
-  </si>
-  <si>
-    <t>Not Panelized! Cost will change with panelization</t>
-  </si>
-  <si>
-    <t>4PCB</t>
-  </si>
-  <si>
-    <t>Assembly+Printing</t>
-  </si>
-  <si>
-    <t>Cost Quoted+Extra Parts/Quantities (See formula for details)</t>
-  </si>
-  <si>
-    <t>10 Day</t>
-  </si>
-  <si>
-    <t>Includes everything</t>
-  </si>
-  <si>
-    <t>26 Day</t>
-  </si>
-  <si>
-    <t>Add approximately $89.28 for power supply, SD Card holder; 10% Discount for being a student</t>
-  </si>
-  <si>
-    <t>Quote is for 3 panels containing 4 pcbs each</t>
-  </si>
-  <si>
     <t>P033-ND</t>
   </si>
   <si>
@@ -914,9 +845,6 @@
     <t>SE-120</t>
   </si>
   <si>
-    <t>http://seahorsecases.com/Merchant2/merchant.mvc?Screen=PROD&amp;Store_Code=S&amp;Product_Code=SE-120&amp;Category_Code=SE_CASES</t>
-  </si>
-  <si>
     <t>Available from other sources</t>
   </si>
   <si>
@@ -1154,12 +1082,6 @@
     <t>1&amp;5/16" to 2&amp;1/4" Hose Clamp</t>
   </si>
   <si>
-    <t>Lowes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.lowes.com/pd/10-Pack-1-5-16-in-to-2-1-4-in-dia-Stainless-Steel-Adjustable-Clamps/3878586 </t>
-  </si>
-  <si>
     <t>94579</t>
   </si>
   <si>
@@ -1194,6 +1116,87 @@
   </si>
   <si>
     <t>BatterySharks is US source. The $30 ones were bought in europe, explaining the price</t>
+  </si>
+  <si>
+    <t>PVC T Conduit</t>
+  </si>
+  <si>
+    <t>PVC Elbow</t>
+  </si>
+  <si>
+    <t>Lowe's</t>
+  </si>
+  <si>
+    <t>50916</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/CARLON-1-2-in-Schedule-40-PVC-Elbow/1091493</t>
+  </si>
+  <si>
+    <t>PVC 90-Degree T Fitting</t>
+  </si>
+  <si>
+    <t>23873</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/LASCO-1-2-in-Dia-90-Degree-PVC-Sch-40-Tee/1067651</t>
+  </si>
+  <si>
+    <t>Faucet Repair Kit</t>
+  </si>
+  <si>
+    <t>502098</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/BrassCraft-Faucet-Repair-Kit/4778474</t>
+  </si>
+  <si>
+    <t>Only need screen, not washer</t>
+  </si>
+  <si>
+    <t>1/2" Coupling</t>
+  </si>
+  <si>
+    <t>423565</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/The-Hillman-Group-2-Count-5-16-in-x-1-1-4-in-Rubber-Standard-SAE-Flat-Washers/4582595</t>
+  </si>
+  <si>
+    <t>Comes in 2 pack</t>
+  </si>
+  <si>
+    <t>Rubber Flat Washer</t>
+  </si>
+  <si>
+    <t>Zinc-Plated Standard Washer</t>
+  </si>
+  <si>
+    <t>136616</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/The-Hillman-Group-4-Count-1-4-in-x-1-in-Zinc-Plated-Standard-SAE-Fender-Washers/3012355</t>
+  </si>
+  <si>
+    <t>Comes in 4 pack</t>
+  </si>
+  <si>
+    <t>1-5/16" to 2-1/4" Hose Clamp</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/10-Pack-1-5-16-in-to-2-1-4-in-dia-Stainless-Steel-Adjustable-Clamps/3878586</t>
+  </si>
+  <si>
+    <t>Comes in 10 pack</t>
+  </si>
+  <si>
+    <t>http://www.seahorsecases.com/Seahorse-SE120-Small-Waterproof-Protective-Equipment-Storage-Shipping-Case.html</t>
+  </si>
+  <si>
+    <t>5415K18</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#5415k18/=178w5hq</t>
   </si>
 </sst>
 </file>
@@ -1208,14 +1211,7 @@
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1235,14 +1231,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1659,28 +1647,28 @@
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1702,7 +1690,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1710,7 +1698,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -1738,7 +1726,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1753,7 +1741,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1769,17 +1757,8 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="17" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="17" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1790,6 +1769,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1822,7 +1804,6 @@
     </xf>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Currency" xfId="20" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1833,6 +1814,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2178,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2206,13 +2188,13 @@
       <c r="A1" s="46"/>
       <c r="B1" s="1"/>
       <c r="D1" s="3" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="J1" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="K1">
         <v>12</v>
@@ -2220,34 +2202,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="90"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="97" t="s">
+      <c r="D2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="100" t="s">
+      <c r="E2" s="91"/>
+      <c r="F2" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="97" t="s">
+      <c r="G2" s="91"/>
+      <c r="H2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="97" t="s">
+      <c r="I2" s="91"/>
+      <c r="J2" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="K2" s="95"/>
+      <c r="L2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="101"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="95" t="s">
+      <c r="M2" s="93"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="87" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2297,7 +2279,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="96"/>
+      <c r="P3" s="88"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2329,11 +2311,11 @@
         <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
         <v>20.3</v>
       </c>
-      <c r="J4" s="87">
+      <c r="J4" s="78">
         <f>F4</f>
         <v>0.81200000000000006</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="78">
         <f>J4*$K$1</f>
         <v>9.7439999999999998</v>
       </c>
@@ -2341,13 +2323,13 @@
         <v>41</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="P4" s="43" t="s">
         <v>32</v>
@@ -2384,11 +2366,11 @@
         <f t="shared" si="2"/>
         <v>623.75</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="78">
         <f>F5</f>
         <v>24.95</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="78">
         <f t="shared" ref="K5:K30" si="3">J5*$K$1</f>
         <v>299.39999999999998</v>
       </c>
@@ -2405,7 +2387,7 @@
         <v>34</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2439,11 +2421,11 @@
         <f t="shared" si="2"/>
         <v>323.75</v>
       </c>
-      <c r="J6" s="87">
+      <c r="J6" s="78">
         <f>F6</f>
         <v>12.95</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="78">
         <f t="shared" si="3"/>
         <v>155.39999999999998</v>
       </c>
@@ -2460,7 +2442,7 @@
         <v>37</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -2492,11 +2474,11 @@
         <f t="shared" si="2"/>
         <v>561.5</v>
       </c>
-      <c r="J7" s="87">
+      <c r="J7" s="78">
         <f>F7</f>
         <v>23.7</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="78">
         <f t="shared" si="3"/>
         <v>284.39999999999998</v>
       </c>
@@ -2544,11 +2526,11 @@
         <f t="shared" si="2"/>
         <v>43.875</v>
       </c>
-      <c r="J8" s="87">
+      <c r="J8" s="78">
         <f>F8</f>
         <v>1.7549999999999999</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="78">
         <f t="shared" si="3"/>
         <v>21.06</v>
       </c>
@@ -2571,7 +2553,7 @@
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -2600,16 +2582,16 @@
         <f t="shared" si="2"/>
         <v>408.41666666666663</v>
       </c>
-      <c r="J9" s="87">
+      <c r="J9" s="78">
         <f>331.5/12</f>
         <v>27.625</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="78">
         <f t="shared" si="3"/>
         <v>331.5</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="M9" s="32" t="s">
         <v>18</v>
@@ -2618,21 +2600,21 @@
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="P9" s="43" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="89">
+      <c r="D10" s="80">
         <f>J10*1</f>
         <v>70.732500000000002</v>
       </c>
@@ -2640,7 +2622,7 @@
         <f t="shared" si="0"/>
         <v>70.732500000000002</v>
       </c>
-      <c r="F10" s="90">
+      <c r="F10" s="81">
         <f>J10</f>
         <v>70.732500000000002</v>
       </c>
@@ -2648,7 +2630,7 @@
         <f t="shared" si="1"/>
         <v>707.32500000000005</v>
       </c>
-      <c r="H10" s="90">
+      <c r="H10" s="81">
         <f>J10</f>
         <v>70.732500000000002</v>
       </c>
@@ -2656,16 +2638,16 @@
         <f t="shared" si="2"/>
         <v>1768.3125</v>
       </c>
-      <c r="J10" s="87">
+      <c r="J10" s="78">
         <f>(943.1-94.31)/12</f>
         <v>70.732500000000002</v>
       </c>
-      <c r="K10" s="87">
+      <c r="K10" s="78">
         <f t="shared" si="3"/>
         <v>848.79</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M10" s="32" t="s">
         <v>18</v>
@@ -2674,21 +2656,21 @@
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="P10" s="43" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="89">
+      <c r="D11" s="80">
         <f>J11</f>
         <v>58.594166666666666</v>
       </c>
@@ -2696,7 +2678,7 @@
         <f t="shared" si="0"/>
         <v>58.594166666666666</v>
       </c>
-      <c r="F11" s="90">
+      <c r="F11" s="81">
         <f>J11</f>
         <v>58.594166666666666</v>
       </c>
@@ -2704,7 +2686,7 @@
         <f t="shared" si="1"/>
         <v>585.94166666666661</v>
       </c>
-      <c r="H11" s="90">
+      <c r="H11" s="81">
         <f>J11</f>
         <v>58.594166666666666</v>
       </c>
@@ -2712,16 +2694,16 @@
         <f t="shared" si="2"/>
         <v>1464.8541666666667</v>
       </c>
-      <c r="J11" s="87">
+      <c r="J11" s="78">
         <f>703.13/12</f>
         <v>58.594166666666666</v>
       </c>
-      <c r="K11" s="87">
+      <c r="K11" s="78">
         <f t="shared" si="3"/>
         <v>703.13</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M11" s="32" t="s">
         <v>18</v>
@@ -2730,16 +2712,16 @@
         <v>18</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="P11" s="43" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="25" t="s">
-        <v>385</v>
+        <v>359</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -2767,15 +2749,15 @@
         <f t="shared" si="2"/>
         <v>209.75</v>
       </c>
-      <c r="J12" s="87">
+      <c r="J12" s="78">
         <v>32</v>
       </c>
-      <c r="K12" s="87">
+      <c r="K12" s="78">
         <f t="shared" si="3"/>
         <v>384</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>384</v>
+        <v>358</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>18</v>
@@ -2784,16 +2766,16 @@
         <v>18</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>386</v>
+        <v>360</v>
       </c>
       <c r="P12" s="43" t="s">
-        <v>387</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="25" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -2821,33 +2803,33 @@
         <f t="shared" si="2"/>
         <v>295.75</v>
       </c>
-      <c r="J13" s="87">
+      <c r="J13" s="78">
         <v>11.83</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="78">
         <f t="shared" si="3"/>
         <v>141.96</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="N13" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>294</v>
+        <v>386</v>
       </c>
       <c r="P13" s="43" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="25" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -2875,33 +2857,33 @@
         <f t="shared" si="2"/>
         <v>999.75</v>
       </c>
-      <c r="J14" s="87">
+      <c r="J14" s="78">
         <v>39.99</v>
       </c>
-      <c r="K14" s="87">
+      <c r="K14" s="78">
         <f t="shared" si="3"/>
         <v>479.88</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="M14" s="29" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="N14" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="P14" s="43" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="25" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -2928,16 +2910,16 @@
         <f t="shared" si="2"/>
         <v>314</v>
       </c>
-      <c r="J15" s="87">
+      <c r="J15" s="78">
         <f>F15</f>
         <v>12.56</v>
       </c>
-      <c r="K15" s="87">
+      <c r="K15" s="78">
         <f t="shared" si="3"/>
         <v>150.72</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="M15" s="29">
         <v>2857</v>
@@ -2946,14 +2928,14 @@
         <v>18</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="25" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
@@ -2980,34 +2962,34 @@
         <f t="shared" si="2"/>
         <v>336.5</v>
       </c>
-      <c r="J16" s="87">
+      <c r="J16" s="78">
         <f>F16</f>
         <v>13.46</v>
       </c>
-      <c r="K16" s="87">
+      <c r="K16" s="78">
         <f t="shared" si="3"/>
         <v>161.52000000000001</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="N16" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="P16" s="43" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
@@ -3033,34 +3015,34 @@
         <f t="shared" si="2"/>
         <v>8350</v>
       </c>
-      <c r="J17" s="87">
+      <c r="J17" s="78">
         <f>H17*C17</f>
         <v>334</v>
       </c>
-      <c r="K17" s="87">
+      <c r="K17" s="78">
         <f t="shared" si="3"/>
         <v>4008</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="N17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O17" s="19" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="P17" s="43" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -3088,32 +3070,32 @@
         <f t="shared" si="2"/>
         <v>2674.75</v>
       </c>
-      <c r="J18" s="87">
+      <c r="J18" s="78">
         <f>D18</f>
         <v>106.99</v>
       </c>
-      <c r="K18" s="87">
+      <c r="K18" s="78">
         <f t="shared" si="3"/>
         <v>1283.8799999999999</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="N18" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="P18" s="43"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="25" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
@@ -3139,33 +3121,33 @@
         <f t="shared" si="2"/>
         <v>6480</v>
       </c>
-      <c r="J19" s="87">
+      <c r="J19" s="78">
         <v>259.2</v>
       </c>
-      <c r="K19" s="87">
+      <c r="K19" s="78">
         <f t="shared" si="3"/>
         <v>3110.3999999999996</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="N19" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="P19" s="43" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
@@ -3194,34 +3176,34 @@
         <f t="shared" si="2"/>
         <v>6.1425000000000001</v>
       </c>
-      <c r="J20" s="87">
+      <c r="J20" s="78">
         <f>E20</f>
         <v>0.2457</v>
       </c>
-      <c r="K20" s="87">
+      <c r="K20" s="78">
         <f t="shared" si="3"/>
         <v>2.9483999999999999</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="N20" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O20" s="19" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="P20" s="43" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -3249,34 +3231,34 @@
         <f t="shared" si="2"/>
         <v>7.9270833250000008</v>
       </c>
-      <c r="J21" s="87">
+      <c r="J21" s="78">
         <f>D21</f>
         <v>0.31708333300000002</v>
       </c>
-      <c r="K21" s="87">
+      <c r="K21" s="78">
         <f t="shared" si="3"/>
         <v>3.8049999960000003</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="N21" s="29" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="O21" s="19" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="P21" s="43" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -3305,34 +3287,34 @@
         <f t="shared" si="2"/>
         <v>27.400000000000002</v>
       </c>
-      <c r="J22" s="87">
+      <c r="J22" s="78">
         <f>D22</f>
         <v>1.0960000000000001</v>
       </c>
-      <c r="K22" s="87">
+      <c r="K22" s="78">
         <f t="shared" si="3"/>
         <v>13.152000000000001</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="N22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="P22" s="43" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="C23" s="4">
         <v>2</v>
@@ -3361,34 +3343,34 @@
         <f t="shared" si="2"/>
         <v>7.3599999999999994</v>
       </c>
-      <c r="J23" s="87">
+      <c r="J23" s="78">
         <f>E23</f>
         <v>0.2944</v>
       </c>
-      <c r="K23" s="87">
+      <c r="K23" s="78">
         <f t="shared" si="3"/>
         <v>3.5327999999999999</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="N23" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="P23" s="43" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
@@ -3417,34 +3399,34 @@
         <f t="shared" si="2"/>
         <v>248.00916667499999</v>
       </c>
-      <c r="J24" s="87">
+      <c r="J24" s="78">
         <f>D24</f>
         <v>9.9203666669999997</v>
       </c>
-      <c r="K24" s="87">
+      <c r="K24" s="78">
         <f t="shared" si="3"/>
         <v>119.044400004</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="M24" s="29" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="N24" s="29" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="P24" s="43" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
@@ -3473,90 +3455,89 @@
         <f t="shared" si="2"/>
         <v>1.6500000000000001</v>
       </c>
-      <c r="J25" s="87">
+      <c r="J25" s="78">
         <f>D25</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="K25" s="87">
+      <c r="K25" s="78">
         <f t="shared" si="3"/>
         <v>0.39600000000000002</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="N25" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O25" s="19" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="P25" s="43" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="25" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
       <c r="D26" s="39">
-        <f>10.22/10</f>
-        <v>1.022</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="E26" s="26">
         <f t="shared" si="0"/>
-        <v>2.044</v>
+        <v>1.3979999999999999</v>
       </c>
       <c r="F26" s="21">
         <f>D26</f>
-        <v>1.022</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="G26" s="20">
         <f t="shared" si="1"/>
-        <v>20.440000000000001</v>
+        <v>13.979999999999999</v>
       </c>
       <c r="H26" s="21">
         <f>D26</f>
-        <v>1.022</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="I26" s="20">
         <f t="shared" si="2"/>
-        <v>51.1</v>
-      </c>
-      <c r="J26" s="87">
+        <v>34.949999999999996</v>
+      </c>
+      <c r="J26" s="78">
         <f>D26</f>
-        <v>1.022</v>
-      </c>
-      <c r="K26" s="87">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="K26" s="78">
         <f t="shared" si="3"/>
-        <v>12.263999999999999</v>
+        <v>8.3879999999999999</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>374</v>
+        <v>319</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="N26" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="O26" s="4" t="s">
-        <v>375</v>
+      <c r="O26" s="19" t="s">
+        <v>388</v>
       </c>
       <c r="P26" s="43" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="25" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -3584,28 +3565,28 @@
         <f t="shared" si="2"/>
         <v>113.75</v>
       </c>
-      <c r="J27" s="87">
+      <c r="J27" s="78">
         <f>D27</f>
         <v>4.55</v>
       </c>
-      <c r="K27" s="87">
+      <c r="K27" s="78">
         <f t="shared" si="3"/>
         <v>54.599999999999994</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>380</v>
+        <v>354</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>381</v>
+        <v>355</v>
       </c>
       <c r="N27" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="O27" s="4" t="s">
-        <v>382</v>
+      <c r="O27" s="19" t="s">
+        <v>356</v>
       </c>
       <c r="P27" s="43" t="s">
-        <v>383</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -3627,8 +3608,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87">
+      <c r="J28" s="78"/>
+      <c r="K28" s="78">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3657,8 +3638,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87">
+      <c r="J29" s="78"/>
+      <c r="K29" s="78">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3687,8 +3668,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88">
+      <c r="J30" s="79"/>
+      <c r="K30" s="79">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3704,28 +3685,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>1067.9968833333335</v>
+        <v>1067.3508833333333</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>10147.838833333333</v>
+        <v>10141.378833333332</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>25338.597083333338</v>
+        <v>25322.44708333334</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>12583.526600000001</v>
+        <v>12579.650600000003</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3735,28 +3716,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>1067.9968833333335</v>
+        <v>1067.3508833333333</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>1014.7838833333333</v>
+        <v>1014.1378833333332</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>1013.5438833333335</v>
+        <v>1012.8978833333335</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>1048.6272166666668</v>
+        <v>1048.3042166666669</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -3774,6 +3755,8 @@
     <hyperlink ref="O9" r:id="rId1"/>
     <hyperlink ref="O10" r:id="rId2"/>
     <hyperlink ref="O11" r:id="rId3"/>
+    <hyperlink ref="O26" r:id="rId4" location="5415k18/=178w5hq"/>
+    <hyperlink ref="O27" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3810,10 +3793,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="104"/>
+      <c r="B1" s="96"/>
       <c r="C1" s="50" t="s">
         <v>61</v>
       </c>
@@ -3825,33 +3808,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="97" t="s">
+      <c r="G2" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="99"/>
-      <c r="I2" s="100" t="s">
+      <c r="H2" s="91"/>
+      <c r="I2" s="92" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="99"/>
-      <c r="K2" s="97" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="99"/>
-      <c r="M2" s="97" t="s">
+      <c r="L2" s="91"/>
+      <c r="M2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="101"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="95" t="s">
+      <c r="N2" s="93"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="87" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3904,7 +3887,7 @@
       <c r="P3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="96"/>
+      <c r="Q3" s="88"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -5801,7 +5784,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5828,10 +5811,10 @@
       <c r="A1" s="46"/>
       <c r="B1" s="1"/>
       <c r="D1" s="3" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="J1" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="K1">
         <v>12</v>
@@ -5839,34 +5822,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="97" t="s">
+      <c r="B2" s="90"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="99"/>
-      <c r="F2" s="100" t="s">
+      <c r="E2" s="91"/>
+      <c r="F2" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="97" t="s">
+      <c r="G2" s="91"/>
+      <c r="H2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="102" t="s">
-        <v>281</v>
-      </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="97" t="s">
+      <c r="I2" s="91"/>
+      <c r="J2" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="K2" s="95"/>
+      <c r="L2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="101"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="95" t="s">
+      <c r="M2" s="93"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="87" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5916,12 +5899,12 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="96"/>
+      <c r="P3" s="88"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="C4" s="45">
         <v>3</v>
@@ -5950,34 +5933,34 @@
         <f t="shared" ref="I4:I17" si="4">C4*H4*25</f>
         <v>16.68</v>
       </c>
-      <c r="J4" s="87">
+      <c r="J4" s="78">
         <f>E4</f>
         <v>0.66720000000000002</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="78">
         <f t="shared" ref="K4:K17" si="5">J4*$K$1</f>
         <v>8.0063999999999993</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -6006,34 +5989,34 @@
         <f t="shared" si="4"/>
         <v>6.6449999999999996</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="78">
         <f>E5</f>
         <v>0.26579999999999998</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="78">
         <f t="shared" si="5"/>
         <v>3.1895999999999995</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -6062,34 +6045,34 @@
         <f t="shared" si="4"/>
         <v>64.6875</v>
       </c>
-      <c r="J6" s="87">
+      <c r="J6" s="78">
         <f>E6</f>
         <v>2.5874999999999999</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="78">
         <f t="shared" si="5"/>
         <v>31.049999999999997</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -6118,34 +6101,34 @@
         <f t="shared" si="4"/>
         <v>61.5</v>
       </c>
-      <c r="J7" s="87">
+      <c r="J7" s="78">
         <f>E7</f>
         <v>2.46</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="78">
         <f t="shared" si="5"/>
         <v>29.52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
@@ -6174,34 +6157,34 @@
         <f t="shared" si="4"/>
         <v>12.08</v>
       </c>
-      <c r="J8" s="87">
+      <c r="J8" s="78">
         <f>E8</f>
         <v>0.48320000000000002</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="78">
         <f t="shared" si="5"/>
         <v>5.7984</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -6229,102 +6212,102 @@
         <f t="shared" si="4"/>
         <v>78.5</v>
       </c>
-      <c r="J9" s="87">
+      <c r="J9" s="78">
         <f>D9</f>
         <v>3.14</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="78">
         <f t="shared" si="5"/>
         <v>37.68</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="93">
+      <c r="D10" s="84">
         <v>0.31666666700000001</v>
       </c>
       <c r="E10" s="26">
         <f t="shared" si="0"/>
         <v>0.31666666700000001</v>
       </c>
-      <c r="F10" s="94">
+      <c r="F10" s="85">
         <v>0.31666666700000001</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="2"/>
         <v>3.1666666700000001</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="85">
         <v>0.31666666700000001</v>
       </c>
       <c r="I10" s="20">
         <f t="shared" si="4"/>
         <v>7.9166666750000001</v>
       </c>
-      <c r="J10" s="87">
+      <c r="J10" s="78">
         <f>D10</f>
         <v>0.31666666700000001</v>
       </c>
-      <c r="K10" s="87">
+      <c r="K10" s="78">
         <f t="shared" si="5"/>
         <v>3.8000000040000002</v>
       </c>
       <c r="L10" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="M10" s="32" t="s">
         <v>343</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>367</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="P10" s="43" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="93"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="94"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H11" s="94"/>
+      <c r="H11" s="85"/>
       <c r="I11" s="20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87">
+      <c r="J11" s="78"/>
+      <c r="K11" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6353,8 +6336,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87">
+      <c r="J12" s="78"/>
+      <c r="K12" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6383,8 +6366,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87">
+      <c r="J13" s="78"/>
+      <c r="K13" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6413,8 +6396,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J14" s="91"/>
-      <c r="K14" s="87">
+      <c r="J14" s="82"/>
+      <c r="K14" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6443,8 +6426,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87">
+      <c r="J15" s="78"/>
+      <c r="K15" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6473,8 +6456,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87">
+      <c r="J16" s="78"/>
+      <c r="K16" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6503,8 +6486,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87">
+      <c r="J17" s="78"/>
+      <c r="K17" s="78">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -6533,8 +6516,8 @@
         <f t="shared" ref="I18:I30" si="8">C18*H18*25</f>
         <v>0</v>
       </c>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87">
+      <c r="J18" s="78"/>
+      <c r="K18" s="78">
         <f t="shared" ref="K18:K30" si="9">J18*$K$1</f>
         <v>0</v>
       </c>
@@ -6563,8 +6546,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87">
+      <c r="J19" s="78"/>
+      <c r="K19" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6593,8 +6576,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J20" s="87"/>
-      <c r="K20" s="87">
+      <c r="J20" s="78"/>
+      <c r="K20" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6623,8 +6606,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J21" s="87"/>
-      <c r="K21" s="87">
+      <c r="J21" s="78"/>
+      <c r="K21" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6653,8 +6636,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87">
+      <c r="J22" s="78"/>
+      <c r="K22" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6683,8 +6666,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87">
+      <c r="J23" s="78"/>
+      <c r="K23" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6713,8 +6696,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87">
+      <c r="J24" s="78"/>
+      <c r="K24" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6743,8 +6726,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87">
+      <c r="J25" s="78"/>
+      <c r="K25" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6773,8 +6756,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J26" s="87"/>
-      <c r="K26" s="87">
+      <c r="J26" s="78"/>
+      <c r="K26" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6803,8 +6786,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87">
+      <c r="J27" s="78"/>
+      <c r="K27" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6833,8 +6816,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87">
+      <c r="J28" s="78"/>
+      <c r="K28" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6863,8 +6846,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87">
+      <c r="J29" s="78"/>
+      <c r="K29" s="78">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6893,8 +6876,8 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88">
+      <c r="J30" s="79"/>
+      <c r="K30" s="79">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6982,331 +6965,1153 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I11"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="78" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="85" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.83203125" style="82" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="82" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="118.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="101" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" s="84" t="s">
-        <v>254</v>
-      </c>
-      <c r="C2" s="79" t="s">
-        <v>255</v>
-      </c>
-      <c r="D2" s="79" t="s">
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="46"/>
+      <c r="B1" s="1"/>
+      <c r="D1" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="E2" s="79" t="s">
-        <v>256</v>
-      </c>
-      <c r="F2" s="86" t="s">
+      <c r="J1" t="s">
         <v>259</v>
       </c>
-      <c r="G2" s="81" t="s">
-        <v>272</v>
-      </c>
-      <c r="H2" s="83" t="s">
+      <c r="K1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="90"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="91"/>
+      <c r="H2" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="91"/>
+      <c r="J2" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="K2" s="95"/>
+      <c r="L2" s="89" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="93"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="80" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" s="78">
-        <v>42607</v>
-      </c>
-      <c r="C3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="88"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="C4" s="45">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="26">
+        <f t="shared" ref="E4:E30" si="0">C4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="20">
+        <f t="shared" ref="G4:G30" si="1">C4*F4*10</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="41"/>
+      <c r="I4" s="20">
+        <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78">
+        <f t="shared" ref="K4:K30" si="3">J4*$K$1</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="43"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.65</v>
+      </c>
+      <c r="E5" s="26">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="F5" s="21">
+        <f>D5</f>
+        <v>0.65</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="H5" s="21">
+        <f>D5</f>
+        <v>0.65</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="2"/>
+        <v>16.25</v>
+      </c>
+      <c r="J5" s="78">
+        <v>0.65</v>
+      </c>
+      <c r="K5" s="78">
+        <f t="shared" si="3"/>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="N5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="P5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="39">
+        <v>0.39</v>
+      </c>
+      <c r="E6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+      <c r="F6" s="21">
+        <f>D6</f>
+        <v>0.39</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="1"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="H6" s="21">
+        <f>D6</f>
+        <v>0.39</v>
+      </c>
+      <c r="I6" s="20">
+        <f t="shared" si="2"/>
+        <v>9.75</v>
+      </c>
+      <c r="J6" s="78">
+        <v>0.39</v>
+      </c>
+      <c r="K6" s="78">
+        <f t="shared" si="3"/>
+        <v>4.68</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="P6" s="43"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="39">
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
+      <c r="F7" s="21">
+        <f>D7</f>
+        <v>0.99</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+      <c r="H7" s="21">
+        <f>D7</f>
+        <v>0.99</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="2"/>
+        <v>24.75</v>
+      </c>
+      <c r="J7" s="78">
+        <v>0.99</v>
+      </c>
+      <c r="K7" s="78">
+        <f t="shared" si="3"/>
+        <v>11.879999999999999</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="P7" s="43" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="21"/>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="43"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="39">
+        <f>1.07/2</f>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F9" s="21">
+        <f>D9</f>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="1"/>
+        <v>5.3500000000000005</v>
+      </c>
+      <c r="H9" s="21">
+        <f>D9</f>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>13.375</v>
+      </c>
+      <c r="J9" s="78">
+        <f>D9</f>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="K9" s="78">
+        <f t="shared" si="3"/>
+        <v>6.42</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="P9" s="43" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="84">
+        <f>1.15/4</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="E10" s="26">
+        <f t="shared" si="0"/>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="F10" s="85">
+        <f>D10</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" si="1"/>
+        <v>2.875</v>
+      </c>
+      <c r="H10" s="85">
+        <f>D10</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="I10" s="20">
+        <f t="shared" si="2"/>
+        <v>7.1874999999999991</v>
+      </c>
+      <c r="J10" s="78">
+        <f>D10</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="K10" s="78">
+        <f t="shared" si="3"/>
+        <v>3.4499999999999997</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="P10" s="43" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="84">
+        <f>10.22/10</f>
+        <v>1.022</v>
+      </c>
+      <c r="E11" s="26">
+        <f t="shared" si="0"/>
+        <v>1.022</v>
+      </c>
+      <c r="F11" s="85">
+        <f>D11</f>
+        <v>1.022</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="1"/>
+        <v>10.220000000000001</v>
+      </c>
+      <c r="H11" s="85">
+        <f>D11</f>
+        <v>1.022</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>25.55</v>
+      </c>
+      <c r="J11" s="78">
+        <f>D11</f>
+        <v>1.022</v>
+      </c>
+      <c r="K11" s="78">
+        <f t="shared" si="3"/>
+        <v>12.263999999999999</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="P11" s="43" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="43"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="82"/>
+      <c r="K14" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="43"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="43"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="43"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="43"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="43"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="21"/>
+      <c r="I22" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="43"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="78"/>
+      <c r="K23" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="43"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="78"/>
+      <c r="K24" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="43"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="43"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="21"/>
+      <c r="I26" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="43"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="78"/>
+      <c r="K27" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="43"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="43"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="43"/>
+    </row>
+    <row r="30" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="G30" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="44"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D31" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="85">
-        <v>1368.93</v>
-      </c>
-      <c r="G3" s="85">
-        <f>F3+89.28+G7</f>
-        <v>1700.71</v>
-      </c>
-      <c r="H3" s="82">
-        <f>G3/E3</f>
-        <v>141.72583333333333</v>
-      </c>
-      <c r="I3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B4" s="78">
-        <v>42607</v>
-      </c>
-      <c r="C4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D4" t="s">
-        <v>261</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4" s="85">
-        <v>1902.4</v>
-      </c>
-      <c r="G4" s="85">
-        <f>F4+148.8+G7*2</f>
-        <v>2536.2000000000003</v>
-      </c>
-      <c r="H4" s="82">
-        <f t="shared" ref="H4:H5" si="0">G4/E4</f>
-        <v>126.81000000000002</v>
-      </c>
-      <c r="I4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B5" s="78">
-        <v>42607</v>
-      </c>
-      <c r="C5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E5">
+      <c r="E31" s="24">
+        <f>SUM(E4:E30)</f>
+        <v>3.8745000000000003</v>
+      </c>
+      <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="85">
-        <v>1720.43</v>
-      </c>
-      <c r="G5" s="85">
-        <f>F5+89.28+F8*4</f>
-        <v>2006.71</v>
-      </c>
-      <c r="H5" s="82">
-        <f t="shared" si="0"/>
-        <v>167.22583333333333</v>
-      </c>
-      <c r="I5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>257</v>
-      </c>
-      <c r="B6" s="78">
-        <v>42611</v>
-      </c>
-      <c r="C6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E6">
+      <c r="G31" s="24">
+        <f>SUM(G4:G30)</f>
+        <v>38.745000000000005</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="85">
-        <v>2331.33</v>
-      </c>
-      <c r="G6" s="85">
-        <f>F6+90.28</f>
-        <v>2421.61</v>
-      </c>
-      <c r="H6" s="82">
-        <f>G6/E6</f>
-        <v>201.80083333333334</v>
-      </c>
-      <c r="I6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>266</v>
-      </c>
-      <c r="B7" s="78">
-        <v>42612</v>
-      </c>
-      <c r="C7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E7">
+      <c r="I31" s="24">
+        <f>SUM(I4:I30)</f>
+        <v>96.862499999999997</v>
+      </c>
+      <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="85">
-        <v>242.5</v>
-      </c>
-      <c r="G7" s="85">
-        <f>F7</f>
-        <v>242.5</v>
-      </c>
-      <c r="H7" s="82">
-        <f>G7/E7</f>
-        <v>20.208333333333332</v>
-      </c>
-      <c r="I7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B8" s="78">
-        <v>42607</v>
-      </c>
-      <c r="C8" t="s">
-        <v>267</v>
-      </c>
-      <c r="D8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" s="85">
-        <v>49.25</v>
-      </c>
-      <c r="G8" s="85"/>
-      <c r="H8" s="82">
-        <f>F8/E8</f>
-        <v>16.416666666666668</v>
-      </c>
-      <c r="I8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B9" s="78">
-        <v>42611</v>
-      </c>
-      <c r="C9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" t="s">
-        <v>273</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="85">
-        <v>2528.4899999999998</v>
-      </c>
-      <c r="G9" s="85">
-        <f>F9</f>
-        <v>2528.4899999999998</v>
-      </c>
-      <c r="H9" s="82">
-        <f>G9/E9</f>
-        <v>252.84899999999999</v>
-      </c>
-      <c r="I9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>270</v>
-      </c>
-      <c r="B10" s="78">
-        <v>42611</v>
-      </c>
-      <c r="C10" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" t="s">
-        <v>273</v>
-      </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10" s="85">
-        <v>3372.79</v>
-      </c>
-      <c r="G10" s="85">
-        <f t="shared" ref="G10:G11" si="1">F10</f>
-        <v>3372.79</v>
-      </c>
-      <c r="H10" s="82">
-        <f t="shared" ref="H10:H11" si="2">G10/E10</f>
-        <v>168.6395</v>
-      </c>
-      <c r="I10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>270</v>
-      </c>
-      <c r="B11" s="78">
-        <v>42611</v>
-      </c>
-      <c r="C11" t="s">
-        <v>271</v>
-      </c>
-      <c r="D11" t="s">
-        <v>273</v>
-      </c>
-      <c r="E11">
-        <v>25</v>
-      </c>
-      <c r="F11" s="85">
-        <v>3826.44</v>
-      </c>
-      <c r="G11" s="85">
-        <f t="shared" si="1"/>
-        <v>3826.44</v>
-      </c>
-      <c r="H11" s="82">
-        <f t="shared" si="2"/>
-        <v>153.05760000000001</v>
-      </c>
-      <c r="I11" t="s">
-        <v>274</v>
-      </c>
+      <c r="K31" s="24">
+        <f>SUM(K4:K30)</f>
+        <v>46.494</v>
+      </c>
+      <c r="N31" s="30"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="24">
+        <f>E31</f>
+        <v>3.8745000000000003</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="35">
+        <f>G31/10</f>
+        <v>3.8745000000000003</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="35">
+        <f>I31/25</f>
+        <v>3.8744999999999998</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="35">
+        <f>K31/K1</f>
+        <v>3.8744999999999998</v>
+      </c>
+      <c r="N32" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:O2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated MLX housing instructions
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="393">
   <si>
     <t>Number</t>
   </si>
@@ -1154,9 +1154,6 @@
     <t>Only need screen, not washer</t>
   </si>
   <si>
-    <t>1/2" Coupling</t>
-  </si>
-  <si>
     <t>423565</t>
   </si>
   <si>
@@ -1197,6 +1194,21 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/#5415k18/=178w5hq</t>
+  </si>
+  <si>
+    <t>1/2" PVC Coupling</t>
+  </si>
+  <si>
+    <t>115991</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/CARLON-1-2-in-PVC-Transition/3127629</t>
+  </si>
+  <si>
+    <t>23761</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Genova-1-2-in-Dia-Coupling-CPVC-Fittings/1000200923</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
@@ -2820,7 +2832,7 @@
         <v>18</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="P13" s="43" t="s">
         <v>271</v>
@@ -3522,13 +3534,13 @@
         <v>319</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N26" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="P26" s="43" t="s">
         <v>351</v>
@@ -6967,8 +6979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6979,6 +6991,7 @@
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="101" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.5" bestFit="1" customWidth="1"/>
@@ -7086,30 +7099,49 @@
       <c r="C4" s="45">
         <v>1</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="37">
+        <v>2.48</v>
+      </c>
       <c r="E4" s="26">
         <f t="shared" ref="E4:E30" si="0">C4*D4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="41"/>
+        <v>2.48</v>
+      </c>
+      <c r="F4" s="41">
+        <f>D4</f>
+        <v>2.48</v>
+      </c>
       <c r="G4" s="20">
         <f t="shared" ref="G4:G30" si="1">C4*F4*10</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="41"/>
+        <v>24.8</v>
+      </c>
+      <c r="H4" s="41">
+        <f>D4</f>
+        <v>2.48</v>
+      </c>
       <c r="I4" s="20">
         <f t="shared" ref="I4:I30" si="2">C4*H4*25</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="78"/>
+        <v>62</v>
+      </c>
+      <c r="J4" s="78">
+        <f>D4</f>
+        <v>2.48</v>
+      </c>
       <c r="K4" s="78">
         <f t="shared" ref="K4:K30" si="3">J4*$K$1</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="19"/>
+        <v>29.759999999999998</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="19" t="s">
+        <v>390</v>
+      </c>
       <c r="P4" s="43"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -7273,39 +7305,59 @@
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>374</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="39"/>
+        <v>388</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39">
+        <v>0.33</v>
+      </c>
       <c r="E8" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="21"/>
+        <v>0.33</v>
+      </c>
+      <c r="F8" s="21">
+        <f>D8</f>
+        <v>0.33</v>
+      </c>
       <c r="G8" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="21"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="H8" s="21">
+        <f>D8</f>
+        <v>0.33</v>
+      </c>
       <c r="I8" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="78"/>
+        <v>8.25</v>
+      </c>
+      <c r="J8" s="78">
+        <v>0.33</v>
+      </c>
       <c r="K8" s="78">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="19"/>
+        <v>3.96</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>392</v>
+      </c>
       <c r="P8" s="43"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -7346,22 +7398,22 @@
         <v>364</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="P9" s="43" t="s">
         <v>376</v>
-      </c>
-      <c r="P9" s="43" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -7402,22 +7454,22 @@
         <v>364</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="P10" s="43" t="s">
         <v>381</v>
-      </c>
-      <c r="P10" s="43" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -7464,10 +7516,10 @@
         <v>18</v>
       </c>
       <c r="O11" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="P11" s="43" t="s">
         <v>384</v>
-      </c>
-      <c r="P11" s="43" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -8046,28 +8098,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>3.8745000000000003</v>
+        <v>6.6844999999999999</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f>SUM(G4:G30)</f>
-        <v>38.745000000000005</v>
+        <v>66.844999999999999</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f>SUM(I4:I30)</f>
-        <v>96.862499999999997</v>
+        <v>167.11250000000001</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>46.494</v>
+        <v>80.213999999999999</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -8077,28 +8129,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>3.8745000000000003</v>
+        <v>6.6844999999999999</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>3.8745000000000003</v>
+        <v>6.6844999999999999</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>3.8744999999999998</v>
+        <v>6.6845000000000008</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>3.8744999999999998</v>
+        <v>6.6844999999999999</v>
       </c>
       <c r="N32" s="30"/>
     </row>

</xml_diff>

<commit_message>
Added LEMS scaling to BOM
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Full Device" sheetId="3" r:id="rId1"/>
     <sheet name="Shield Parts" sheetId="1" r:id="rId2"/>
     <sheet name="LiCor_Leveling_Base" sheetId="5" r:id="rId3"/>
-    <sheet name="MLX90614 Housing" sheetId="6" r:id="rId4"/>
+    <sheet name="MLX90614_Housing" sheetId="6" r:id="rId4"/>
+    <sheet name="v2.1 Scaling" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="409">
   <si>
     <t>Number</t>
   </si>
@@ -887,12 +888,6 @@
     <t>Can maybe be found on eBay</t>
   </si>
   <si>
-    <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-12069-1. More expensive on Noco website</t>
-  </si>
-  <si>
-    <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-13106-2. More expensive on Noco website</t>
-  </si>
-  <si>
     <t>Davis Anemometer</t>
   </si>
   <si>
@@ -1209,6 +1204,60 @@
   </si>
   <si>
     <t>BatterySharks is US source. The $30 ones were bought in europe, explaining the price. F2 terminals are typically used</t>
+  </si>
+  <si>
+    <t>3D Printed Plates</t>
+  </si>
+  <si>
+    <t>UofU ME Dept.</t>
+  </si>
+  <si>
+    <t>Pricing is for UofU Mechanical Engineering Dept. printer</t>
+  </si>
+  <si>
+    <t>Ideal Cost/50 Units</t>
+  </si>
+  <si>
+    <t>Ideal Cost/75 Units</t>
+  </si>
+  <si>
+    <t>Ideal Cost/100 Units</t>
+  </si>
+  <si>
+    <t>DS-2 Sonic Anemometer</t>
+  </si>
+  <si>
+    <t>Thermocouple Chip</t>
+  </si>
+  <si>
+    <t>This sheet is used to estimate the costs of making LEMSv2.1, in quantity. Many prices are approximate, and not all parts may be included!</t>
+  </si>
+  <si>
+    <t>Wifi Chip</t>
+  </si>
+  <si>
+    <t>MAX31856, see https://www.adafruit.com/product/3263</t>
+  </si>
+  <si>
+    <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-12069-1. More expensive on Noco website. Also known as BLSOLAR2</t>
+  </si>
+  <si>
+    <t>Other options available, see https://no.co/products/solar. Noco UPC: 0-46221-13106-2. More expensive on Noco website. Also known as GC027</t>
+  </si>
+  <si>
+    <t>LiCor Leveling Base</t>
+  </si>
+  <si>
+    <t>MLX90614 Housing</t>
+  </si>
+  <si>
+    <t>See MLX90614_Housing sheet for details</t>
+  </si>
+  <si>
+    <t>PCB Assembly Total</t>
+  </si>
+  <si>
+    <t>PCB Assembly/Board</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1272,7 @@
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1247,8 +1296,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,8 +1324,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1656,8 +1724,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1679,8 +1771,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1784,6 +1877,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="21" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1814,8 +1914,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="22">
+    <cellStyle name="Bad" xfId="21" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2172,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2203,7 +2314,7 @@
         <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J1" t="s">
         <v>259</v>
@@ -2214,34 +2325,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="90"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="94" t="s">
+      <c r="I2" s="94"/>
+      <c r="J2" s="97" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="89" t="s">
+      <c r="K2" s="98"/>
+      <c r="L2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="87" t="s">
+      <c r="M2" s="96"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="90" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2291,7 +2402,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="88"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -2399,7 +2510,7 @@
         <v>34</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>285</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2454,7 +2565,7 @@
         <v>37</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>286</v>
+        <v>403</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -2733,7 +2844,7 @@
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="25" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
@@ -2769,7 +2880,7 @@
         <v>384</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="M12" s="29" t="s">
         <v>18</v>
@@ -2778,10 +2889,10 @@
         <v>18</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="P12" s="43" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -2832,7 +2943,7 @@
         <v>18</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="P13" s="43" t="s">
         <v>271</v>
@@ -3001,7 +3112,7 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C17" s="4">
         <v>2</v>
@@ -3036,25 +3147,25 @@
         <v>4008</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N17" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O17" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P17" s="43" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -3091,23 +3202,23 @@
         <v>1283.8799999999999</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N18" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="P18" s="43"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
@@ -3141,25 +3252,25 @@
         <v>3110.3999999999996</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N19" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P19" s="43" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
@@ -3197,25 +3308,25 @@
         <v>2.9483999999999999</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N20" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O20" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P20" s="43" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
@@ -3252,25 +3363,25 @@
         <v>3.8049999960000003</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M21" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="O21" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="N21" s="29" t="s">
+      <c r="P21" s="43" t="s">
         <v>308</v>
-      </c>
-      <c r="O21" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="25" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
@@ -3308,25 +3419,25 @@
         <v>13.152000000000001</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="N22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P22" s="43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C23" s="4">
         <v>2</v>
@@ -3364,81 +3475,81 @@
         <v>3.5327999999999999</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M23" s="29" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N23" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P23" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="25" t="s">
-        <v>339</v>
+        <v>404</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="39">
         <f>LiCor_Leveling_Base!$E$32</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="E24" s="26">
         <f t="shared" si="0"/>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="F24" s="21">
         <f>LiCor_Leveling_Base!$G$32</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="G24" s="20">
         <f t="shared" si="1"/>
-        <v>99.20366666999999</v>
+        <v>228.387</v>
       </c>
       <c r="H24" s="21">
         <f>LiCor_Leveling_Base!$I$32</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="I24" s="20">
         <f t="shared" si="2"/>
-        <v>248.00916667499999</v>
+        <v>570.96749999999997</v>
       </c>
       <c r="J24" s="78">
         <f>D24</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="K24" s="78">
         <f t="shared" si="3"/>
-        <v>119.044400004</v>
+        <v>274.06439999999998</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M24" s="29" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N24" s="29" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P24" s="43" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="25" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
@@ -3476,25 +3587,25 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="N25" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O25" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P25" s="43" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
@@ -3531,25 +3642,25 @@
         <v>8.3879999999999999</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N26" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P26" s="43" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="25" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -3586,50 +3697,76 @@
         <v>54.599999999999994</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N27" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="P27" s="43" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="39"/>
+      <c r="B28" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="39">
+        <f>MLX90614_Housing!$E$32</f>
+        <v>6.6844999999999999</v>
+      </c>
       <c r="E28" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="21"/>
+        <v>6.6844999999999999</v>
+      </c>
+      <c r="F28" s="21">
+        <f>D28</f>
+        <v>6.6844999999999999</v>
+      </c>
       <c r="G28" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="21"/>
+        <v>66.844999999999999</v>
+      </c>
+      <c r="H28" s="21">
+        <f>D28</f>
+        <v>6.6844999999999999</v>
+      </c>
       <c r="I28" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="78"/>
+        <v>167.11250000000001</v>
+      </c>
+      <c r="J28" s="78">
+        <f>D28</f>
+        <v>6.6844999999999999</v>
+      </c>
       <c r="K28" s="78">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="43"/>
+        <v>80.213999999999999</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N28" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="P28" s="43" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
@@ -3697,28 +3834,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>1067.3508833333333</v>
+        <v>1086.9537166663333</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f t="shared" ref="G31:I31" si="4">SUM(G4:G30)</f>
-        <v>10141.378833333332</v>
+        <v>10337.407166663332</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f t="shared" si="4"/>
-        <v>25322.44708333334</v>
+        <v>25812.517916658337</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>12579.650600000003</v>
+        <v>12814.884599996001</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3728,28 +3865,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>1067.3508833333333</v>
+        <v>1086.9537166663333</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>1014.1378833333332</v>
+        <v>1033.7407166663331</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>1012.8978833333335</v>
+        <v>1032.5007166663336</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>1048.3042166666669</v>
+        <v>1067.9070499996667</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -3805,10 +3942,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="96"/>
+      <c r="B1" s="99"/>
       <c r="C1" s="50" t="s">
         <v>61</v>
       </c>
@@ -3820,33 +3957,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92" t="s">
+      <c r="H2" s="94"/>
+      <c r="I2" s="95" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="91"/>
-      <c r="K2" s="89" t="s">
+      <c r="J2" s="94"/>
+      <c r="K2" s="92" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="91"/>
-      <c r="M2" s="89" t="s">
+      <c r="L2" s="94"/>
+      <c r="M2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="93"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="87" t="s">
+      <c r="N2" s="96"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="90" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3899,7 +4036,7 @@
       <c r="P3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="88"/>
+      <c r="Q3" s="91"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -5796,7 +5933,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5834,34 +5971,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="90"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="83"/>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="94" t="s">
+      <c r="I2" s="94"/>
+      <c r="J2" s="97" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="89" t="s">
+      <c r="K2" s="98"/>
+      <c r="L2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="87" t="s">
+      <c r="M2" s="96"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="90" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5911,12 +6048,12 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="88"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C4" s="45">
         <v>3</v>
@@ -5954,25 +6091,25 @@
         <v>8.0063999999999993</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
@@ -6010,25 +6147,25 @@
         <v>3.1895999999999995</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -6066,25 +6203,25 @@
         <v>31.049999999999997</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -6122,25 +6259,25 @@
         <v>29.52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
@@ -6178,25 +6315,25 @@
         <v>5.7984</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="P8" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -6233,23 +6370,23 @@
         <v>37.68</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -6284,50 +6421,73 @@
         <v>3.8000000040000002</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P10" s="43" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="84"/>
+      <c r="B11" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="84">
+        <v>12.918333333</v>
+      </c>
       <c r="E11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="85"/>
+        <v>12.918333333</v>
+      </c>
+      <c r="F11" s="85">
+        <f>D11</f>
+        <v>12.918333333</v>
+      </c>
       <c r="G11" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="85"/>
+        <v>129.18333332999998</v>
+      </c>
+      <c r="H11" s="85">
+        <f>D11</f>
+        <v>12.918333333</v>
+      </c>
       <c r="I11" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="78"/>
+        <v>322.95833332500001</v>
+      </c>
+      <c r="J11" s="78">
+        <f>D11</f>
+        <v>12.918333333</v>
+      </c>
       <c r="K11" s="78">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
+        <v>155.019999996</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="O11" s="19"/>
-      <c r="P11" s="43"/>
+      <c r="P11" s="43" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
@@ -6905,28 +7065,28 @@
       </c>
       <c r="E31" s="24">
         <f>SUM(E4:E30)</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="24">
         <f>SUM(G4:G30)</f>
-        <v>99.203666670000004</v>
+        <v>228.387</v>
       </c>
       <c r="H31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="24">
         <f>SUM(I4:I30)</f>
-        <v>248.00916667499999</v>
+        <v>570.96749999999997</v>
       </c>
       <c r="J31" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="24">
         <f>SUM(K4:K30)</f>
-        <v>119.04440000399998</v>
+        <v>274.06439999999998</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -6936,28 +7096,28 @@
       </c>
       <c r="E32" s="24">
         <f>E31</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="35">
         <f>G31/10</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="35">
         <f>I31/25</f>
-        <v>9.9203666669999997</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="J32" t="s">
         <v>13</v>
       </c>
       <c r="K32" s="35">
         <f>K31/K1</f>
-        <v>9.9203666669999979</v>
+        <v>22.838699999999999</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -7012,34 +7172,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="90"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="86"/>
-      <c r="D2" s="89" t="s">
+      <c r="D2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="94" t="s">
+      <c r="I2" s="94"/>
+      <c r="J2" s="97" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="95"/>
-      <c r="L2" s="89" t="s">
+      <c r="K2" s="98"/>
+      <c r="L2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="87" t="s">
+      <c r="M2" s="96"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="90" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7089,12 +7249,12 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="88"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C4" s="45">
         <v>1</v>
@@ -7131,23 +7291,23 @@
         <v>29.759999999999998</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="P4" s="43"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -7183,23 +7343,23 @@
         <v>7.8000000000000007</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M5" s="29" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="N5" s="29" t="s">
         <v>18</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P5" s="43"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="25" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -7235,23 +7395,23 @@
         <v>4.68</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="N6" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P6" s="43"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -7287,25 +7447,25 @@
         <v>11.879999999999999</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="N7" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="P7" s="43" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="25" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -7341,23 +7501,23 @@
         <v>3.96</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="P8" s="43"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="25" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -7395,25 +7555,25 @@
         <v>6.42</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N9" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="P9" s="43" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -7451,25 +7611,25 @@
         <v>3.4499999999999997</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P10" s="43" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -7507,19 +7667,19 @@
         <v>12.263999999999999</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M11" s="32" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="N11" s="32" t="s">
         <v>18</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="P11" s="43" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -8166,4 +8326,1735 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:P39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="156.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="127.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="100" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+    </row>
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="88"/>
+      <c r="B3" s="6"/>
+      <c r="D3" s="3"/>
+      <c r="N3" s="30"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="102"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
+        <v>394</v>
+      </c>
+      <c r="G4" s="94"/>
+      <c r="H4" s="92" t="s">
+        <v>395</v>
+      </c>
+      <c r="I4" s="94"/>
+      <c r="J4" s="92" t="s">
+        <v>396</v>
+      </c>
+      <c r="K4" s="94"/>
+      <c r="L4" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="96"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="90" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="91"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="45">
+        <v>1</v>
+      </c>
+      <c r="D6" s="37">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="38">
+        <f t="shared" ref="E6:E34" si="0">C6*D6</f>
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="41">
+        <v>0.72140000000000004</v>
+      </c>
+      <c r="G6" s="42">
+        <f>C6*F6*50</f>
+        <v>36.07</v>
+      </c>
+      <c r="H6" s="41">
+        <f>F6</f>
+        <v>0.72140000000000004</v>
+      </c>
+      <c r="I6" s="42">
+        <f>C6*H6*75</f>
+        <v>54.105000000000004</v>
+      </c>
+      <c r="J6" s="78">
+        <f>0.6312</f>
+        <v>0.63119999999999998</v>
+      </c>
+      <c r="K6" s="78">
+        <f>C6*J6*100</f>
+        <v>63.12</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="P6" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="39">
+        <v>24.95</v>
+      </c>
+      <c r="E7" s="26">
+        <f t="shared" si="0"/>
+        <v>24.95</v>
+      </c>
+      <c r="F7" s="21">
+        <f>D7</f>
+        <v>24.95</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" ref="G7:G34" si="1">C7*F7*50</f>
+        <v>1247.5</v>
+      </c>
+      <c r="H7" s="21">
+        <f>D7</f>
+        <v>24.95</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" ref="I7:I34" si="2">C7*H7*75</f>
+        <v>1871.25</v>
+      </c>
+      <c r="J7" s="78">
+        <f>F7</f>
+        <v>24.95</v>
+      </c>
+      <c r="K7" s="78">
+        <f t="shared" ref="K7:K34" si="3">C7*J7*100</f>
+        <v>2495</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="43" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39">
+        <v>14.95</v>
+      </c>
+      <c r="E8" s="26">
+        <f t="shared" si="0"/>
+        <v>14.95</v>
+      </c>
+      <c r="F8" s="21">
+        <f>D8</f>
+        <v>14.95</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" si="1"/>
+        <v>747.5</v>
+      </c>
+      <c r="H8" s="21">
+        <f>D8</f>
+        <v>14.95</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="2"/>
+        <v>1121.25</v>
+      </c>
+      <c r="J8" s="78">
+        <f>F8</f>
+        <v>14.95</v>
+      </c>
+      <c r="K8" s="78">
+        <f t="shared" si="3"/>
+        <v>1495</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="43" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="39">
+        <v>24.95</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>24.95</v>
+      </c>
+      <c r="F9" s="21">
+        <v>22.46</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="1"/>
+        <v>1123</v>
+      </c>
+      <c r="H9" s="21">
+        <f>F9</f>
+        <v>22.46</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>1684.5</v>
+      </c>
+      <c r="J9" s="78">
+        <f>21.21</f>
+        <v>21.21</v>
+      </c>
+      <c r="K9" s="78">
+        <f t="shared" si="3"/>
+        <v>2121</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="P9" s="43"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="39">
+        <v>1.95</v>
+      </c>
+      <c r="E10" s="26">
+        <f t="shared" si="0"/>
+        <v>1.95</v>
+      </c>
+      <c r="F10" s="21">
+        <f>D10</f>
+        <v>1.95</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" si="1"/>
+        <v>97.5</v>
+      </c>
+      <c r="H10" s="21">
+        <f>D10</f>
+        <v>1.95</v>
+      </c>
+      <c r="I10" s="20">
+        <f t="shared" si="2"/>
+        <v>146.25</v>
+      </c>
+      <c r="J10" s="78">
+        <f>D10</f>
+        <v>1.95</v>
+      </c>
+      <c r="K10" s="78">
+        <f t="shared" si="3"/>
+        <v>195</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="P10" s="43" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="89" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="39">
+        <v>16.441500000000001</v>
+      </c>
+      <c r="E11" s="26">
+        <f t="shared" si="0"/>
+        <v>16.441500000000001</v>
+      </c>
+      <c r="F11" s="21">
+        <f>9.8649</f>
+        <v>9.8649000000000004</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="1"/>
+        <v>493.245</v>
+      </c>
+      <c r="H11" s="21">
+        <f>F11</f>
+        <v>9.8649000000000004</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>739.86750000000006</v>
+      </c>
+      <c r="J11" s="78">
+        <f>F11</f>
+        <v>9.8649000000000004</v>
+      </c>
+      <c r="K11" s="78">
+        <f t="shared" si="3"/>
+        <v>986.49</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="P11" s="43" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="89" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="84">
+        <v>104.232222222</v>
+      </c>
+      <c r="E12" s="63">
+        <f t="shared" si="0"/>
+        <v>104.232222222</v>
+      </c>
+      <c r="F12" s="85">
+        <v>56.13</v>
+      </c>
+      <c r="G12" s="64">
+        <f t="shared" si="1"/>
+        <v>2806.5</v>
+      </c>
+      <c r="H12" s="85">
+        <v>51.79</v>
+      </c>
+      <c r="I12" s="64">
+        <f t="shared" si="2"/>
+        <v>3884.25</v>
+      </c>
+      <c r="J12" s="78">
+        <v>49.62</v>
+      </c>
+      <c r="K12" s="78">
+        <f t="shared" si="3"/>
+        <v>4962</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="P12" s="43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="89" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="84">
+        <v>63.345555556000001</v>
+      </c>
+      <c r="E13" s="63">
+        <f t="shared" si="0"/>
+        <v>63.345555556000001</v>
+      </c>
+      <c r="F13" s="85">
+        <v>35.68</v>
+      </c>
+      <c r="G13" s="64">
+        <f t="shared" si="1"/>
+        <v>1784</v>
+      </c>
+      <c r="H13" s="85">
+        <v>34.43</v>
+      </c>
+      <c r="I13" s="64">
+        <f t="shared" si="2"/>
+        <v>2582.25</v>
+      </c>
+      <c r="J13" s="78">
+        <v>31</v>
+      </c>
+      <c r="K13" s="78">
+        <f t="shared" si="3"/>
+        <v>3100</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="P13" s="43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="39">
+        <v>8.99</v>
+      </c>
+      <c r="E14" s="26">
+        <f t="shared" si="0"/>
+        <v>8.99</v>
+      </c>
+      <c r="F14" s="21">
+        <f>D14</f>
+        <v>8.99</v>
+      </c>
+      <c r="G14" s="20">
+        <f t="shared" si="1"/>
+        <v>449.5</v>
+      </c>
+      <c r="H14" s="21">
+        <f>D14</f>
+        <v>8.99</v>
+      </c>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>674.25</v>
+      </c>
+      <c r="J14" s="78">
+        <f>D14</f>
+        <v>8.99</v>
+      </c>
+      <c r="K14" s="78">
+        <f t="shared" si="3"/>
+        <v>899</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="P14" s="43" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="39">
+        <v>13</v>
+      </c>
+      <c r="E15" s="26">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="21">
+        <v>11.47</v>
+      </c>
+      <c r="G15" s="20">
+        <f t="shared" si="1"/>
+        <v>573.5</v>
+      </c>
+      <c r="H15" s="21">
+        <v>11.19</v>
+      </c>
+      <c r="I15" s="20">
+        <f t="shared" si="2"/>
+        <v>839.25</v>
+      </c>
+      <c r="J15" s="78">
+        <v>11.01</v>
+      </c>
+      <c r="K15" s="78">
+        <f t="shared" si="3"/>
+        <v>1101</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="P15" s="43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="39">
+        <v>39.99</v>
+      </c>
+      <c r="E16" s="26">
+        <f t="shared" si="0"/>
+        <v>39.99</v>
+      </c>
+      <c r="F16" s="21">
+        <v>35.99</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" si="1"/>
+        <v>1799.5</v>
+      </c>
+      <c r="H16" s="21">
+        <f>F16</f>
+        <v>35.99</v>
+      </c>
+      <c r="I16" s="20">
+        <f t="shared" si="2"/>
+        <v>2699.25</v>
+      </c>
+      <c r="J16" s="78">
+        <f>F16</f>
+        <v>35.99</v>
+      </c>
+      <c r="K16" s="78">
+        <f t="shared" si="3"/>
+        <v>3599</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="M16" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="N16" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="P16" s="43" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="39">
+        <v>13.95</v>
+      </c>
+      <c r="E17" s="26">
+        <f t="shared" si="0"/>
+        <v>13.95</v>
+      </c>
+      <c r="F17" s="21">
+        <v>12.56</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="1"/>
+        <v>628</v>
+      </c>
+      <c r="H17" s="21">
+        <f>F17</f>
+        <v>12.56</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="2"/>
+        <v>942</v>
+      </c>
+      <c r="J17" s="78">
+        <f>11.16</f>
+        <v>11.16</v>
+      </c>
+      <c r="K17" s="78">
+        <f t="shared" si="3"/>
+        <v>1116</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M17" s="29">
+        <v>2857</v>
+      </c>
+      <c r="N17" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="P17" s="43"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="39">
+        <v>14.95</v>
+      </c>
+      <c r="E18" s="26">
+        <f t="shared" si="0"/>
+        <v>14.95</v>
+      </c>
+      <c r="F18" s="21">
+        <v>12.71</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="1"/>
+        <v>635.5</v>
+      </c>
+      <c r="H18" s="21">
+        <f>F18</f>
+        <v>12.71</v>
+      </c>
+      <c r="I18" s="20">
+        <f t="shared" si="2"/>
+        <v>953.25000000000011</v>
+      </c>
+      <c r="J18" s="78">
+        <f>F18</f>
+        <v>12.71</v>
+      </c>
+      <c r="K18" s="78">
+        <f t="shared" si="3"/>
+        <v>1271</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="P18" s="43" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="39">
+        <v>186</v>
+      </c>
+      <c r="E19" s="26">
+        <f t="shared" si="0"/>
+        <v>372</v>
+      </c>
+      <c r="F19" s="21">
+        <v>167</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" si="1"/>
+        <v>16700</v>
+      </c>
+      <c r="H19" s="21">
+        <v>167</v>
+      </c>
+      <c r="I19" s="20">
+        <f t="shared" si="2"/>
+        <v>25050</v>
+      </c>
+      <c r="J19" s="78">
+        <f>F19</f>
+        <v>167</v>
+      </c>
+      <c r="K19" s="78">
+        <f t="shared" si="3"/>
+        <v>33400</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M19" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="N19" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="P19" s="43" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="39">
+        <v>529</v>
+      </c>
+      <c r="E20" s="26">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+      <c r="F20" s="21">
+        <f>453</f>
+        <v>453</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" si="1"/>
+        <v>22650</v>
+      </c>
+      <c r="H20" s="21">
+        <f>F20</f>
+        <v>453</v>
+      </c>
+      <c r="I20" s="20">
+        <f t="shared" si="2"/>
+        <v>33975</v>
+      </c>
+      <c r="J20" s="78">
+        <f>F20</f>
+        <v>453</v>
+      </c>
+      <c r="K20" s="78">
+        <f t="shared" si="3"/>
+        <v>45300</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20" s="19"/>
+      <c r="P20" s="43"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="39">
+        <v>270</v>
+      </c>
+      <c r="E21" s="26">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="F21" s="21">
+        <v>243</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" si="1"/>
+        <v>12150</v>
+      </c>
+      <c r="H21" s="21">
+        <v>229</v>
+      </c>
+      <c r="I21" s="20">
+        <f t="shared" si="2"/>
+        <v>17175</v>
+      </c>
+      <c r="J21" s="78">
+        <v>216</v>
+      </c>
+      <c r="K21" s="78">
+        <f t="shared" si="3"/>
+        <v>21600</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="M21" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="N21" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="P21" s="43" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3</v>
+      </c>
+      <c r="D22" s="39">
+        <f>8.19/100</f>
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="E22" s="26">
+        <f t="shared" si="0"/>
+        <v>0.2457</v>
+      </c>
+      <c r="F22" s="21">
+        <f>D22</f>
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="G22" s="20">
+        <f t="shared" si="1"/>
+        <v>12.285</v>
+      </c>
+      <c r="H22" s="21">
+        <f>D22</f>
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="I22" s="20">
+        <f t="shared" si="2"/>
+        <v>18.427499999999998</v>
+      </c>
+      <c r="J22" s="78">
+        <f t="shared" ref="J22:J29" si="4">D22</f>
+        <v>8.1900000000000001E-2</v>
+      </c>
+      <c r="K22" s="78">
+        <f t="shared" si="3"/>
+        <v>24.57</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="N22" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="P22" s="43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="39">
+        <v>0.31708333300000002</v>
+      </c>
+      <c r="E23" s="26">
+        <f t="shared" si="0"/>
+        <v>0.31708333300000002</v>
+      </c>
+      <c r="F23" s="21">
+        <f>D23</f>
+        <v>0.31708333300000002</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="1"/>
+        <v>15.854166650000002</v>
+      </c>
+      <c r="H23" s="21">
+        <f>D23</f>
+        <v>0.31708333300000002</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="2"/>
+        <v>23.781249975000001</v>
+      </c>
+      <c r="J23" s="78">
+        <f t="shared" si="4"/>
+        <v>0.31708333300000002</v>
+      </c>
+      <c r="K23" s="78">
+        <f t="shared" si="3"/>
+        <v>31.708333300000003</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="O23" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="P23" s="43" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="39">
+        <f>10.96/10</f>
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="E24" s="26">
+        <f t="shared" si="0"/>
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="F24" s="21">
+        <f>D24</f>
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="1"/>
+        <v>54.800000000000004</v>
+      </c>
+      <c r="H24" s="21">
+        <f>D24</f>
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="I24" s="20">
+        <f t="shared" si="2"/>
+        <v>82.2</v>
+      </c>
+      <c r="J24" s="78">
+        <f t="shared" si="4"/>
+        <v>1.0960000000000001</v>
+      </c>
+      <c r="K24" s="78">
+        <f t="shared" si="3"/>
+        <v>109.60000000000001</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="N24" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O24" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="P24" s="43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+      <c r="D25" s="39">
+        <f>7.36/50</f>
+        <v>0.1472</v>
+      </c>
+      <c r="E25" s="26">
+        <f t="shared" si="0"/>
+        <v>0.2944</v>
+      </c>
+      <c r="F25" s="21">
+        <f>D25</f>
+        <v>0.1472</v>
+      </c>
+      <c r="G25" s="20">
+        <f t="shared" si="1"/>
+        <v>14.719999999999999</v>
+      </c>
+      <c r="H25" s="21">
+        <f>D25</f>
+        <v>0.1472</v>
+      </c>
+      <c r="I25" s="20">
+        <f t="shared" si="2"/>
+        <v>22.08</v>
+      </c>
+      <c r="J25" s="78">
+        <f t="shared" si="4"/>
+        <v>0.1472</v>
+      </c>
+      <c r="K25" s="78">
+        <f t="shared" si="3"/>
+        <v>29.439999999999998</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="P25" s="43" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="39">
+        <f>LiCor_Leveling_Base!$E$32</f>
+        <v>22.838699999999999</v>
+      </c>
+      <c r="E26" s="26">
+        <f t="shared" si="0"/>
+        <v>22.838699999999999</v>
+      </c>
+      <c r="F26" s="21">
+        <f>LiCor_Leveling_Base!$G$32</f>
+        <v>22.838699999999999</v>
+      </c>
+      <c r="G26" s="20">
+        <f t="shared" si="1"/>
+        <v>1141.9349999999999</v>
+      </c>
+      <c r="H26" s="21">
+        <f>LiCor_Leveling_Base!$I$32</f>
+        <v>22.838699999999999</v>
+      </c>
+      <c r="I26" s="20">
+        <f t="shared" si="2"/>
+        <v>1712.9024999999999</v>
+      </c>
+      <c r="J26" s="78">
+        <f t="shared" si="4"/>
+        <v>22.838699999999999</v>
+      </c>
+      <c r="K26" s="78">
+        <f t="shared" si="3"/>
+        <v>2283.87</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="M26" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N26" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="O26" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="P26" s="43" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2</v>
+      </c>
+      <c r="D27" s="39">
+        <f>3.3/100</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E27" s="26">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F27" s="21">
+        <f>D27</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="H27" s="21">
+        <f>D27</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I27" s="20">
+        <f t="shared" si="2"/>
+        <v>4.95</v>
+      </c>
+      <c r="J27" s="78">
+        <f t="shared" si="4"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K27" s="78">
+        <f t="shared" si="3"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M27" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O27" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="P27" s="43" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2</v>
+      </c>
+      <c r="D28" s="39">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="E28" s="26">
+        <f t="shared" si="0"/>
+        <v>1.3979999999999999</v>
+      </c>
+      <c r="F28" s="21">
+        <f>D28</f>
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="G28" s="20">
+        <f t="shared" si="1"/>
+        <v>69.899999999999991</v>
+      </c>
+      <c r="H28" s="21">
+        <f>D28</f>
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="I28" s="20">
+        <f t="shared" si="2"/>
+        <v>104.85</v>
+      </c>
+      <c r="J28" s="78">
+        <f t="shared" si="4"/>
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="K28" s="78">
+        <f t="shared" si="3"/>
+        <v>139.79999999999998</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="N28" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O28" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="P28" s="43" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="39">
+        <v>4.55</v>
+      </c>
+      <c r="E29" s="26">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+      <c r="F29" s="21">
+        <f>D29</f>
+        <v>4.55</v>
+      </c>
+      <c r="G29" s="20">
+        <f t="shared" si="1"/>
+        <v>227.5</v>
+      </c>
+      <c r="H29" s="21">
+        <f>D29</f>
+        <v>4.55</v>
+      </c>
+      <c r="I29" s="20">
+        <f t="shared" si="2"/>
+        <v>341.25</v>
+      </c>
+      <c r="J29" s="78">
+        <f t="shared" si="4"/>
+        <v>4.55</v>
+      </c>
+      <c r="K29" s="78">
+        <f t="shared" si="3"/>
+        <v>455</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="M29" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="O29" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="P29" s="43" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="21"/>
+      <c r="I30" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="43" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="21"/>
+      <c r="I31" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="43"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="43"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="21"/>
+      <c r="I33" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="43"/>
+    </row>
+    <row r="34" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="23"/>
+      <c r="I34" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="79"/>
+      <c r="K34" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="44"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D35" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="24">
+        <f>SUM(E6:E34)</f>
+        <v>1544.4051611109999</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="24">
+        <f t="shared" ref="G35:I35" si="5">SUM(G6:G34)</f>
+        <v>65461.609166650014</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="24">
+        <f t="shared" si="5"/>
+        <v>96702.163749975007</v>
+      </c>
+      <c r="J35" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="24">
+        <f>SUM(K6:K34)</f>
+        <v>126784.19833330002</v>
+      </c>
+      <c r="N35" s="30"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="24">
+        <f>E35</f>
+        <v>1544.4051611109999</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="35">
+        <f>G35/50</f>
+        <v>1309.2321833330002</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="35">
+        <f>I35/75</f>
+        <v>1289.3621833330001</v>
+      </c>
+      <c r="J36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="35">
+        <f>K35/100</f>
+        <v>1267.8419833330001</v>
+      </c>
+      <c r="M36" s="103"/>
+      <c r="N36" s="30"/>
+    </row>
+    <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>407</v>
+      </c>
+      <c r="E38" s="24">
+        <f>SUM(E12:E13)</f>
+        <v>167.57777777800001</v>
+      </c>
+      <c r="F38" t="s">
+        <v>407</v>
+      </c>
+      <c r="G38" s="24">
+        <f>SUM(G12:G13)</f>
+        <v>4590.5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>407</v>
+      </c>
+      <c r="I38" s="24">
+        <f>SUM(I12:I13)</f>
+        <v>6466.5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>407</v>
+      </c>
+      <c r="K38" s="24">
+        <f>SUM(K12:K13)</f>
+        <v>8062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>408</v>
+      </c>
+      <c r="E39" s="24">
+        <f>E38/1</f>
+        <v>167.57777777800001</v>
+      </c>
+      <c r="F39" t="s">
+        <v>408</v>
+      </c>
+      <c r="G39" s="24">
+        <f>G38/50</f>
+        <v>91.81</v>
+      </c>
+      <c r="H39" t="s">
+        <v>408</v>
+      </c>
+      <c r="I39" s="24">
+        <f>I38/75</f>
+        <v>86.22</v>
+      </c>
+      <c r="J39" t="s">
+        <v>408</v>
+      </c>
+      <c r="K39" s="24">
+        <f>K38/100</f>
+        <v>80.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:O4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O11" r:id="rId1"/>
+    <hyperlink ref="O12" r:id="rId2"/>
+    <hyperlink ref="O13" r:id="rId3"/>
+    <hyperlink ref="O28" r:id="rId4" location="5415k18/=178w5hq"/>
+    <hyperlink ref="O29" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates and preparation for 2018 builds/deployments
</commit_message>
<xml_diff>
--- a/Hardware Information/Bill of Materials.xlsx
+++ b/Hardware Information/Bill of Materials.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,7 +18,7 @@
     <sheet name="MLX90614_Housing" sheetId="6" r:id="rId4"/>
     <sheet name="v2.1 Scaling" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1263,7 +1263,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1884,6 +1884,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="21" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1923,7 +1924,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Bad" xfId="21" builtinId="27"/>
@@ -1954,6 +1954,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2325,34 +2328,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="92" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="97" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="98" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="92" t="s">
+      <c r="K2" s="99"/>
+      <c r="L2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="96"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="90" t="s">
+      <c r="M2" s="97"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2402,7 +2405,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="91"/>
+      <c r="P3" s="92"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -3942,10 +3945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="99"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="50" t="s">
         <v>61</v>
       </c>
@@ -3957,33 +3960,33 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="94"/>
-      <c r="I2" s="95" t="s">
+      <c r="H2" s="95"/>
+      <c r="I2" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="94"/>
-      <c r="K2" s="92" t="s">
+      <c r="J2" s="95"/>
+      <c r="K2" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="94"/>
-      <c r="M2" s="92" t="s">
+      <c r="L2" s="95"/>
+      <c r="M2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="96"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="90" t="s">
+      <c r="N2" s="97"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4036,7 +4039,7 @@
       <c r="P3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="91"/>
+      <c r="Q3" s="92"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -5971,34 +5974,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="83"/>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="92" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="97" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="98" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="92" t="s">
+      <c r="K2" s="99"/>
+      <c r="L2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="96"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="90" t="s">
+      <c r="M2" s="97"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6048,7 +6051,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="91"/>
+      <c r="P3" s="92"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -7172,34 +7175,34 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="86"/>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95" t="s">
+      <c r="E2" s="95"/>
+      <c r="F2" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="92" t="s">
+      <c r="G2" s="95"/>
+      <c r="H2" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="97" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="98" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="92" t="s">
+      <c r="K2" s="99"/>
+      <c r="L2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="96"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="90" t="s">
+      <c r="M2" s="97"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -7249,7 +7252,7 @@
       <c r="O3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="91"/>
+      <c r="P3" s="92"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -8332,8 +8335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8357,15 +8360,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="88"/>
@@ -8374,34 +8377,34 @@
       <c r="N3" s="30"/>
     </row>
     <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="87"/>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="95" t="s">
+      <c r="E4" s="95"/>
+      <c r="F4" s="96" t="s">
         <v>394</v>
       </c>
-      <c r="G4" s="94"/>
-      <c r="H4" s="92" t="s">
+      <c r="G4" s="95"/>
+      <c r="H4" s="93" t="s">
         <v>395</v>
       </c>
-      <c r="I4" s="94"/>
-      <c r="J4" s="92" t="s">
+      <c r="I4" s="95"/>
+      <c r="J4" s="93" t="s">
         <v>396</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="92" t="s">
+      <c r="K4" s="95"/>
+      <c r="L4" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="96"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="90" t="s">
+      <c r="M4" s="97"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="91" t="s">
         <v>27</v>
       </c>
     </row>
@@ -8451,7 +8454,7 @@
       <c r="O5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="91"/>
+      <c r="P5" s="92"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
@@ -9308,7 +9311,7 @@
         <v>300</v>
       </c>
       <c r="C22" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="39">
         <f>8.19/100</f>
@@ -9316,7 +9319,7 @@
       </c>
       <c r="E22" s="26">
         <f t="shared" si="0"/>
-        <v>0.2457</v>
+        <v>0.1638</v>
       </c>
       <c r="F22" s="21">
         <f>D22</f>
@@ -9324,7 +9327,7 @@
       </c>
       <c r="G22" s="20">
         <f t="shared" si="1"/>
-        <v>12.285</v>
+        <v>8.19</v>
       </c>
       <c r="H22" s="21">
         <f>D22</f>
@@ -9332,7 +9335,7 @@
       </c>
       <c r="I22" s="20">
         <f t="shared" si="2"/>
-        <v>18.427499999999998</v>
+        <v>12.285</v>
       </c>
       <c r="J22" s="78">
         <f t="shared" ref="J22:J29" si="4">D22</f>
@@ -9340,7 +9343,7 @@
       </c>
       <c r="K22" s="78">
         <f t="shared" si="3"/>
-        <v>24.57</v>
+        <v>16.38</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>317</v>
@@ -9909,28 +9912,28 @@
       </c>
       <c r="E35" s="24">
         <f>SUM(E6:E34)</f>
-        <v>1544.4051611109999</v>
+        <v>1544.323261111</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="24">
         <f t="shared" ref="G35:I35" si="5">SUM(G6:G34)</f>
-        <v>65461.609166650014</v>
+        <v>65457.514166650013</v>
       </c>
       <c r="H35" s="24" t="s">
         <v>12</v>
       </c>
       <c r="I35" s="24">
         <f t="shared" si="5"/>
-        <v>96702.163749975007</v>
+        <v>96696.021249975005</v>
       </c>
       <c r="J35" s="24" t="s">
         <v>12</v>
       </c>
       <c r="K35" s="24">
         <f>SUM(K6:K34)</f>
-        <v>126784.19833330002</v>
+        <v>126776.00833330002</v>
       </c>
       <c r="N35" s="30"/>
     </row>
@@ -9940,30 +9943,30 @@
       </c>
       <c r="E36" s="24">
         <f>E35</f>
-        <v>1544.4051611109999</v>
+        <v>1544.323261111</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="35">
         <f>G35/50</f>
-        <v>1309.2321833330002</v>
+        <v>1309.1502833330003</v>
       </c>
       <c r="H36" t="s">
         <v>13</v>
       </c>
       <c r="I36" s="35">
         <f>I35/75</f>
-        <v>1289.3621833330001</v>
+        <v>1289.2802833330002</v>
       </c>
       <c r="J36" t="s">
         <v>13</v>
       </c>
       <c r="K36" s="35">
         <f>K35/100</f>
-        <v>1267.8419833330001</v>
-      </c>
-      <c r="M36" s="103"/>
+        <v>1267.7600833330002</v>
+      </c>
+      <c r="M36" s="90"/>
       <c r="N36" s="30"/>
     </row>
     <row r="37" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>